<commit_message>
Add abstract extraction from PDFs
</commit_message>
<xml_diff>
--- a/szamteches_info_extracted.xlsx
+++ b/szamteches_info_extracted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>Év</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Kivonat</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -462,6 +467,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>A dolgozat egy olyan rendszert és annak felépítését mutatja be részletesen, amely a különböző hajtányokon történő irányváltásra és fékezésre vonatkozó jelzéseket kezeli, egy gyorsulásmérőt és giroszkópot tartalmazó szenzor segítségével, ami a kézfejen kap helyet.  A projekt megoldást próbál nyújtani a hajtányokon történő irányjelzésekre a kéz kormányról való levétele nélkül, ezzel elkerülve az ebből fakadó baleseteket. Az irányváltásra vonatkozó jelzéseket a felhasználó képes jelezni különböző gesztusok segítségével,  mint a kéz oldal irányú forgatása , így nem szükséges levennie a kezét a kormányról teljesen, ezzel megtartva a jármű egyensúlyát . A fékjelzések automatikusan történik a gyorsulás érzékelése köve tkeztében. A rendszer két mikrovezérlőt használ (ESP32 és ESP8266) amik közül az egyik a szenzor adatokat dolgozza  fel, míg  a másik futtat egy webszervert és megvilágítja a megfelelő led -eket. A webszerver a kommunikációért felel a mikrovezérlők között, va lamint egy felhasználói felületként funkcionáló weboldalt is üzemeltet. A weboldalon láthatóak az aktív jelzések , mint a kanyarjelzések és a fékjelzések , valami nt ki- és bekapcsolhatjuk ezeknek a működését . A különböző komponensek közötti kommunikáció veze ték nélkül valósul meg WiFi technológiát használva .</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -477,6 +487,11 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>2023</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>A dolgozat egy okosotthon vezérlőrendszer megvalósítását mutatja be. A rendszer elsősorban otthon automatizálási feladatokat lát el, mint például a hőmérsé klet szabályzása, a növények öntözése és a redőnyök automatikus mozgatása, ezzel megkönnyítve a felhasználó mindennapjait.  Napjainkban az IoT eszközök egyre fontosabb szerepet töltenek be az ember számára, már el sem tudjuk képzelni ezek nélkül az életünke t. Mivel az emberek nagy része rendelkezik otthoni internetkapcsolattal, ezért egy ilyen IoT rendszer kiépítése egyszerűbb, olcsóbb és hatékonyabb, mert nincs szükség vezetékekre az eszközök közötti kommunikáció megvalósítására.   Az általam fejlesztett és megépített  rendszer egy központi részből áll, amihez egy érintőképernyős kijelző van csatlakoztatva, itt lehet követni, illetve beavatkozni az automatizálási folyamatokba, statisztikákat lehet megnézni például a szobában lévő hőmérsékletekről. Ehhez a közp onti részhez több érzékelő kapcsolódik Bluetooth, illetve MQTT kommunikációs protokollok segítségével, amik adatokat szolgáltatnak, valamint ellátják az egyes automatizálási feladatokat. A dolgozatomban ennek a rendszernek a tervezését és megépíté sét dokum entálom le részletesen, az egyes részeket ábrákkal szemléltetve .</t>
         </is>
       </c>
     </row>
@@ -484,6 +499,11 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>A hőmérséklet mérése mindig is egy fontos szerepet játszott az ember életében, kíváncsi természete miatt. A technika és a világ fejlődése miatt mára már játszi könnyedséggel mérünk meg egy térben egy átlaghőmérsékletet, vagy akár konkrét eszközök, vagy akár emberek hőmérsékletét. Jelen dolgozatom célja egy robot megalkotása mely egy zárt térben képes a legmelegebb pont meghatározására és megközelítésére, illetve ezt egy alkalmazáson keresztül a felhasználójának is megjeleníteni egy kép formájában. Ezt a képet a robot bluetooth segítségével juttatja el a kijelzőre. Ezen keresztül a felhasználó szabadon vezérelheti is a robotot.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -501,6 +521,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>A dolgozat témája az agyi tumorok osztályozása konvolúciós neuronhálókkal. A dolgozat elsőfelében a szakirodalom alapján  ismertetem a neurális hálózatokat, kezdve az egyszerű M-Pneurontól  a  konvolúciós  neuronhálókig,  kitérve  a  felépítésükre  és  tanításukra.  A  dolgozatmásodik  felében  három  általam  fejlesztett   modellt  mutatok  be,  amelyek  85%  fölöttipontossággal osztályozták  négy csoportba az agyi tumorokat. Az első megvalósított modellemegy egyszerű konvolúciós neuronháló volt. A második modellel csak mérsékelt teljesítményjavulást  értem  el  az  architektúra  megváltoztatásával  és  a  túltanulás  megakadályozásával .Mindkét  modell  esetében  hangoltam  a  hiperparamétereket.  A  legjobban  teljesítő  modell  aharmadik volt, amel y transfer  learninggel volt megvalósítva  és  a VGG16  volt felhasználvaalapmodellként. Ez a modell érte el legjobb pontosságot  (96%).  A három modell kifejlesztésesorán olyan módszereket alkalmaztam, amelyekkel javítani tudtam folyamatosan neuronhálókteljesítményét, megértve a különböző hatás  mechanizmusokat. Az általam fejlesztett modellalapját  képezheti  egy  olyan  alkalmazásnak,  ami  gyakorló  radiológusoknak  nyújt  gyorselőosztályozást, másodpercek alatt, ezzel megkönnyítve a munkájukat.</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -518,6 +543,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Dolgozatom  témája  a  táblajáték,  dokumentálása  és  nyomon  követése  A  munkám  során  foglalkoztam  a  játék  programozásával,  képfeldolgozással,  játék  valós  időben  való  nyomonkövetésével  a  játék  előrehaladásának  valós  idejű  dokumentálásával.  A  táblajátékok  és  a  képfeldolgozás  két  számomra  egy  izgalmas  területet  ölelnek  fel.  A  Román  Backgammon  Szövetség  különféle  hazai  és  nemzetközi  versenyeket  szervez,  ahol  a  nyomkövetés  és  az  automatikus döntőbíráskodás különösen érdekes.  A  Python  programozási  nyelv  lehetővé  teszi  a  táblajátékok  virtuális  változatának  létrehozását,  amelyek  segítségével  interaktívan  játszhatunk  a  számítógépünkön.  A  játék  programozás  során  az  volt  a  célom,  hogy  két  személy  tudjon  egymás  ellen  játszani  a  számítógépen és lehessen rögzíteni a játékot későbbi visszajátszás céljából.  Az  OpenCV  (Open  Source  Computer  Vision  Library)  egy  népszerű  könyvtár ,  amelyet  a  képfeldolgozásban  alkalmaznak.  Segítségével  a  számítógép  képes  felismerni  és  feldolgozni  a  képeket,  használatával  lehet  rögzíteni  a  játék  állapotát.  Célom  a  képfeldolgozás  terén  az  volt  hogy  egy  videóból  mentsem  ki  az  állóképeket  és  ezeken  azonosítsam  a  figurákat  vagyis  kövessem a játék egymásútani állapotát.  Tehát  a  célom  az  volt,  hogy  a  Python  és  az  OpenCV  kombinálásával  olyan  alkalmazást  csináljak,  amely  automatikusan  értékeli  a  táblajátékot.  Az  elkészítendő  szoftvernek  fel  kell  ismernie  a  figurákat,  pozícióikat,  kockadobásokat,  nyomon  kell  követnie  a  játékosok  lépéseit,  lehetővé téve két ember számára a játékot. játszanak egymás ellen a valós környezetben.</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -531,6 +561,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Az érzékelők használata a mindennapjaink részévé vált, folyamatosan leh etőségünk van a minket körülvevő világban lévő fizikai, kémiai, biológiai jellemzők mérésére. Dolgozatom témája egy interaktív érzékelőrendszer megvalósítása Arduino környezetben, ami megkönnyíti az érzékelők integrálását a rendszerbe, ami kihívást jelenth et egy felhasználó számára, aki még csak ismerkedik az Arduino és a mikrovezérlők világával.  A rendszer működéséhez szükség volt egy szöveges, emberi szem által olvasható ASCII alapú általános protokoll megírására, ami segítségével az érzékelők dinamikusa n konfigurálhatóak és az adatok egységes adatformában továbbíthatóak. Az érzékelőrendszerbe több különböző szenzor is integrálva lett, melyek által különböző fizikai mennyiségek mérésére van lehetőség és az értékek változásának a nyomon követésére.  A felh asználók számára készült egy felhasználói felület, ami egy asztali alkalmazást foglal magába, amin keresztül megjeleníthetők az Arduinohoz kötött szenzorok által mért valósidejű adatok, illetve lehetőség nyílik az adatok mentésére és visszanézésére is. Az alkalmazás és mikrovezérlő között soros kommunikáció valósul meg.  Az alkalmazást laboratóriumi célokra való felhasználásra terveztem meg.</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -544,6 +579,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>A Vezeték nélküli érzékelő hálózatok modellezése című dokumentáció célja, hogy bemutassa az útválasztó protokollok alkalmazását a hálózatok tervezésében és működtetésében. Az útválasztó protokollok kulcsfontosságú szerepet játszanak az adatcsomagok kiválasztásában és irányításában, hogy azok célba érjenek a h álózaton keresztül. Az útválasztó protokollok különböző algoritmusokon alapulnak, amelyeknek különböző jellemzői és működési elvei vannak.  A dokumentáció célja egy modell létrehozása, amely segítségével vizualizálhatjuk az útválasztó protokollok alkalmazás át, a csomagok terjedését és az adatok kiértékelését. Emellett lehetőség nyílik a különböző útválasztó protokollok teljesítményének és hatékonyságának összehasonlítására.  Az útválasztó protokollok kritikus jelentőséggel bírnak a vezeték nélküli hálózatok m űködtetésében. Az algoritmusok és azok implementációinak alapos megértése lehetővé teszi a hálózatok működésének jobb átlátását, esetleges hibák felderítését, valamint hatékony tervezést, optimalizálást és üzemeltetést. A dokumentáció segítséget nyújt a kü lönböző útválasztó protokollok működésének megértésében, előnyeinek és korlátainak feltárásában , valamint segítséget nyújt a hálózatok szimulációjának elkészítésében, mivel részletesen tárgyalja az OMNeT++ keretrendszerben íródott szimulációk kódját. Három  útválasztó protokollról olvashatunk, egy adatközpontúról (Gossiping), egy hierarchikusról (LEACH) és egy helyalapúról (GAF), ezek összehasonlításáról, k övetkeztetések levonás áról és  a vizsgált útválasztó protokollok teljesítményéről és hatékonyságáról.</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -559,6 +599,11 @@
       <c r="C9" t="inlineStr">
         <is>
           <t>2023</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>A biológiai jelenségek jelentős része visszavezethető a genetikára. A genetika pedig a génszekvenciák alapján működik. A különféle élőlények génszekvenciájának megfejtése a biológiai tudományok nagy kihívása, amely merész becslések szerint is még ötszáz évig munkát ad a tudományos világnak.  Dolgozatom célja egy egyszerű génszekvencia osztályozó algoritmus megvalósítása és beépítése egy grafikus felhasználói felülettel rendelkező szoftverbe, amellyel talán egy apró lépést lehet tenni a génszekvenciák megfejtése felé.  A megvalósított algoritmus génszekvencia párok hasonlósági adatai alapján egy csoportosítást hajt végre egy nagyobb szekvencia adathalmazon. A módszer lehetővé teszi nagy mennyiségű proteinszekvencia egyidejű feldologozását, a szekvenciák csoportokra való osztását hasonlóság alapján. Mindez azáltal válik lehetővé, hogy a megvalósítás ritka mátrixokkal dolgozik és nem végez el fölösleges műveleteket, mint amilyenek a nullával való összeadás és szorzás. Ugyanakkor a módszernek jelentős memória hatékonysága is van, mert a ritka mátrix nem tárolja a nullás értékeket.  A megvalósított módszer gráfként kezeli a bemneti szekvencia halmazt. Minden fehérjéhez hozzárendel egy csomópontot a gráfban, és a kezdeti éleket a csomópontok között bemeneti adatként kapja meg a SCOP95 adatbázisból. Ezeket az értékeket a BLAST algoritmussal hozták létre és egy ritka mátrixot alkotnak. A megvalósított algoritmus egy bizonyos módosított Markov klaszterezés, amelyben a két fő művelet, az infláció és a kiterjesztés egymás ellenében dolgozik és a kialakuló egyensúlyi állapotban megmaradó összefüggő részgráfok határozzák meg a csoportosítás végeredményét. Az algoritmus fő paramétere az inflációs ráta, ezzel lehet szabákyozni azt, hogy az algoritmus mennyire szakítsa szét a csoportokat egymástól.   A grafikus felhasználói felület lehetőséget ad a 11944 elemű SCOP95 adathalmazon vagy annak részein végrehajtani az osztályozást különféle beállításokkal, illetve meg tudja mutatni a kialakuló fehérje csoportokat. Továbbá bármely csoportból ki tudunk választani két szekvenciát és megnézhetjük azok egymáshol illesztésének eredményét, melyet a Needleman-Wunsch algoritmussal valósít meg.  _____________________________________________________________________________    10   Az algoritmus képes lenne akár egymillió protein szekvenciát is feldolgozni néhány óra alatt, de ehhez nem állt rendelkezésemre megfelelő valós adathalmaz.</t>
         </is>
       </c>
     </row>
@@ -566,6 +611,11 @@
       <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>A dolgozatom témája egy olyan rendszer megtervezése és kivitelezése, amely egyaránt segít az egyetemi nyílt napok szervezőinek és résztvevőinek abban, hogy az eseménysorozat lebonyolítása könnyebb és átláthatóbb legyen mindenki számára.  Az egyetemi nyílt napok egy évente megrendezett e seménysorozat, melynek célja, hogy népszerűsítse az egyetemet a középiskolás diákok körében, és betekintést engedjen az egyetem működésébe az érdeklődők számára. Ez egy rendkívül fontos folyamat, mert egy kívülálló igazán csak itt pillanthat be mélyebben a z egyetem mindennapjaiba mielőtt úgy döntene, hogy ide jelentkezik. A szervezés során több olyan teendő van, mint az eseményekkel és résztvevőkkel kapcsolatos információk menedzselése, amelyek megoldása hagyományos módszerekkel lassú és körülményes, ezért létrejön az igény egy olyan rendszerre, amely mindezt megkönnyíti.  A dolgozatom célja egy olyan rendszer elkészítése, amely az előbb említett problémákra kínál megoldást két modern keretrendszer előnyeit kihasználva. Az rendszerem megkönnyíti az eseményekk el kapcsolatos információk átadását, a jelenlévők adatainak elmentését és statisztikák készítését a meglévő adathalmazból.  Az rendszer tulajdonképpen 3 részből áll. A mobilalkalmazást a Flutter keretrendszer segítségével valósítottam meg, amelyet a felhasz nálók telefonjaira kell telepíteni és a keretrendszernek köszönhetően platformfüggetlen. Itt a felhasználóknak szerepkörüktől függően lehetőségük van regisztrálni, új eseményeket létrehozni, meglévő eseményeket módosítani, eseményekre jelentkezni, statiszt ikákat generálni. A háttérben egy Spring Boot alkalmazás fut, amely hozzáférést biztosít az adatbázisban tárolt adatokhoz és feldolgozza, valamint elmenti a mobilalkalmazás által generált adatokat. A harmadik rész pedig a Firebase által biztosított felhő a lapú tárhely, ahol a képeket tárolom, valamint a MySQL relációs adatbázis, ahol minden egyéb adatot tárolok.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -579,6 +629,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>A dolgozat célja egy alacsony költségű, könnyen hozzáférhető digitális hangeffektus egység megvalósítása. A projekt magába foglalja a digitális jelfeldolgozási elmélet tanulmányozását, algoritmusok tervezését és fejlesztését, valamint hardveres megvalósítását. Első fázisban a tanulmányozott effektusokat Python alatt teszteltük előre mintavételezett nyers gitár hangállományokkal. Második fázisban STM32G491 mikrovezérlőt tartalmazó saját fejlesztésű multimédia rendszeren teszteltük az algoritmusokat mesterségesen előállított és hangszeren szintetizált jelek segítségével. Az effektusok minőségét mind objektív, mind szubjektív módszerekkel teszteltük.</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -596,6 +651,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>A mai diagnosztikai módszerek  az orvoslásban  folyamatosan fejlődnek, és ma már olyan technikákat alkalmaz hatunk , amelyeket korábban elképzelni sem tudtunk. Az új lehetőségek és technológiai kihívások között olyan megoldások at szeretnék találni , amelyek révén hatékonyabban tudunk felismerni és kezelni gyakori szív- és érrendszeri betegségeket, elkerülve ezáltal a korai vagy az elkerülhető elhalálozást . A kutatásom fő célja az, hogy új és fejlettebb diagnosztikai rendszereket fejlesszek ki, amelyek specifikusan a szív- és érrendszeri betegségek jellegzetességeire fókuszálnak. Ezen rendszerek segítségével pontosabb és hatékonyabb diagnózisokat lehetne elvégezni a betegségek azonosítása és kezelése során.  A módszerem alapját az orvosi elektrokardiográfia (EKG) jel einek felhasználása képezi. Ezen  jelek precíz és részletes információkat nyújtanak a szív elektromos aktivitásáról, amelyek alapján lehetséges különböző szívbetegségek jelenlétét vagy egyéb eltéréseket kimutatni.  Az első lépés a jel ek előzetes feldolgozása, a mely során szűrést és egyéb normalizáló  eljárásokat alkalmazok.  Ezután egy RGB színcsatornás képet, spektrogrammot hozok létre. A spektrogramm egy olyan vizuális reprezentáció, amely bemutatja a jelzés frekvencia -spektrumát az idő függvényében. A színcsato rnák különböző árnyalatai jelzik a frekvencia intenzitását, így könnyebbé válik a jelzés struktúrájának és változásainak vizsgálata. Ez a folyamat segít kivonni a lényeges információkat a jel ekből , és csökkenti a zajok által okozott torzításokat.  Ezek a ké pek pedig bemeneti halmazként szolgálnak a mélytanúlás alapú tanító szoftveremhez, melynek fő feladata az lesz, hogy felismerjen négy konkrét betegséget.  Tehát  a rendszer em képes  lesz felismerni  olyan mintákat , vagy apró részleteket , amelyek emberi szemmel  nem láthatóak, így pontosabb diagnózist biztosít hat az emberek számára , ami jelentősen hozzájárulhat az egészségügyi eredmények javulásához és az életminőség növekedéséhez.</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -613,6 +673,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Az emberek mindig is érdekeltek voltak a robotokban. Gyakran találkozhatunk robotokkal, nem csak a tudományokban, hanem az élet különböző területein is. Bár régebb úgy tekintettünk az ember -robot interakcióra, mint sci -fi (pl. R2D2 a Csillagok háborúja cí mű filmből) napjainkban ez egyre inkább valósággá vált.  Mivel az emberek természetes kommunikációja beszéden keresztül történik, nem nehéz elképzelni a beszéden keresztül történő irányítást sem. A hangvezérlés egy izgalmas téma, ami a robotok irányítását teszi lehetővé hangparancsok által. Erre különböző módszerek léteznek azonban a területen mai napig is kutatások zajlanak. Ez a tudományág nagyon sok izgalmas megvalósítást és alkalmazást hozhat magával a továbbiakban az élet minden területén (tudomány, szórakoztatás, ipar stb.).  A dolgozatom célja, hogy bemutassam a hangvezérlés előnyeit és potenciálját a mobilis robotok irányításban. Ennek érdekében egy megvalósítást fogok bemutatni, amely egy szimulációs környezetben való robot, valamint egy fizikai robo t irányítását teszi lehetővé hangparancsokkal. A továbbiakban olvashatnak a részletes megvalósításról, a felhasznált technológiákról, valamint az elvégzett mérések eredményéről, következtetésekről és továbbfejlesztési lehetőségeiről.</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -624,6 +689,11 @@
       <c r="C14" t="inlineStr">
         <is>
           <t>2023</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Mivel napjainkban egyre elterjedtebbé váltak a kriptovaluták, ezért az ezzel foglalkozó oldalak és alkalmazások rendkívül felkapottak lettek. Létfontosságú, hogy létezzenek olyan eszközök, platformok, amelyek lehetővé teszik a kriptovaluták kereskedését. A kripto világban ezek alkotják a decentralizált tőzsdéket. Ezek olyan platformok vagy alkalmazások, amelyek lehetővé teszik a kriptovaluták közvetlen cseréjét egymás között anélkül, hogy egy közvetítőre lenne szükség. Ezenfelül a decentralizált tőzsdék lehetőséget adnak arra, hogy likviditást szolgáltassunk a rendszerbe. Ugyanakkor lehetővé teszik a likviditás kivételét is. Ezen információk alapján a dolgozatom célja, hogy egy olyan mobil alkalmazást fejlesszek, amely lehetővé teszi a kriptovaluták cseréjét a felhasználók számára úgy Android-on, mint iOS-en. Figyelembe kell vegyük, hogy a kriptovaluták vásárlását nem tesszük lehetővé a felhasználók számára, csupán azok cseréjét.  A dolgozatom létrehozása során megkellett ismerjem azokat a technológiákat, különböző elveket és megoldásokat, amelyek lehetővé teszik egy decentralizált tőzsde működését. Ezek között voltak a különböző blokklánc technológiák, okos szerződésk, illetve a decentralizált tőzsdék főbb funkcionalitásai.</t>
         </is>
       </c>
     </row>
@@ -631,6 +701,11 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Napjainkra az informatika az egyik leggyorsabban növekvő iparággá nőtte ki magát. Gyakran hónaponta, vagy akár hetente hallunk új technológiák megjelenéséről. Ahhoz, hogy a felsőoktatási intézményekből érkező frissen végzett hallgatók megállják a helyüket egy ilyen dinamikusan növekvő környezetben, elengedhetetlen hogy tanulmányaik alatt jól elsajátítsák a programozás alapjait. Az egyik alapfogalom amelynek mélyebb megértése sok fejtörést tud okozni az e gyetemeken tanuló diákoknak, az nem más mint a rekurzió.   Ezen dolgozatnak és a hozzá társuló vizualizációs szoftvernek az a célja, hogy oktatási  segédeszközként szolgálljon mindazok számára, akik szeretnék mélyebben megérteni a rekurzió jelenségét. A fel használó számára lehetőség nyílik arra, hogy különböző rekurzív függvényeket vizualizáljon a szoftver segítségével. A szokásos vizualizációs eszközöktöl eltérően ez az alkalmazás a lépcsők módszerét használja a rekurzió mélységének vizualizációjához.   A be mutatott szoftver nem csak a tanulni vágyó diákok számára lehet hasznos, hanem mindazok számára is akik kutatni szeretnék a rekurzió jelenségét a vizualizációkon megfigyelhető érdekes mintázatok segítségével.             7  Abstract     Nowadays, IT has become  one of the fastest growing industries. We often hear about new technologies every month or even every week. For recent graduates from academic institutions to succeed in such a dynamic and  fast growing environment, it is essential that they have mastered the basics of programming during their studies. One of the basic concepts that can give university students a lot of headaches is recursion.  The aim of this paper and the accompanying visualisation software is to serve as an educational tool for those who wish to gain a deeper understanding of the phenomenon of recursion. The user is given the opportunity to visualise different recursive functions using the software. Unlike the usual visualization tools, this application uses the method of stairs to visuali ze the depth of recursion.   The presented software can be useful not only for students who want to learn, but also for all those who want to explore the phenomenon of recursion by observing interesting patterns in visualizations.             8  Tartalomjegyzék : 1.Beve zető ................................ ................................ ................................ ................................ ............  12 2.Elméleti megalapozás  ................................ ................................ ................................ .........................  12 2.1. A rekurziótörténete  ................................ ................................ ................................ .....................  13 2.2. Rekurzió a matematikában  ................................ ................................ ................................ ..........  14 2.3 Rekurzió a természetben  ................................ ................................ ................................ ..............  15 2.4 Rekurzió a programozásban  ................................ ................................ ................................ .........  16 2.5 Ciklus VS Rekurzió  ................................ ................................ ................................ .....................  17 2.6 A rekurzió oktatása  ................................ ................................ ................................ ......................  19 3.Hasonló alkalmazások és munkák  ................................ ................................ ................................ .......  20 3.1. VisuAlgo  ................................ ................................ ................................ ................................ .... 20 3.2.Sort Visualizer  ................................ ................................ ................................ .............................  21 3.3 Reku rzió kutatása a Sapientia egyetemen  ................................ ................................ .....................  23 4.Szoftver tervezése és kivitelezése  ................................ ................................ ................................ .......  25 4.1 Felhasználói követelmények  ................................ ................................ ................................ ........  25 4.2 Rendszer követelmények  ................................ ................................ ................................ .............  28 4.2.1. Funkcionális követelmények  ................................ ................................ ................................  28 4.2.2. Nem funkcionális követelmények  ................................ ................................ .........................  29 4.3 A rendszer architektúrája  ................................ ................................ ................................ .............  30 4.4 Függvény kiválasztása  ................................ ................................ ................................ .................  31 4.5 Függvény megírása  ................................ ................................ ................................ ......................  32 5. Szo ftver bemutatása  ................................ ................................ ................................ ...........................  34 5.1 Oldalak bemutatása  ................................ ................................ ................................ ......................  34 5.2 Megírt függvények vizualizálása  ................................ ................................ ................................ .. 37 5.2.1 Faktoriális függvény ................................ ................................ ................................ ..............  37 5.2.3 Egy szám páros vagy páratlan hatványa  ................................ ................................ .................  38 5.2.3 Fibonacci függvény  ................................ ................................ ................................ ...............  39 5.2.4 Hanoi tornyai függvény  ................................ ................................ ................................ .........  41 5.2.5 Ackermann függvény  ................................ ................................ ................................ ............  42 5.2.6 Hofstadter Female -Male függvény  ................................ ................................ ........................  44 6.Kihívások a fejlesztés során  ................................ ................................ ................................ ................  45 6.1 Dinamikus string tömb kompilálása  ................................ ................................ .............................  45 6.2 A vizualizációk láthatósága  ................................ ................................ ................................ ..........  48 9  7.Összefoglaló  ................................ ................................ ................................ ................................ .......  49 8.Továbbfejlesztési lehetőségek  ................................ ................................ ................................ .............  50 Irodalomjegyzék  ................................ ................................ ................................ ................................ .... 51                           10   Ábrák jegyzéke :    2.1.ábra :Fibonacci számsorozat (Forrás:[9])   2.2 ábra:  Összeadás és szorzás rekurzív képletek (Forrás:[1])  2.3 ábra : Ackermann képlete (Forrás:[ 2]) 2.4 ábra:  Arany spirál (Forrás:[ 3]) 2.5 ábra : Rekurzív brokkoli (Forrás:[ 10])  2.6. ábra : Aranymetszet a természetben (Forrás:[ 11]) 2.7 ábra : Hanoi tornyai rekurzív implementációja  2.8. ábra : Hanoi tornyai iteratív megvalósítás  2.9. ábra : Hanoi tornyai iteratív megvalósítás  3.1. ábra :VisuAlgo Fibonacci(5) értékre (Forrás:[ 5]) 3.2.ábra : QuickSort a Sort Visualizer programban (Forrás:[ 12]) 3.3.ábra : Merge Sort a Sort Visualizer programban (Forrás:[ 12]) 3.4. ábra:  Rekurzió lépcsőzetes ilusztrációja (Forrás:[ 8]) 4.1. ábra:  Use case diagramm  4.2. ábra : Activity diagramm  4.3. ábra:  Rendszer architektúra  4.4. ábra:  Szekvencia diagramm függvény választ ásnál  4.5. ábra : Szekvencia diagramm függvény írásnál  5.1. ábra:  Az alkalmazás főoldala és a választó ablak  5.2. ábra:  Főoldal részlet a létrehozott szövegdobozzal  5.3. ábra : Nézet a saját kód megírásához  5.4. ábra : Szövegdobozok generálása  11  5.5. ábra:  A kód megírásának folyamata  5.6. ábra : Faktoriális függvény  5.7.ábra : Hatványozás, indirekt rekurzió  5.8. ábra : Fibonacci függvény  5.9. ábra : Fibonacci függvény, szintek megjelölve  5.10. ábra : Hanoi tornyai  5.11.  ábra:  Ackermann függvény (2,4) értékekre  5.12. ábra : Ackermann függvény (2,20) értékre  5.13. ábra:  Ackermann függvény (3,4) értékre  5.14. ábra:  Hofstadter Female -Male függvény 7 -es értékre  5.15. ábra: Hofstadter Female -Male függvény 25 -ös értékre  6.1. ábra : Reflexióhoz szükséges osztályok  6.2. ábra : Main meghívása a dinamikusan futtatott objektumból  6.3. ábra:  Objektum létrehozása stringek segítségével  6.4. ábra : Vonal meghúzása a kezdet és a végpont közé  6.5. ábra : Közelítés a vizualizáción            12  1.Beve zető   A rekurzió egyike azon  programozásban használt  fogalmaknak, amely ek sok fejtörést okoznak a liceumokban, illetve az egyetemeken tanuló diákoknak.  A tapasztalat azt mutatja, hogy a rekurzió programkód alapú elemzését a legtöbb, programozási készségeit tekintve kezdő diák, nehézk esnek találja.   Ezen okból kifolyólag, napjainkra már nagyon sok segédeszköz elérhető számítógépes szoftverek, illetve az online térben weboldalak formájában , amelyek arra hivatottak, hogy segítsék a diákokat a rekurzió elsajátításában. Általában ezek a segédeszközök a rekurzió vizualizálásával foglalkoznak, a legtöbb esetben egy fa struktúrát hozva létre , ahol a fának a levelei a rekurzív hívásokat szemléltetik.  A fa struktúra által való vizualizációnak viszont van egy eléggé szembetűnő gyengesége. A viz ualizáció jól működik kisebb értékekre, viszont ahogy növekedik a bemeneti adatok értéke, egyre nehezebbé válik a vizualizáció értelmezése.   Ennek okán született meg az a gondolat, hogy hozzunk létre egy olyan oktatási, illetve kutatási  eszközt, amely más szemszögből közelíti meg a rekurzió vizualizálását. Az általam készített szoftver a hagyományos fa struktúra helyett, egy koordináta rendszerben ábrázolja a rekurzív függvényeket , ezáltal könnyebbé téve annak megértését, hogy a rekurzív hívások milyen mély ségeket járnak be mielőtt visszatérnek az eredeti hívó füg gvényhez.  Ezen vizualizációs módszer a bemeneti adatok növelésén kívül, lehetővé teszi különböző mintázatok ismétlődésének a megfigyelését bizonyos függvényeknél, megfelelő felületet nyújtva  ezáltal  azok számára is akik nemcsak megérteni, hanem kutatni is szeretnék a rekurzió jelenségét .  2.Elméleti megalapozás   A rekurzivítás mint fogalom, az életünk számos területén felbukkan. A rekurzió megfigyelhető például a természetben és a matematikában is. K étségtelen viszont, hogy a rekurzió fő felhasználási területe nem más mint az informatika.  Tekintsük át most röviden ezeket a területeket.  13  2.1. A rekurzió története   Amikor a rekurzióra gondolunk, valószínű, hogy első meggondolásra a modern kor számítógépei és az ezekre megírt rekurzív programkódok jutnak eszünkbe. Nem sokan gondolnák, de rekurzív definiciók már az ókori és középkori matematikában is megjelentek. Ezen definíciók egyik legismertebb példája a Fibonacci számsorozat mely et a 13. -ik században Leonardo di Pisa jegyzett fel . A Fibonaccihoz hasonló számsorozatok már az időszámításunk előtti 700 -as évektől megtalálhatók különböző egyiptomi, görög és szanszkrit iratokban  [1]. A Fibonacci számsorozat megadható az alábbi rekurzív  kapcsolattal :  2.1 ábra . Fibonacci számsorozat [ 9]  A 19. -ik század közepére megnőtt az érdeklődés a rekurzió iránt, és a függvénydefiníciók egyik módozataként kezdték használni. Ebben az időszakban például Grassman és Pierce rekurzív definíciókat adott az összeadás, illetve a szorzás műveleteknek  [1].  2.2 ábra . Összeadás és szorzás rekurzív képletek[1]  A 20. -ik sz ázad elején egy a Thoralf Albert Skolem által kiadott cikk nagy befolyással volt a rekurzió számítástechnikai elméletének fejlődésére. Ezen cikk tartalmaz egy leírást olyan függvénekről, amelyeket napjainkban primitív rekurzív függvényeknek nevezünk [1]. Skolem, illetve a későbbiekben Hilbert, Bernays és Ackermann munkássága nagyban hozzájárult a rekurzió számítástechnikai felhasználásának megs zületéséhez.  14  2.2. Rekurzió a matematikában    Amint azt már az előző alpontban is megemlítettük, a matematika volt az a tudományág, amely elsőként használta valamilyen formában a rekurzivítás fogalmát [1]. A matematikában a rekurzió egy ik klasszikus p éldája a faktoriális függvény amely kijelenti, hogy n ! = n * (n -1)!ahol n egy po zitív ternmészetes szám kell hogy legyen. Ez a rekurzív folyamat egészen addig folytatódik amíg az (n -1) egyenlő nem lesz 0 -val, ugyanis a 0 ! = 1. Ha egy programo zásban használatos kifejezést szeretnénk használni, a 0 ! az algoritmus meg állási feltételének felel meg.   A matematikában egymásba ágyazott rekurzióra is találunk példákat. Megemlíthetnénk például az Ackermann függvényt, mely a nevét a felfedezőjéről, Wilhelm Ackermannról ka pta. Az Ackermann függvény a,  teljesen kiszámítható függvények közé tartozik, viszont nem primitív rekurzív. Az idők során nagyon sok változata elterjedt, melyek közül az egyik legismertebb az Ackermann -Péter függvény, amely a következőképpen definiálható [2]:  2.3 ábra . Ackermann képlete [2]   Egy másik klasszikus példa amírő l bővebben szeretnénk beszélni ebben az alpontban, az nem más, mint a már említett Fibonacci szá msorozat. Ez a számsorozat a végtelenségig növelhető, de  vegyük most csak  az első  tíz elemét : 0, 1, 1, 2, 3, 5, 8, 13, 21, 34, 5 5.  Az n. -ik Fibonacci szám a következő rekurzív képlettel írható fel: F(n) = F(n -1) + F(n -2) ahol az n egy pozitív természetes szám, amely nagyobb mint 1. Első látásra ez a számsorozat lehet, hogy nem túlságos an érdkefeszítő, de figyeljük meg egy kicsit, hogy mi történik akkor, ha minden egyes számot elosztuk az előtte található Fibonacci számmal. Ha ezt megtesszük a következő számsorozatot kapjuk : 1/1, 2/1, 3/2, 5/3, 8/5, 13/8, 21/13, 34/21 , 55/34. Ezen os ztások eredményei : 1, 2, 1.5, 1.667, 1.625, 1.615, 1.619, 1.617. Megfi gyelhető, hogy ahogy a számok növekednek, az osztások eredményei egyre inkább közelítenek az 1,618033988749 895-ös 15  számhoz, ami nem más mint az aranymetszet. A 2.4-es ábrán az aranymetszet al apján megrazolt aranyspirál látható. Az aranymetszet, többek között a természetben is megfigyelhető. [3]    2.4 ábra.  Arany spirál [3]  2.3 Rekurzió a természetben    A rekurzivítás meglepően sok formában fellelhető a természetben. Rekurzív jellegeket figyelhetünk meg például hegyek, felhők és folyók elágazó szerkezetében, de még az állati bőr mintázataiban is.  A növényvilágban is számtalan példát találunk, amikor egy növény önmagára hasonlító mintázatokat mutat, a nagyobb forma mitha saját magának kise bb változatait hordozná magában. Természetesen a természet korlátozva van a rekurziót tekintve, ezek a kisebb formák nem zsugorodnak össze a végtelenségig [4]. Ezen növények ékes példája, az úgynevez ett Romanesco brokkoli ami a 2.5 -ös ábrán látható.   A term észetben  az önhasonló alakzatokon kívül megfigyelhető még az előző alcímben fejtegetett aranymetszet jelenléte is.  Ez a szabályosság megfigyelhető külünböző virágok szirmainak , illetve a napraforgóvirág megvainak elhelyezkedésében.  16                                  2.5 ábra  Rekurzív brokkoli [10]                             2.6. ábra  Aranymetszet a természetben [11] 2.4 Rekurzió a programozásban    Ezen alcím alatt a rekurzió fő felhasználási területéről fogunk beszélni, ami nem más mint a számítógépes programozás. A programozásban azt a folyamatot nevezzük rekurziónak, amikor egy függvény önmagát hívja meg, egy feladat megoldásának érdekében.  A rekurzió alap kérdéséül az szolgál, hogy hogyan lehet egy feladatot visszavezetni egyetlen egyszerűbb feladatra.  Ha egy aDr. Kátai Zoltán által használt hasonlattal  szeretnénk élni a rekurzív hívásokat tekintően, mondhatnánk azt is, hogy a függvény amel yből kiindul a rekurzív hívás, létre hoz egy klónt saját magáról  és a feladatának nagy részét át adja ennek a klónnak. Ez a klón ugyan azt az alapelvet követi, így létrehoz magáról egy következő klónt. Ez a folyamat nem folytatódik a végtelenségig, mivel  a függvényhívás feltételes kell legyen, ami azt jelenti, hogy van egy megállási feltétele, ami ha beteljesül, többé már nem jön létre egy következő klón , hanem vissza térítődnek az értékekek  az előző klónokhoz . Típusait tekintve a rekurziót két  különböző ré szre bonthatjuk : direkt vag y közvetlen rekurzió, illetve indirekt vagy közvetett rekurzió. Direkt rekurziónak nevezzük azt amikor egy függvény saját magára hivatkozik amikor függvényhívást végez. Indirekt rekurziónak azt nevezzük amikor egy rekurzív függvé ny nem saját magát hívja meg, hanem egy másik függvényt, amely szintén nem önmagát hívja meg, hanem azt a fügvényt aki őt meghívta.   17  2.5 Ciklus VS Rekurzió    A rekurzió ellenpárja az iteratív ciklusos megoldás.  Annak ellenére, hogy ellenpároknak hívjuk őket , a rekurz ív függvényeket ciklussá lehet alakítani és ugyan így az iteratív ciklusokat rekurzióvá. Elmondható, hogy az iteráció  gyorsabb a rekurziónál, mivel a rekurzió esetében függvényhívás történik, ami meg növeli a futási időt. A rekurziónak eg y másik hátránya az, hogyha a rekurzió túl nagy mélységeket jár be, akkor feltelhet a verem.   De miért éri meg akkor rekurziót használni ? A rekurzi ó ereje nem a gyorsaságában, hanem az eleganciájában rejlik. Sok esetbe n a rekurzióval megoldott feladat tömörebb és jobban olvasható mint az iterációs ellenpárja. Ennek egyik ékes példája a Hanoi tornyai nevű feladvány. A Hanoi tornyai rekurzív implementálása nagyon rövid és elegáns . Lásd 2.7  ábra.    2.7 ábra . Hanoi tornyai rekurzív implementációja  Ezzel ellentétben, Hanoi tornyai iteratív implementálása még sok informatika tanárt is gondolkodóba ejtene. Fi gyeljük meg egy kicsit a 2.8 -as és 2.9 -es ábrán ezt a megvalósítást is, a fentiekben látott bemeneti értékekre.  Ezeken  az ábrákon megfigyelhető, hogy Hanoi tornyai iteratív megvalósítása több mint tizszer annyi kódolást igényel mint a rekurzív megvalósítás . 18   2.8. ábra  Hanoi t ornyai iteratív megvalósítás    2.9. ábra Hanoi t ornyai iteratív megvalósítás   Ezen két megvalósításból  láthatjuk, hogy a a re kurziót igenis megéri használni, mert a példaként említett Hanoi tornyai probléma rekurzív megvalósítása sokkal  érthetőbb,  rövidebb  és elegánsabb mint az iterációval megírt ellenpárja . 19  2.6 A rekurzió oktatása    A reku rzív programozás egyike azon témáknak, amelynek tanítása során az oktatók előszeretettel nyúlnak bizonyos oktatási segédeszközökhöz. A legtöbb ilyen segédeszköz  a látást célozza meg mint felhasználandó érzéket, mivel felismerték, hogy a látás fontos szerep et játszik az új fogalmak elsajátításában. Ezen felismerés különböző kutatási vonalakat nyitott meg a rekurzió oktatását tekintve, mint például a rekurzió vizuális analógiái, vagy a programok eredményének animálása [13].   Az analógiákat tekintve az oktatók és kutatók túlnyomó többsége ugyan azokkal a példákkal áll elő, ilyen például a rekurzív mintázatokat mutató brokkoli, a fák ágai, illetve az egymással szembe helyezett tükrök tükröződései.  A kutatások során nem csak tárgyakat, hanem külöböző rekurzív foly amatokat is megvizsgáltak mindennapi példák segítségével. Megvizsgálták például azt, hogy hogyan értelmezik a gyerekek az egymás mellé helyezett dominók eldőlését [13].  A 12 év körüli és idősebb gyerekek esetében a dominók eldőlésének leírásában megfigyelh ető a rekurzív gondolkodás, mivel a gyerekek megfigyelték, hogy minden dominóelem eldőlését az előtte levő dominó okozta. Ezzel ellentétben, a 12 évnél fiatalabb gyerekek esetében a leírás inkább iteratív jellegű, eldől egy dominó, majd a következő, egésze n ameddig egy se marad állva[13].   A rekurzi ót kutató személyek  számos javaslatot tettek a rekurziós gráfok használatára, annak érdekében, hogy gyorsítani lehessen ezáltal a kezdőknél a rekurzió elsajátításának a folyamatát. Ezen gráfok lehetővé teszik a d iákok számára a függvényhívások kiértékelésének a követését  és mélyebb elemzését . Ha ezen gráf egy bináris fa, akkor minden egyes csomópont ugyan azt a függvényhívást jelenti [13].     20  3.Hasonló alkalmazások  és munkák    3.1. VisuAlgo     A “VisuAlgo” egy interneten el érhető weboldal, amely animációk segítségével próbál vizualizálni különböző adatstruktúrákat és algoritmusokat .[5] Az oldal segítségével többek között képesek vagyunk vizualizálni rendezéseket, láncolt listákat, hasító táblákat, és nem utolsó sorban, a rekurziót .   3.1 ábra  VisuAlgo Fibonacci(5) értékre [5]  A „VisuAlgo” a rekurziót egy fa struktúra segítségév el vizualizálja, ahogy ezt a 3.1 -es ábra is mutatja.  Az oldal bal alsó sarkában található egy mező, amely segítségével ki tudjuk választani, hogy mit i s szeretnénk vizualizálni. A 3.1 -es ábrán például a Fibonacci számok vizualizációja van kiválasztva n =5 értékre. A Fibonacci számokon kívül további 19 függvé ny vizualizációjára ad lehetőseget a program, amelyeknek forráskódját ki is vetíti egy szövegdobozba. Lehetőség van saját kód kipróbálására is, ugyanis a lenyíló listában az utoló elem a „Custom code” nevet viseli, ha ezt kiválasztjuk, akkor megírhatjuk a szövegdobozban a saját kódunkat JavaScript programozási nyelv segítségével.   21   Ahogy a 3.1 -es ábra jobb oldalán is megfigyelhető , a fa struktúra levelei különböző színeket  vesznek fel. A legalsó szinteken található levelek a zöld színt veszik fel, ezek a le velek azokat a rekurzív hívásokat jelölik, amikor a megállási feltétel igaznak bizonyul és elkezdődik az értékek visszatérítése.  A levelek fehér színűek amikor egy hívás az adott n értékre először történt meg.  A program világoskék színnel jelöli azokat a h ívásokat amikor  az n bemeneti értékre a hívás egyszer már feldolgozásra került [5]. Vegyük például az ábra alapján a Fibonacci(2) – es értéket. Mivel a bináris fa balról jobbra kerül bejárásra, a fa leginkább baloldalán található kettes értékű levél fehér színnel van jelölve, míg az utána következő összes többi kettes értékű levél kék színnel lett jelölve.   Következtetésként kijelenthető, hogy a “VisuAlgo” hasznos  segédeszköznek bizonyu l a rekurzió vizualizálását illetően, és mint diákok, mint tanárok hasznát vehetik akik többet szeretnének tudni a rekurzióról.   3.2.Sort Visualizer    A “Sort Visualizer” szintén egy interneten elérhető weboldal, amely rendezési algoritmusok vizualiz álására specializálódott. A 16 darab vizualizálható a lgoritmus közül van néhány amely előszeretettel alkalmazza a rekurziót. Ilyen algoritmus például a quicksort, illetve a merge sort. Ezen alpont keretén belül szeretnénk bemutatni ezeknek a vizualizációját a program segítségével.   A quicksort vagy g yorsrendezés a divide et imp era elv alapján működik. A rendezendő listát egy pivot segítségével két különálló részre bontja, majd erre a két új listára külön külön ismét meghívja a gyorsrendezést. [6] Ez a rekurzív folyamat addig folytatódik, amíg az átadott lista hossza kisebb vagy e gyenlő nem lesz 1 -el. Nezzük meg hogyan is vizualizálja ezt a rendezést a program. Lásd 3.2  ábra.     22   3.2 ábra . QuickSort  a Sort Visualizer  programban  [12]  Első lépéskent a rendező algoritmus végig iterál a listán, és elkezdi kicserélni a kiválasztott pivot elem két oldalán levő értékeket. Azokat az elemeket amelyek kisebbek mint a pivot a bal oldalára rendezi, míg azokat amelyek nagyobbak a jobb oldalára. Ez után következik az algoritmus rekurzív része , amit az előbbiekben már ismertettünk. Megfigyelhe tő hogy a lista legeleje kerül leghamarabb rendezésre, ez annak köszönhető, hogy az oszd meg és uralkodj módszert használó algoritmus, először a pivot bal oldalán levő listára hívja meg rekurzívan a quicksortot.   A következőkben figyeljük meg egy kicsit, h ogyan figyelhető meg a rekurzió a merge sort esetében.  Lásd 3.3  ábra.   3.3 ábra . Merge Sort a  Sort Visualizer  programban  [12] 23    A merge sort a quicksorthoz hasonlóan az oszd meg és uralkodj módszert alkalmazza. A rendező algoritmus rekurzívan felosztja a bemeneti listát, egészen ameddig az átadott lista csupán egyetlen elemet tartalmaz. Amint ez megtörténik, a részsorozatok összevonódnak és rendezésre kerülnek. Az algoritmus fokozatosan összevonja a részlistákat, egészen addig amíg egyetlen rendezett lista  marad a végén.[7]  Az összevonás folyamata a 3.3 -as ábrán is nagyon jól megfigyelhető.   Összességében kijelethető, hogy a “Sort Visualizer” is sokat tud segíteni egy felhasználónak a rekurzió megértésében.      3.3 Rekurzió kutatása a Sapientia egyetemen     A Sapientia Erdélyi Magyar Tudományegyetem Marosvásárhelyi karán a 2008 -as évben Dr. Kátai Zoltán vezetésével elvégzésre került egy kutatás, amelynek keretén belül egy úgynevezett többérzékelős módszert probáltak ki a rekurzió oktatására.  Ezen alpontban bemutatásra kerül ez a kutatás, amely a [8] –as cikkben található, és az ehhez fejlesztett szoftver is bemutatásra kerül.   A kutatás egyik részeként megkértek az egyetem diákjai közül néhányat, hogy játszák el egy rekurzív függvény futási f olyamatát. Az első diák szemléltette a main függvényt, míg a többiek  a rekurzív függvény példányait szemléltették. Amikor egy a cikk által rekurzív szereplőnek megnevezett diák meghívásra került, a szereplő kilépett a meghívója mögül és elkezdte elemezni az általa kapott feladatot. Két lehetősége volt, követi a rekurzív forgatókönyvet, vagy követi a triviálisat , ami a megállási feltétel teljesülését jelentette. Ha az első lehetőséget választotta, akkor meghívta a társát  és saját magát felfüggesztette amíg nem kapott választ a hívásra. A legutolsó diáknak a triviális forgatókönyvet kellett választania, mivel akkor teljesült a megállási feltétel. Neki az volt a dolga, hogy a részfeladatának az eredményét átadja a hívójának, aki ennek hatására felébredt a felf üggesztett állapotából és ugyan ezt a 24  műveletet elvégezte.  Ez a folyamat addig folytatódott amí a main függvényt szemléltető diák megkapta az eredményt [8].   Ezen kísérlet segített a diákoknak jobban megérteni, hogy hogyan is működik a rekurzió.  A néző diá kok megérthették belőle a rekurzív folyamatok működését, míg azok a diákok aki eljátszodták folyamatokat, kinetikus módon is memorizálták a rekurziót, a műveletekhez kapcsolódó mozgások által  [8].  A kutatás egy másik fontos része , egy a rekurzió oktatására  kifejlesztett szoftver kipróbálása volt.  Ezen szoftver audio -vizuális eszközökkel próbálja megértetni a felhasználóval a rekurzivítást. A rekurziót a program lépcsőzetesen vizualizálja, ezáltal minden egyes rekurzív hívás egy úgynevezett emelete t hoz létr e . Lásd 3.4 -es ábra. Minden egyes emeleten a vizualizációhoz egy zenei bejátszás is társul, melynek hangmagassága az emelet magasságának függvényében növekszik.   3.4 ábra.  Rekurzió lépcsőzetes ilusztrációja  [8]  A kísérletben 43 nagyjából azonos képességekkel rendelkező  első éves  diák vett részt . A diákokat két csoportra osztották, 23 -at közűlük a tradicionális módszerekkel tanítottak, míg a megmaradt 20 diáknál az előbbiekben említett módszereket használták a rekurzió oktatására. Az utólag os teszt eredmények azt mutatták, hogy akiket a többérzékelős módszerekkel tanítottak, jobban teljesítettek mint azok a társaik akik tradicionális oktatásban részesültek. [8] Ezen kísérlet ékes példája annak, hogy a különböző segédeszközök könnyebbé tudják tenni a rekurzió megértését és tanulását.  25  4.Szoftver tervezése és kivitelezése    A dolgozat ezen részében bemutatásra kerül a szoftver, amelyet a rekurzió lépcsőzetes módszerrel való vizualizálásához fejlesztettem. Az alkalmazás  egy Windows Form aplikáció amely  C# programozási nyelven íródott és a .Net keretrendszer 4.7.2 - es verzióját használja.  A szoftver lehetőséget ad rekurzív függvények illetve rekurzív eljárások vizualizációjára.  A különbség a két fogalom között az, hogy míg a rekurzív függvény vissza  térít egy eredményt a hívójához, addig a rekurzív eljárás csupán elvégez egy feladatot anélkül, hogy bármit is vissza térítene a hívójához. Természetesen a rekurzív eljárásokban is jelen van a megállási feltétel [14].  4.1 Felhasználói követelmények    Az szoftver  elindítása  után, a felhasználó előtt egyenesen az alkalmazás fő ablaka jelenik meg. Ezen a fő ablakon történik meg a rekurzív függvények vizualizálása egy koordináta rendszerben. Az elindítás pillanatában a fő ablakon három gomb jelenik meg, a “Choose File”, “Run”, illetve a “Write own c ode” elneve zésekkel.   A “Choose File”  gomb lenyomásávál egy különálló ablakban megnyílik  a projektnek a könyvtára, ahol a felhasználó ki tudja választani az előre megírt rekurzív jellegű függvények közül azt amelyiket vizualizálni szeretné. Minden egyes függvény különálló .txt kiterjesztésű fájlokban van megírva, a felhasználónak csak annyi a  feladata, hogy kiválassza a fájlt és megnyomja az „Open” gombot.  Miután ki lett választva a függvény, a szoftver átvizsgálja a kapott függvényt és megállapítja, hogy hány paraméter megadására van szüksége az adott függvénynek. Annak fügvényében, hogy ez a  szám mennyi, a szoftver kigenerálja azokat a szövegdobozokat ahova a felhasználó be tudja írni az értékeket. Például, ha kiválasztottuk a faktoriális függvényt, aminek meghívásához egyetlen paraméterre van szükség, a program egyetlen szövegdobozt fog létr ehozni ahova be tudjuk írni ezt az értéket.   A “Run” gomb lenyomásával tudjuk elindítani az előző lépésben kiválasztott függvény vizualizációját. Ha sikeres volt a program lefuttatása, akkor az ablak gombok alatti üres részében megjelenik a függvény vizual izációja. Abban ez esetben ha nem választottunk még ki egyetlen 26  függvényt sem amit vizualizálni szeretnénk és megnyomjuk a “Run” gombot, a szoftver egy üzenetet közvetít a felhasználó felé, hogy előbb válasszon ki egy függvényt és csak azután nyomja meg a “Run” gombot. Hasonl ó figyelmeztetést kapunk abban az esetben  is ha a kigenerált szövegdobozokba egy érvénytelen karaktert ütünk be. Minden beütött érték szám kell hogy legyen, ennek értelmében ha egy betüt adunk meg paraméterként, a szoftver figyelmeztet,  hogy a megadott paraméter nem érvényes.   4.1 ábra.  Use case diagramm   27   A “Write own c ode” gomb megny omásával egy új ablak fog megnyílni a felhasználó előtt. Ebben az új ablakban lehetőség nyílik arra, hogy a felhasználó egy saját maga által szerkesztett kódot is levizualizáljon. Az ablak megnyitásakor még nincs kigenerálva az a szövegdoboz , ahova a felhasználó beírhatja a saját C # nyelven megírt kódját, viszont az ablak legtetején talál két gombot, név szerint a “Direct Recursion” és az “Indirect Recursio n” gombokat. Ezek a gombok azért szükségesek, hogy a felhasználó ki tudja választani a kívánt rekuzió típusát. Ha a felhasználó a “Direct Recursion” gombot n yomja meg akkor egyetlen szövegdoboz kerül kigenerálásra, mivel a közvetlen rekurzióhoz csak egyetl en megírt függvényre van szükség. Ha az “Indirekt Recursion” gombot nyomja meg a felhasz náló, két szövegdoboz generálódik ki, mivel a közvetett rekurzióhoz legalább két függvényre van szükség. Az előzőekben feldolgozott fájl kiválasztásos módszernél azért nem volt szükség hasonló műveletre, mivel a szoftver a beolvasott szöveges fájl alapján el tudja dönteni a rekurzió típusát.   4.2 ábra . Activity diagramm  28   Miután ki lett generálva a megfelelő számú szövegdoboz a függvények beírásához, a felhasználó neki kezdhet kódolni. A szövegdoboz első sorába a felhasz náló az úgynevezett “method signaturet” kell hogy beírja, amely tartalmazza a függvény nevét, típusát, és  a függvény paramétereit. Miután az első sor be lett írva, enter gomb lenyomására a program meghatározza, hogy hány paramétere van a megírt metódusnak, amely után kigenerálja a megfelelő mennyiségű szövegdobozt a paraméterek értékeinek megadására. Abban ez  esetben ha hibát vétettünk ezen műveletek közben, például nem adtunk meg megfelelő mennyiségű paramétert az első sorban, de már kigeneráltuk a paraméterek szövegdobozait, nyomjuk meg a “Clear all” elnevezésű gombot, mely vissza állít mindent az eredeti ál lapotára.Ezután előlről kezdhetjük az előbbiekben vázolt műveleteket. A füg</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -644,6 +719,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>A dolgozat témája  egy webalkalmazás  fejlesztése , amely a hallgatókat, a cégeket és az egyetemeket a szakmai gyakorlat tevékenysége során köti össze . A cél az, hogy egy könnyen használható, felhasználóbarát platformot fejlesszek, amely képes a szakmai gyakorlatokkal kapcsolatos teljes folyamat lebonyolí tására.   A projekt egyik célja, hogy a hallgatók és a cégek számára egy szakmai  közösségi platformként működjön az alkalmazás, ezáltal elősegítve a szakmai kapcsolatok kialakulását, valamint a cégek és az egyetemek közötti partneri kapcsolatok ápolását.   A projekt másik fontos célja, hogy a platformon a hallgatók a saját profiljuknak és szakjuknak megfelelően kapjanak ajánlásokat. Ez lehetővé teszi számukra, hogy releváns lehetőségeket találjanak a szakmai gyakorlatok terén. Az ajánlórendszerem  algoritmusa i, például a Cosinus hasonlóságot felhasználva figyelembe veszik a hallgatók készségeit, érdeklődését és a cégek által meghatározott követelményeket. Így a platform segít a hallgatóknak a legmegfelelőbb gyakorlati helyek megtalálásában, optimalizálva ezzel  a kapcsolódó folyamatokat és eredményessé téve a gyakorlatokat.   A projekt elkészítéséhez modern webes technológiákat használok, Angular -t, Java Spring Bootot, PostgreSQL -t és AWS -t. Ezek segítenek a platformomat robusztussá, skálázhatóvá biztonságossá és  gyorssá tenni.</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -657,6 +737,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>A biztonsági rendszerek az emberek, vállalkozások és intézmények számára egyarántfontosak a biztonságos környezet fenntartásához és az anyagi javak megóvásához. A maimodern technológia erre változatos megoldásokat nyújt. Minden ilyen rendszernek fcélja kiszrni az illetéktelen behatolókat a belép joggal rendelkez emberek közül. Abeléptet rendszerek erre egy hatékony valós idej megoldást kínálnak. Az épületekbevaló bejutást csak azoknak a személyeknek teszik lehetvé, akik megfelel engedéllyelrendelkeznek, tehát hitelesíteni tudják magukat.A diplomamunkám témájának egy biometrikus beléptet rendszer megvalósításátválasztottam, ami arcfelismerés segítségével azonosítja az embereket. Célom volt egykönnyen kezelhet, gyors, hatékony és els sorban biztonságos rendszer megvalósításaegy költséghatékony módon, ezzel megkönnyítve az emberek mindennapjait, illetve le-egyszersítve az épületekbe belépni vágyó személyek azonosításását.A nagymérték biztonság érdekében a biometrikus azonosítási módszerek közül azarcfelismerést választottam, ez egy széleskörben ismert és használt technológia, gyakranhasználják biztonságos számítógépes rendszerekhez, laptopokhoz, okostelefonokhoz vagybankautomatákhoz. Az elnyei mellett megemlíthet, hogy nem igényel közvetlen ﬁzikaiérintést az azonosítás során, illetve gyors és hatékony módszer.Más hasonló azonosításhoz viszonyítva biztonságosabb, illetve nehezebben átjátszha-tóbb egy arcfelismerésen alapuló rendszer. A jelszavak és PIN kódok könnyen kitudódhat-nak, feltörhetek, a különböz kártyák és kulcsok pedig elveszíthetek vagy ellophatóak,így illetéktelen kezekbe kerülve visszaélés történhet a biztonsági intézkedésekkel szemben.Ezeket a szempontokat szemeltt tartva terveztem meg a rendszer mködését. Abelépéshez feltétel hogy az adminisztrátor hozzáadja a személyek adatait és képeit. Enneka feltételnek a beteljesülésével belépésre jogsult az épületbe. A felhasználó egyszerencsak a kamera elé áll, megfelel ható távolságban és ha megtalálható a rendszerben, akkorkinyílik az ajtó és beléphet. A könny használat érdekében létrehoztam egy felhasználóifelületet is, amelynek segítségével egyszeren hozzá lehet adni a személyeket, illetve akövethetség érdekében megtekinthet az épületbe belép személyek listája is, pontosbelépési idvel együtt.Az általam megvalósított rendszer megkönnyíti a belépés során az azonosítás folya-matát, és egy biztonságos megoldást nyújt az illetéktelen személyek kiszrésére a min-dennapokban</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -670,6 +755,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>A dolgozat célja egy web alkalmazás, amely digitalizálja a diploma témák választását.Szükség volt egy megoldásra, ami segítene és megkönnyítene hallgatók munkáját a dip-loma témával kapcsolatos teendknél.Célkitzések közé tartozott egy olyan web applikáció lefejlesztése, amely képes nagy-számú adatot és felhasználót kezelni és könnyedén használható bárki számára. Az adottapplikáció feleljen meg minden egyetemi elvárásnak és kérés esetén tovább fejleszthetlegyen. Legyen biztonságos és biztosítva legyen, hogy az applikáció karbantartható.Sikerült megvalósítani a célkitzéseket minden terén. Egy olyan web applikáció szü-letett, amelyet azoak a személyek használhatnak akik részt vesznek a diploma dolgozatokmeghirdetésében és hallgatókhoz való hozzárendelésében. A tanszéki titkárok és munka-folyamatot hozhatnak létre és meghívhatják a tanárokat és a hallgatókat a rendszerbe. Atanárok feltölthetik a diploma témáikat és a hallgatók jelentkezhetnek azokra. Vendégekpedig megtekinthetik az elkészített diploma témákat.A fejlesztéshez használtam az Angular és Spring Boot keretrendszereket, melyekneksegítségével egy skálázható és biztonságos web applikációt lett fejlesztve. Az adatoktárolásához a PostgreSQL adatbázis használva és a karbantarthatóság érdekében tesztelkeretrendszereket és applikációkat, a Cypress-t és Postman-t.AbstractThe aim of the thesis is to design and develop a web application that digitises thechoice of subjects for the diploma. A solution was needed that would help and facilitatethe work of the university committee and students in the diploma topic selection process.Our objectives included the development of a web application that could handle alarge number of data and users and could be easily used by anyone. The applicationshould meet all university requirements and could be further developed on request. Besecure and ensure that the application is maintainable.The objectives have been achieved in all areas. A web application has been developedthat secretaries can log into and create periods and invite teachers and students to thesystem. Teachers can upload their degree topics and students can apply for them. Andguests can view the diploma topics they have created.A wide range of technologies have been used in the development. Most prominent arethe frontend and backend frameworks. Using Angular and Spring to boot I was able todevelop a highly scalable and secure web application. Using PostgreSQL database to storedata and testing frameworks and applications Cypress and Postman for maintainability.TartalomjegyzékÁbrák jegyzéke 3Táblázatok jegyzéke 41. Bevezet 52. Elméleti megalapozás és szakirodalmi tanulmány 72.1. Szakirodalmi tanulmány ........................... 72.2. Elméleti alapok ................................ 82.2.1. Hatékony eszközök a webalkalmazások fejlesztéséhez ........ 82.3. Ismert hasonló alkalmazások ......................... 82.4. Felhasznált technológiák ........................... 92.4.1. Angular frontend keretrendszer ................... 92.4.2. Spring boot backend keretrendszer ................. 102.4.3. Szervletek ............................... 132.4.4. Postgres és annak kezelése ...................... 142.4.5. Liquibase ............................... 152.4.6. Tesztelést elsegít frameworkok ................... 152.4.7. Verzió követ és feladat vezérl alkalmazások ............ 163. A rendszer speciﬁkációi és architektúrája 173.1. Követelmény speciﬁkációk .......................... 173.1.1. Funkcionális követelmények ..................... 173.1.2. Nem funkcionális követelmények ................... 213.2. Adatbázis ................................... 223.3. Alkalmazás architektúra ........................... 244. Részletes tervezés 304.1. Tervezési fázisok ............................... 304.1.1. Frontend ................................ 304.1.2. Backend ................................ 424.2. Tesztelés .................................... 484.2.1. Frontend tesztelés ........................... 484.2.2. Backend tesztelés ........................... 504.2.3. Éles tesztelés ............................. 5115. Üzembe helyezési lépések 525.1. Felmerült problémák és megoldásaik .................... 525.1.1. Idszakok beintegrálása az applikációba ............... 525.1.2. Hallgatók leosztása automatikusan ................. 536. Következtetések 546.1. Megvalósítások ................................ 546.2. Továbbfejlesztési lehetségek ......................... 54Irodalomjegyzék 56Függelék 57F.1. Kód részletek ................................. 572Ábrák jegyzéke2.1. Különbség egy MPA (Multiple Page Application) és egy SPA (Single PageApplication) között [ 8]............................ 92.2. Angular applikáció elemi felépítése [ 1].................... 102.3. Mikroszolgáltatások felépítése [ 5]...................... 112.4. Rétegelt architektúra megvalósítása Spring bootban. ............ 122.5. ORM mködése[ 4].............................. 143.1. Adatbázis diagram .............................. 243.2. Alkalmazás architektúra [ 3]......................... 254.1. Frontend oldali typescript osztály ...................... 374.2. Szerver oldali java osztály .......................... 374.3. Cypress tesztelés ............................... 504.4. Postman tesztelés ............................... 504.5. Diploma téma jelentkezés hallgató szemszögébl .............. 514.6. Diploma téma leosztás eredményei ...................... 513Táblázatok jegyzéke3.1. Bejelentkezési funkció ............................. 193.2. Hallgatók feltöltése funkció .......................... 203.3. Diplomamunka létrehozása funkció ..................... 203.4. Véglegesíteni a leosztott eredményeket a saját szakukról funkció. ..... 203.5. Diplomamunkára jelentkezni funkció. .................... 213.6. Keresni az elvégzett diplomamunkák között név és</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -683,6 +773,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>A dolgozat célja a mellkasi röntgenfelvételek osztályozása tüdőgyulladás jelenléténekdetektálására. A kutatásban egy konvolúciós neurális hálózatot alkalmaztunk a pon-tosabb osztályozás elérése érdekében. Célunk az volt, hogy fejlesszünk egy hatékonyosztályozót, amely egy saját modell által létrehozott neurális háló, vagy egy GoogleNetarchitektúrájú neuronháló, amelyet “transfer learning” technikával saját célokra edzet-tünk fel.A kutatási módszerünk a meglévő megoldások tanulmányozásán, saját kísérletekenés adatgyűjtésen alapult. A “transfer learning” technikát alkalmaztuk a GoogleNet ar-chitektúrára, ami egy előzetesen tréningezett nagy modell, ezáltal javítva az osztályozáspontosságát. Az adatgyűjtés során tüdőgyulladással és tünetmentes esetekkel rendelkezőmellkasi röntgenfelvételeket használtunk.Az eredmények alapján sikerült fejlesztenünk egy grafikus felhasználói felületet, amelylehetővé teszi a mellkasröntgen automatikus osztályozását és a tüdőgyulladás diagnózisát.A GoogleNet architektúrájú neuronháló kiemelkedő pontosságot ért el a tesztelt adathal-mazon, és összehasonlítva a saját osztályozó hálóval, szignifikánsan jobb eredményeketprodukált, hasonlóan a szakirodalomból tanulmányozott háló eredményeihez.Ezen eredmények alapján arra a következtetésre jutottunk, hogy a jól megírt, aGoogleNet architektúrával együttműködő neurális háló hatékonyan képes detektál-ni a tüdőgyulladást a mellkasi röntgenfelvételek alapján. Ez a kutatás hozzájárulhataz orvosi diagnosztika fejlesztéséhez, segítve a korai felismerést és a hatékonyabb kezelést.</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -700,6 +795,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Az ember életében az egyik legértékesebb és legfontosabb dolog az idő. A mai rohanó világban annyira felgyorsultak az események, hogy valódi nehézséget jelent kézben tartani őket és jól menedzselni az időnket. Az időmegtakarítás céljából számos okos készül ék és rendszer jelent meg, megkönnyítve az emberek életét. Akár úgy is fogalmazhatunk, hogy az okos rendszerek korát éljük.  A dolgozatom témája is egy ilyen rendszert foglal magába. Nemcsak időt spórol a felhasználóknak, hanem egy felelősségtől is megszaba dítja őket. Ez a modern és innovatív megoldás lehetővé teszi, hogy gondoskodjunk növényeinkről a legmegfelelőbb módon, miközben minimalizáljuk a gondozási feladatokat és maximalizáljuk a virágok egészségét és szépségét. Segít, hogy a növények optimális áll apotát fenntartsuk, különösen akkor, amikor távol vagyunk otthonunktól vagy nem tudunk elég időt fordítani a gondozásra. Az érzékelők figyelik a környezeti paramétereket, azaz a hőmérsékletet és nedvességtartalmat. Az okos virágtartó rendszer automatikusan  szabályozza az öntözést és világítást, biztosítva a növények számára a megfelelő mennyiségű vizet és hőmérsékletet a megfelelő időben. Nem kell többé aggódnunk a túl vagy alulöntözés miatt, hiszen a rendszer precízen és pontosan gondoskodik a virágaink ví zellátásáról.  A felhasználói felület segítségével könnyedén beállíthatjuk az öntözési ütemtervet, profilokat hozhatunk létre, nyomon követhetjük a növények állapotát és a környezeti paramétereket. Akár otthon vagyunk, akár távol, a rendszer távoli elérést biztosít, hogy mindig kapcsolatban maradhassunk a növényeinkkel és szükség esetén beavatkozhassunk.  A rendszer vezérléséhez az ESP32 mikrovezérlőt használtam, ami egy rendkívül sokoldalú és erőteljes platform és feladata a rendszer teljes körű vezérlése és  felügyelete.</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -713,6 +813,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Az ipari robotok egyre inkább elterjednek a különböző gyártási és logisztikai folyamatokban, ahol a pontosság, a sebesség és a biztonság fontos szempontok. A robotok képesek automatizálni olyan feladatokat, amelyek unalmasak, veszélyesek vagy túl bonyolultak az emberek számára. Azonban a robotok és az emberek közötti együttműködés még mindig kihívást jelent, különösen akkor, ha a robotnak rugalmasan kell alkalmazkodniuk a változó környezethez és feladatokhoz.   Téglatest alakú tárgyak felismerése és mozgatása olyan feladat, amelyet számos ipari és oktatási célra használnak. A tárgyak típusának és elhelyezkedésének meghatározása azonban nem mindig egyszerű, különösen akkor, ha azok színükben vagy méretükben hasonlítanak egymásra. Ebben a dolgozatban egy olyan módszert mutatok be, amely a Baxter robot az ArUco kódok segítségével könnyeden megkülönbözteti a kockákat. Leírom, hogyan programoztam a Baxter robotot, hogy képes legyen meghatározni egy munkafelületen lévő tárgyak típusát és helyzetét, valamint rendezni azokat. A tanulmányom során részletesen bemutatom a rendszer tervezését, megvalósítását és tesztelését.  A dolgozatomban egy olyan rendszert fejlesztettem ki, amely képes a Baxter robotot vezérelni úgy, hogy képes legyen téglatest alakú tárgyakat felismerni és mozgatni. A rendszer három fő komponensből áll: egy képfeldolgozó modulból, amely az opencv valamit a cv2.aruco könyvtárak segítségével érzékelik és azonosítják a tárgyakat, egy kommunikációs modulból, amely ZMQ (ZeroMQ) protokollt használva küldi és fogadja az adatokat, és egy robotvezérlő modulból, amely ROS (Robot Operating System) könyvtárakat használva irányítja a robot karjait és megfogóit. A rendszer működése során a robot fényképet csinál a munkaterületről, meghatározza a tárgyak helyzetét és típusát, majd ezek alapján elvégzi a szétválogatást.</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -726,6 +831,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Napjainkban  minden  ember  rendelkezik  okostelefonnal,  amelyek  segítségével  rengeteg problémát megoldhat különböző alkalmazásokkal. Ilyen hasznos alkalmazások például a számláink kifizetésére szolgáló alkalmazások, de akár feladataink vezetésére is rengeteg alkalmazást találunk.  A  telefonos  alkalmazások  nem  csak  a  mindennapjainkat  könnyítik  meg,  hanem  akár  a tanügyi intézményekben is segítségünkre lehetnek. A legtöbb telefonos alkalmazás, amit előszeretettel használnak az iskolákban és az egyetemeken: a különböző számológépek, fordítók és a jegyzetelésre szolgáló alkalmazások.   Viszont a PowerPoint bemutatására szolgáló alkalmazások az emberek körében nincsenek elterjedve, ezért a számuk igen kevés és nem a legjobban karbantartottak vagy nem rendelkeznek sok lehetőséggel, amely értelmet adna ezen alkalmazások használatának azon kívül, hogy nem kell a felhasználó egy külön eszközt magánál tartson.   A dolgozatom célja egy olyan rendszer tervezése, amely segítségével PowerPoint bemutatók diáin lehessen lézer mutatót használni az okostelefonunk segítségével attól függetlenül, hogy  Android-os  vagy  IOS-es  telefonunk  van.  Ezen  felül  a  diák  közötti  váltást,  illetve  ezekre történő rajzolást is lehetővé tegye. A rendszer két komponensből épül fel: az egyik része a szerver, amely fogadja, illetve  feldolgozza a telefonunk  által küldött adatokat; a másik része  a telefon, amely a felhasználó kézmozdulatait érzékeli a telefonban található gyorsulásmérő segítségével, illetve a megjelenített gombok lenyomását is, amelyeket elküld a szervernek WiFi-n keresztül. A szerverhez történő kapcsolódáshoz szükséges adatokat a szerver által generált QR kód beolvasása teszi lehetővé.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -743,6 +853,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>A modern és gyor san fejlődő világban már minden szükségletünk, hobby és munka mögött egy elektromos technológia áll, amiket kényelmesen, gondok nélkül használunk. A mostani időkben az infláció emelkedésével minden szükségletnek az ára megemelkedett, legfőképpen az elektro mos áram, ezáltal, hogy ha nem figyelünk oda a mindennapi energia fogyasztásunkra és nem változtatunk az energia felhasználási szokásainkon, akkor könnyen anyagi gondokba ütközhetünk.  A dolgozatom célja egy olyan IoT (Internet of Things) rendszer kialakítá sa, amely lehetővé teszi a háztartáson belüli elektronikai berendezések fogyasztásának könnyű mérését és nyomon követését. Emellett a rendszer képes monitorozni a háztartásban telepített napelemek termelését is. Az adatokat egy adatbázisban tárolom, ami le hetővé teszi a későbbi statisztikák és elemzések készítését. Ezáltal pontosabb betekintést lehet nyerni az energiaköltségekbe, valamint segít optimalizálni a fogyasztást és kihasználni a megújuló energiaforrásokat.  A különböző egységek MQTT protokollon ker esztül kommunikálnak egymásközt, a publisherek(háztartási berendezés, napelemek) küldenek mintavételezett adatokat a brokernek(Raspberry pi), ahol az adatok fel vannak dolgozva, el lesznek tárolva egy MongoDB adatbázisban és a kész adatok egy REST API szol áltatáson keresztül el lesznek küldve egy mobilos applikációra.</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -760,6 +875,11 @@
           <t>2023</t>
         </is>
       </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Az elmúlt időszakban jelentős növekedést tapasztalhattunk az ipari robotok terén és felhasználási területük is folyamatosan bővül. Ezek a robotok egyre több funkcióval rendelkeznek és egyre szélesebb körben képesek emberi munkákat elvégezni. A kutatásunk során az ipari robotok vezérlésével foglalkoztunk, célunk egy rendszer kifejlesztése volt, amely rögzíti a felhasználó mozgását és ezek alapján számítja ki az ipari robot vezérléséhez szükséges jeleket.  Diplomadolgozatomban egy távoli vezérlésű kétkarú ipari robot vezérlésére alkalmas rendszer megoldását terveztük, amely az emberi kar mozgását használja alapul. A robot mindkét karját valós időben kellett vezéreljük, ezért a második generációs Kinect érzékelőt alkalmaztuk, amely alkalmas a mozgás követésére és távolság mérésére. A Kinect kamera által nyújtott adatokat olyan formába alakítottuk át, ami alkalmas egy robotkar vezérlésére. Az ipari robot karjainak vezérléséhez a felhasználó végtagjainak és ízületeinek szögeit használtuk. A kivitelezéshez egy fejlesztési célra tervezett Baxter kooperatív robotot használtunk, amely egy fix platformra rögzített robot, amely két, egyenként hét szabadságfokkal rendelkező, robotkarral rendelkezik. A rendszer lehetővé teszi a robot kézmozdulatokkal való vezérlését.  A rendszer a robotkar mozgatása mellett lehetővé teszi a felhasználónak, hogy a robotkar megfogó eszközeit kézmozdulatokkal vezérelje. A kéz állapota alapján a robot megfogó eszközei kinyílnak vagy bezáródnak.  A dolgozatban a robot vezérlésére a ROS (Robot Operating System) könyvtárait használtam. Emellett a Kinect kamera kezelésére a Kinect SDK-t, a komponensek közötti kommunikációra ZMQ protokollt használtam. Az így kifejlesztett rendszer képes felismerni a felhasználót, lekövetni a mozgását, és egy kétkarú ipari robotra ráilleszteni azt.</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -775,6 +895,11 @@
       <c r="C25" t="inlineStr">
         <is>
           <t>2023</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Atechnol ógiaifejlődésnekköszönhetőenazokostelefonok ésazinternet elengedhetetleneklettek azéletünkben, hiszen mindig kéznélvannak, ésmáramáregyfajta személyiasszisztens szerepet betöltve járulnak hozzáazéletünkmegkönnyítéséhez.Azéletünkmásiknagy részétmégmindig személyesügyintézésekéspapíralapúdokumentumokhatározzákmeg.Jólérezhet őegyfajta gátakétpólusköztmelyb őlazegyikre afolyamatosmozgás,gyorsas ágmígamásikraalassúság,időigényességjellemz ő.Adolgozat céljaegyhatékony ésgyors rendszer kidolgoz ásaamely révéneztagátatfeloldjuk, egyújfajta lehetőségetszolgáltatva abüntetésekügyintézésére.Ahagyom ányosmódszerek nem képesek lépésttartani afelgyorsult világunkkal, ésproblémákatokozhatnak, mint példáulabirságoknehézkes rendszerez éseésazebbőlfakadókifizet ésnek azelmúlasztása.Amaitechnol ógiai elvárásoknak megfelel őrendszerkidolgoz ásáttűztükkicélul.Arendszer kifejleszt ésesoránfigyelembe vettükmindk étfélt,akiabüntetéstkiosztja illetve akieztmegkapja, ésigyekezt ünkegyolyan megval ósításraamely mindk étszerepk örszámáraidőtakar ékosésgyors. Abüntetéskiszot ásáhozegyandroidos applik ációhaszn álatatűntalegmegfelel őbbnek, mivel atelefonunk állandóankéznélvanilletve interneten kereszt ülazonnali hozzáféréstistudbiztos ítaniafelhaszn álónak azadatbázishoz. Ajárművezetőknek szántrendszer kivitelez éséhezalegkézenfekv őbbnek egywebes felületmegval ósításatűntmivel ezáltalegyviszonylagnagyobb felületentudunk jobbrálátástnyújtaniszámukra abírságokkönnyebb átlátásáhozilletve kifizet éséhez.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add keyword extraction from PDFs
</commit_message>
<xml_diff>
--- a/szamteches_info_extracted.xlsx
+++ b/szamteches_info_extracted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Kivonat</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Kulcsszavak</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -472,6 +477,11 @@
           <t>A dolgozat egy olyan rendszert és annak felépítését mutatja be részletesen, amely a különböző hajtányokon történő irányváltásra és fékezésre vonatkozó jelzéseket kezeli, egy gyorsulásmérőt és giroszkópot tartalmazó szenzor segítségével, ami a kézfejen kap helyet.  A projekt megoldást próbál nyújtani a hajtányokon történő irányjelzésekre a kéz kormányról való levétele nélkül, ezzel elkerülve az ebből fakadó baleseteket. Az irányváltásra vonatkozó jelzéseket a felhasználó képes jelezni különböző gesztusok segítségével,  mint a kéz oldal irányú forgatása , így nem szükséges levennie a kezét a kormányról teljesen, ezzel megtartva a jármű egyensúlyát . A fékjelzések automatikusan történik a gyorsulás érzékelése köve tkeztében. A rendszer két mikrovezérlőt használ (ESP32 és ESP8266) amik közül az egyik a szenzor adatokat dolgozza  fel, míg  a másik futtat egy webszervert és megvilágítja a megfelelő led -eket. A webszerver a kommunikációért felel a mikrovezérlők között, va lamint egy felhasználói felületként funkcionáló weboldalt is üzemeltet. A weboldalon láthatóak az aktív jelzések , mint a kanyarjelzések és a fékjelzések , valami nt ki- és bekapcsolhatjuk ezeknek a működését . A különböző komponensek közötti kommunikáció veze ték nélkül valósul meg WiFi technológiát használva .</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>mikrovezérlő, WiFi, giroszkóp, gyorsulásmérő</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -492,6 +502,11 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>A dolgozat egy okosotthon vezérlőrendszer megvalósítását mutatja be. A rendszer elsősorban otthon automatizálási feladatokat lát el, mint például a hőmérsé klet szabályzása, a növények öntözése és a redőnyök automatikus mozgatása, ezzel megkönnyítve a felhasználó mindennapjait.  Napjainkban az IoT eszközök egyre fontosabb szerepet töltenek be az ember számára, már el sem tudjuk képzelni ezek nélkül az életünke t. Mivel az emberek nagy része rendelkezik otthoni internetkapcsolattal, ezért egy ilyen IoT rendszer kiépítése egyszerűbb, olcsóbb és hatékonyabb, mert nincs szükség vezetékekre az eszközök közötti kommunikáció megvalósítására.   Az általam fejlesztett és megépített  rendszer egy központi részből áll, amihez egy érintőképernyős kijelző van csatlakoztatva, itt lehet követni, illetve beavatkozni az automatizálási folyamatokba, statisztikákat lehet megnézni például a szobában lévő hőmérsékletekről. Ehhez a közp onti részhez több érzékelő kapcsolódik Bluetooth, illetve MQTT kommunikációs protokollok segítségével, amik adatokat szolgáltatnak, valamint ellátják az egyes automatizálási feladatokat. A dolgozatomban ennek a rendszernek a tervezését és megépíté sét dokum entálom le részletesen, az egyes részeket ábrákkal szemléltetve .</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>IoT, Home -automation, Raspberry Pi,  MQTT</t>
         </is>
       </c>
     </row>
@@ -504,6 +519,11 @@
           <t>A hőmérséklet mérése mindig is egy fontos szerepet játszott az ember életében, kíváncsi természete miatt. A technika és a világ fejlődése miatt mára már játszi könnyedséggel mérünk meg egy térben egy átlaghőmérsékletet, vagy akár konkrét eszközök, vagy akár emberek hőmérsékletét. Jelen dolgozatom célja egy robot megalkotása mely egy zárt térben képes a legmelegebb pont meghatározására és megközelítésére, illetve ezt egy alkalmazáson keresztül a felhasználójának is megjeleníteni egy kép formájában. Ezt a képet a robot bluetooth segítségével juttatja el a kijelzőre. Ezen keresztül a felhasználó szabadon vezérelheti is a robotot.</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>hőmérséklet mérés, bluetooth, alkalmazás, szabad vezérlés</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -526,6 +546,11 @@
           <t>A dolgozat témája az agyi tumorok osztályozása konvolúciós neuronhálókkal. A dolgozat elsőfelében a szakirodalom alapján  ismertetem a neurális hálózatokat, kezdve az egyszerű M-Pneurontól  a  konvolúciós  neuronhálókig,  kitérve  a  felépítésükre  és  tanításukra.  A  dolgozatmásodik  felében  három  általam  fejlesztett   modellt  mutatok  be,  amelyek  85%  fölöttipontossággal osztályozták  négy csoportba az agyi tumorokat. Az első megvalósított modellemegy egyszerű konvolúciós neuronháló volt. A második modellel csak mérsékelt teljesítményjavulást  értem  el  az  architektúra  megváltoztatásával  és  a  túltanulás  megakadályozásával .Mindkét  modell  esetében  hangoltam  a  hiperparamétereket.  A  legjobban  teljesítő  modell  aharmadik volt, amel y transfer  learninggel volt megvalósítva  és  a VGG16  volt felhasználvaalapmodellként. Ez a modell érte el legjobb pontosságot  (96%).  A három modell kifejlesztésesorán olyan módszereket alkalmaztam, amelyekkel javítani tudtam folyamatosan neuronhálókteljesítményét, megértve a különböző hatás  mechanizmusokat. Az általam fejlesztett modellalapját  képezheti  egy  olyan  alkalmazásnak,  ami  gyakorló  radiológusoknak  nyújt  gyorselőosztályozást, másodpercek alatt, ezzel megkönnyítve a munkájukat.</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>konvolúciós neuronhálók, agydaganat, osztályozás, keras</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -548,6 +573,11 @@
           <t>Dolgozatom  témája  a  táblajáték,  dokumentálása  és  nyomon  követése  A  munkám  során  foglalkoztam  a  játék  programozásával,  képfeldolgozással,  játék  valós  időben  való  nyomonkövetésével  a  játék  előrehaladásának  valós  idejű  dokumentálásával.  A  táblajátékok  és  a  képfeldolgozás  két  számomra  egy  izgalmas  területet  ölelnek  fel.  A  Román  Backgammon  Szövetség  különféle  hazai  és  nemzetközi  versenyeket  szervez,  ahol  a  nyomkövetés  és  az  automatikus döntőbíráskodás különösen érdekes.  A  Python  programozási  nyelv  lehetővé  teszi  a  táblajátékok  virtuális  változatának  létrehozását,  amelyek  segítségével  interaktívan  játszhatunk  a  számítógépünkön.  A  játék  programozás  során  az  volt  a  célom,  hogy  két  személy  tudjon  egymás  ellen  játszani  a  számítógépen és lehessen rögzíteni a játékot későbbi visszajátszás céljából.  Az  OpenCV  (Open  Source  Computer  Vision  Library)  egy  népszerű  könyvtár ,  amelyet  a  képfeldolgozásban  alkalmaznak.  Segítségével  a  számítógép  képes  felismerni  és  feldolgozni  a  képeket,  használatával  lehet  rögzíteni  a  játék  állapotát.  Célom  a  képfeldolgozás  terén  az  volt  hogy  egy  videóból  mentsem  ki  az  állóképeket  és  ezeken  azonosítsam  a  figurákat  vagyis  kövessem a játék egymásútani állapotát.  Tehát  a  célom  az  volt,  hogy  a  Python  és  az  OpenCV  kombinálásával  olyan  alkalmazást  csináljak,  amely  automatikusan  értékeli  a  táblajátékot.  Az  elkészítendő  szoftvernek  fel  kell  ismernie  a  figurákat,  pozícióikat,  kockadobásokat,  nyomon  kell  követnie  a  játékosok  lépéseit,  lehetővé téve két ember számára a játékot. játszanak egymás ellen a valós környezetben.</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>táblajáték, képfeldolgozás, opencv , python</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -566,6 +596,11 @@
           <t>Az érzékelők használata a mindennapjaink részévé vált, folyamatosan leh etőségünk van a minket körülvevő világban lévő fizikai, kémiai, biológiai jellemzők mérésére. Dolgozatom témája egy interaktív érzékelőrendszer megvalósítása Arduino környezetben, ami megkönnyíti az érzékelők integrálását a rendszerbe, ami kihívást jelenth et egy felhasználó számára, aki még csak ismerkedik az Arduino és a mikrovezérlők világával.  A rendszer működéséhez szükség volt egy szöveges, emberi szem által olvasható ASCII alapú általános protokoll megírására, ami segítségével az érzékelők dinamikusa n konfigurálhatóak és az adatok egységes adatformában továbbíthatóak. Az érzékelőrendszerbe több különböző szenzor is integrálva lett, melyek által különböző fizikai mennyiségek mérésére van lehetőség és az értékek változásának a nyomon követésére.  A felh asználók számára készült egy felhasználói felület, ami egy asztali alkalmazást foglal magába, amin keresztül megjeleníthetők az Arduinohoz kötött szenzorok által mért valósidejű adatok, illetve lehetőség nyílik az adatok mentésére és visszanézésére is. Az alkalmazás és mikrovezérlő között soros kommunikáció valósul meg.  Az alkalmazást laboratóriumi célokra való felhasználásra terveztem meg.</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Arduino, protokoll, érz ékelők,  asztali alkalmazás       Interactive sensor system</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -584,6 +619,11 @@
           <t>A Vezeték nélküli érzékelő hálózatok modellezése című dokumentáció célja, hogy bemutassa az útválasztó protokollok alkalmazását a hálózatok tervezésében és működtetésében. Az útválasztó protokollok kulcsfontosságú szerepet játszanak az adatcsomagok kiválasztásában és irányításában, hogy azok célba érjenek a h álózaton keresztül. Az útválasztó protokollok különböző algoritmusokon alapulnak, amelyeknek különböző jellemzői és működési elvei vannak.  A dokumentáció célja egy modell létrehozása, amely segítségével vizualizálhatjuk az útválasztó protokollok alkalmazás át, a csomagok terjedését és az adatok kiértékelését. Emellett lehetőség nyílik a különböző útválasztó protokollok teljesítményének és hatékonyságának összehasonlítására.  Az útválasztó protokollok kritikus jelentőséggel bírnak a vezeték nélküli hálózatok m űködtetésében. Az algoritmusok és azok implementációinak alapos megértése lehetővé teszi a hálózatok működésének jobb átlátását, esetleges hibák felderítését, valamint hatékony tervezést, optimalizálást és üzemeltetést. A dokumentáció segítséget nyújt a kü lönböző útválasztó protokollok működésének megértésében, előnyeinek és korlátainak feltárásában , valamint segítséget nyújt a hálózatok szimulációjának elkészítésében, mivel részletesen tárgyalja az OMNeT++ keretrendszerben íródott szimulációk kódját. Három  útválasztó protokollról olvashatunk, egy adatközpontúról (Gossiping), egy hierarchikusról (LEACH) és egy helyalapúról (GAF), ezek összehasonlításáról, k övetkeztetések levonás áról és  a vizsgált útválasztó protokollok teljesítményéről és hatékonyságáról.</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>hálózat, protokoll, útválasztás</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -604,6 +644,11 @@
       <c r="D9" t="inlineStr">
         <is>
           <t>A biológiai jelenségek jelentős része visszavezethető a genetikára. A genetika pedig a génszekvenciák alapján működik. A különféle élőlények génszekvenciájának megfejtése a biológiai tudományok nagy kihívása, amely merész becslések szerint is még ötszáz évig munkát ad a tudományos világnak.  Dolgozatom célja egy egyszerű génszekvencia osztályozó algoritmus megvalósítása és beépítése egy grafikus felhasználói felülettel rendelkező szoftverbe, amellyel talán egy apró lépést lehet tenni a génszekvenciák megfejtése felé.  A megvalósított algoritmus génszekvencia párok hasonlósági adatai alapján egy csoportosítást hajt végre egy nagyobb szekvencia adathalmazon. A módszer lehetővé teszi nagy mennyiségű proteinszekvencia egyidejű feldologozását, a szekvenciák csoportokra való osztását hasonlóság alapján. Mindez azáltal válik lehetővé, hogy a megvalósítás ritka mátrixokkal dolgozik és nem végez el fölösleges műveleteket, mint amilyenek a nullával való összeadás és szorzás. Ugyanakkor a módszernek jelentős memória hatékonysága is van, mert a ritka mátrix nem tárolja a nullás értékeket.  A megvalósított módszer gráfként kezeli a bemneti szekvencia halmazt. Minden fehérjéhez hozzárendel egy csomópontot a gráfban, és a kezdeti éleket a csomópontok között bemeneti adatként kapja meg a SCOP95 adatbázisból. Ezeket az értékeket a BLAST algoritmussal hozták létre és egy ritka mátrixot alkotnak. A megvalósított algoritmus egy bizonyos módosított Markov klaszterezés, amelyben a két fő művelet, az infláció és a kiterjesztés egymás ellenében dolgozik és a kialakuló egyensúlyi állapotban megmaradó összefüggő részgráfok határozzák meg a csoportosítás végeredményét. Az algoritmus fő paramétere az inflációs ráta, ezzel lehet szabákyozni azt, hogy az algoritmus mennyire szakítsa szét a csoportokat egymástól.   A grafikus felhasználói felület lehetőséget ad a 11944 elemű SCOP95 adathalmazon vagy annak részein végrehajtani az osztályozást különféle beállításokkal, illetve meg tudja mutatni a kialakuló fehérje csoportokat. Továbbá bármely csoportból ki tudunk választani két szekvenciát és megnézhetjük azok egymáshol illesztésének eredményét, melyet a Needleman-Wunsch algoritmussal valósít meg.  _____________________________________________________________________________    10   Az algoritmus képes lenne akár egymillió protein szekvenciát is feldolgozni néhány óra alatt, de ehhez nem állt rendelkezésemre megfelelő valós adathalmaz.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Markov klaszterezés, gráf, ritka mátrix, hatékony algoritmus, bioinformatika, fehérje szekvencia         _____________________________________________________________________________    11  Extras O proporție semnificativă a fenomenelor biologice poate fi urmărită înapoi la genetica, care se bazează pe secvențele de gen</t>
         </is>
       </c>
     </row>
@@ -616,6 +661,11 @@
           <t>A dolgozatom témája egy olyan rendszer megtervezése és kivitelezése, amely egyaránt segít az egyetemi nyílt napok szervezőinek és résztvevőinek abban, hogy az eseménysorozat lebonyolítása könnyebb és átláthatóbb legyen mindenki számára.  Az egyetemi nyílt napok egy évente megrendezett e seménysorozat, melynek célja, hogy népszerűsítse az egyetemet a középiskolás diákok körében, és betekintést engedjen az egyetem működésébe az érdeklődők számára. Ez egy rendkívül fontos folyamat, mert egy kívülálló igazán csak itt pillanthat be mélyebben a z egyetem mindennapjaiba mielőtt úgy döntene, hogy ide jelentkezik. A szervezés során több olyan teendő van, mint az eseményekkel és résztvevőkkel kapcsolatos információk menedzselése, amelyek megoldása hagyományos módszerekkel lassú és körülményes, ezért létrejön az igény egy olyan rendszerre, amely mindezt megkönnyíti.  A dolgozatom célja egy olyan rendszer elkészítése, amely az előbb említett problémákra kínál megoldást két modern keretrendszer előnyeit kihasználva. Az rendszerem megkönnyíti az eseményekk el kapcsolatos információk átadását, a jelenlévők adatainak elmentését és statisztikák készítését a meglévő adathalmazból.  Az rendszer tulajdonképpen 3 részből áll. A mobilalkalmazást a Flutter keretrendszer segítségével valósítottam meg, amelyet a felhasz nálók telefonjaira kell telepíteni és a keretrendszernek köszönhetően platformfüggetlen. Itt a felhasználóknak szerepkörüktől függően lehetőségük van regisztrálni, új eseményeket létrehozni, meglévő eseményeket módosítani, eseményekre jelentkezni, statiszt ikákat generálni. A háttérben egy Spring Boot alkalmazás fut, amely hozzáférést biztosít az adatbázisban tárolt adatokhoz és feldolgozza, valamint elmenti a mobilalkalmazás által generált adatokat. A harmadik rész pedig a Firebase által biztosított felhő a lapú tárhely, ahol a képeket tárolom, valamint a MySQL relációs adatbázis, ahol minden egyéb adatot tárolok.</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>platformfüggetlen, mobilalkalmazás, Flutter, Spring Boot, esemén</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -634,6 +684,11 @@
           <t>A dolgozat célja egy alacsony költségű, könnyen hozzáférhető digitális hangeffektus egység megvalósítása. A projekt magába foglalja a digitális jelfeldolgozási elmélet tanulmányozását, algoritmusok tervezését és fejlesztését, valamint hardveres megvalósítását. Első fázisban a tanulmányozott effektusokat Python alatt teszteltük előre mintavételezett nyers gitár hangállományokkal. Második fázisban STM32G491 mikrovezérlőt tartalmazó saját fejlesztésű multimédia rendszeren teszteltük az algoritmusokat mesterségesen előállított és hangszeren szintetizált jelek segítségével. Az effektusok minőségét mind objektív, mind szubjektív módszerekkel teszteltük.</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>digitális jelfeldolgozás, hang effektusok, ARM programozás, Python szimuláció</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -656,6 +711,11 @@
           <t>A mai diagnosztikai módszerek  az orvoslásban  folyamatosan fejlődnek, és ma már olyan technikákat alkalmaz hatunk , amelyeket korábban elképzelni sem tudtunk. Az új lehetőségek és technológiai kihívások között olyan megoldások at szeretnék találni , amelyek révén hatékonyabban tudunk felismerni és kezelni gyakori szív- és érrendszeri betegségeket, elkerülve ezáltal a korai vagy az elkerülhető elhalálozást . A kutatásom fő célja az, hogy új és fejlettebb diagnosztikai rendszereket fejlesszek ki, amelyek specifikusan a szív- és érrendszeri betegségek jellegzetességeire fókuszálnak. Ezen rendszerek segítségével pontosabb és hatékonyabb diagnózisokat lehetne elvégezni a betegségek azonosítása és kezelése során.  A módszerem alapját az orvosi elektrokardiográfia (EKG) jel einek felhasználása képezi. Ezen  jelek precíz és részletes információkat nyújtanak a szív elektromos aktivitásáról, amelyek alapján lehetséges különböző szívbetegségek jelenlétét vagy egyéb eltéréseket kimutatni.  Az első lépés a jel ek előzetes feldolgozása, a mely során szűrést és egyéb normalizáló  eljárásokat alkalmazok.  Ezután egy RGB színcsatornás képet, spektrogrammot hozok létre. A spektrogramm egy olyan vizuális reprezentáció, amely bemutatja a jelzés frekvencia -spektrumát az idő függvényében. A színcsato rnák különböző árnyalatai jelzik a frekvencia intenzitását, így könnyebbé válik a jelzés struktúrájának és változásainak vizsgálata. Ez a folyamat segít kivonni a lényeges információkat a jel ekből , és csökkenti a zajok által okozott torzításokat.  Ezek a ké pek pedig bemeneti halmazként szolgálnak a mélytanúlás alapú tanító szoftveremhez, melynek fő feladata az lesz, hogy felismerjen négy konkrét betegséget.  Tehát  a rendszer em képes  lesz felismerni  olyan mintákat , vagy apró részleteket , amelyek emberi szemmel  nem láthatóak, így pontosabb diagnózist biztosít hat az emberek számára , ami jelentősen hozzájárulhat az egészségügyi eredmények javulásához és az életminőség növekedéséhez.</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>mélytanulás,  szív- és érrendszeri betegségek ,  spektrogram, jel  szűrés, betegség diagnózi</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -678,6 +738,11 @@
           <t>Az emberek mindig is érdekeltek voltak a robotokban. Gyakran találkozhatunk robotokkal, nem csak a tudományokban, hanem az élet különböző területein is. Bár régebb úgy tekintettünk az ember -robot interakcióra, mint sci -fi (pl. R2D2 a Csillagok háborúja cí mű filmből) napjainkban ez egyre inkább valósággá vált.  Mivel az emberek természetes kommunikációja beszéden keresztül történik, nem nehéz elképzelni a beszéden keresztül történő irányítást sem. A hangvezérlés egy izgalmas téma, ami a robotok irányítását teszi lehetővé hangparancsok által. Erre különböző módszerek léteznek azonban a területen mai napig is kutatások zajlanak. Ez a tudományág nagyon sok izgalmas megvalósítást és alkalmazást hozhat magával a továbbiakban az élet minden területén (tudomány, szórakoztatás, ipar stb.).  A dolgozatom célja, hogy bemutassam a hangvezérlés előnyeit és potenciálját a mobilis robotok irányításban. Ennek érdekében egy megvalósítást fogok bemutatni, amely egy szimulációs környezetben való robot, valamint egy fizikai robo t irányítását teszi lehetővé hangparancsokkal. A továbbiakban olvashatnak a részletes megvalósításról, a felhasznált technológiákról, valamint az elvégzett mérések eredményéről, következtetésekről és továbbfejlesztési lehetőségeiről.</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>mobilis  robot, hangvezérlés</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -694,6 +759,11 @@
       <c r="D14" t="inlineStr">
         <is>
           <t>Mivel napjainkban egyre elterjedtebbé váltak a kriptovaluták, ezért az ezzel foglalkozó oldalak és alkalmazások rendkívül felkapottak lettek. Létfontosságú, hogy létezzenek olyan eszközök, platformok, amelyek lehetővé teszik a kriptovaluták kereskedését. A kripto világban ezek alkotják a decentralizált tőzsdéket. Ezek olyan platformok vagy alkalmazások, amelyek lehetővé teszik a kriptovaluták közvetlen cseréjét egymás között anélkül, hogy egy közvetítőre lenne szükség. Ezenfelül a decentralizált tőzsdék lehetőséget adnak arra, hogy likviditást szolgáltassunk a rendszerbe. Ugyanakkor lehetővé teszik a likviditás kivételét is. Ezen információk alapján a dolgozatom célja, hogy egy olyan mobil alkalmazást fejlesszek, amely lehetővé teszi a kriptovaluták cseréjét a felhasználók számára úgy Android-on, mint iOS-en. Figyelembe kell vegyük, hogy a kriptovaluták vásárlását nem tesszük lehetővé a felhasználók számára, csupán azok cseréjét.  A dolgozatom létrehozása során megkellett ismerjem azokat a technológiákat, különböző elveket és megoldásokat, amelyek lehetővé teszik egy decentralizált tőzsde működését. Ezek között voltak a különböző blokklánc technológiák, okos szerződésk, illetve a decentralizált tőzsdék főbb funkcionalitásai.</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>blokklánc, kriptovaluta, decentralizált tőzsde, okos szerződés</t>
         </is>
       </c>
     </row>
@@ -706,6 +776,7 @@
           <t>Napjainkra az informatika az egyik leggyorsabban növekvő iparággá nőtte ki magát. Gyakran hónaponta, vagy akár hetente hallunk új technológiák megjelenéséről. Ahhoz, hogy a felsőoktatási intézményekből érkező frissen végzett hallgatók megállják a helyüket egy ilyen dinamikusan növekvő környezetben, elengedhetetlen hogy tanulmányaik alatt jól elsajátítsák a programozás alapjait. Az egyik alapfogalom amelynek mélyebb megértése sok fejtörést tud okozni az e gyetemeken tanuló diákoknak, az nem más mint a rekurzió.   Ezen dolgozatnak és a hozzá társuló vizualizációs szoftvernek az a célja, hogy oktatási  segédeszközként szolgálljon mindazok számára, akik szeretnék mélyebben megérteni a rekurzió jelenségét. A fel használó számára lehetőség nyílik arra, hogy különböző rekurzív függvényeket vizualizáljon a szoftver segítségével. A szokásos vizualizációs eszközöktöl eltérően ez az alkalmazás a lépcsők módszerét használja a rekurzió mélységének vizualizációjához.   A be mutatott szoftver nem csak a tanulni vágyó diákok számára lehet hasznos, hanem mindazok számára is akik kutatni szeretnék a rekurzió jelenségét a vizualizációkon megfigyelhető érdekes mintázatok segítségével.             7  Abstract     Nowadays, IT has become  one of the fastest growing industries. We often hear about new technologies every month or even every week. For recent graduates from academic institutions to succeed in such a dynamic and  fast growing environment, it is essential that they have mastered the basics of programming during their studies. One of the basic concepts that can give university students a lot of headaches is recursion.  The aim of this paper and the accompanying visualisation software is to serve as an educational tool for those who wish to gain a deeper understanding of the phenomenon of recursion. The user is given the opportunity to visualise different recursive functions using the software. Unlike the usual visualization tools, this application uses the method of stairs to visuali ze the depth of recursion.   The presented software can be useful not only for students who want to learn, but also for all those who want to explore the phenomenon of recursion by observing interesting patterns in visualizations.             8  Tartalomjegyzék : 1.Beve zető ................................ ................................ ................................ ................................ ............  12 2.Elméleti megalapozás  ................................ ................................ ................................ .........................  12 2.1. A rekurziótörténete  ................................ ................................ ................................ .....................  13 2.2. Rekurzió a matematikában  ................................ ................................ ................................ ..........  14 2.3 Rekurzió a természetben  ................................ ................................ ................................ ..............  15 2.4 Rekurzió a programozásban  ................................ ................................ ................................ .........  16 2.5 Ciklus VS Rekurzió  ................................ ................................ ................................ .....................  17 2.6 A rekurzió oktatása  ................................ ................................ ................................ ......................  19 3.Hasonló alkalmazások és munkák  ................................ ................................ ................................ .......  20 3.1. VisuAlgo  ................................ ................................ ................................ ................................ .... 20 3.2.Sort Visualizer  ................................ ................................ ................................ .............................  21 3.3 Reku rzió kutatása a Sapientia egyetemen  ................................ ................................ .....................  23 4.Szoftver tervezése és kivitelezése  ................................ ................................ ................................ .......  25 4.1 Felhasználói követelmények  ................................ ................................ ................................ ........  25 4.2 Rendszer követelmények  ................................ ................................ ................................ .............  28 4.2.1. Funkcionális követelmények  ................................ ................................ ................................  28 4.2.2. Nem funkcionális követelmények  ................................ ................................ .........................  29 4.3 A rendszer architektúrája  ................................ ................................ ................................ .............  30 4.4 Függvény kiválasztása  ................................ ................................ ................................ .................  31 4.5 Függvény megírása  ................................ ................................ ................................ ......................  32 5. Szo ftver bemutatása  ................................ ................................ ................................ ...........................  34 5.1 Oldalak bemutatása  ................................ ................................ ................................ ......................  34 5.2 Megírt függvények vizualizálása  ................................ ................................ ................................ .. 37 5.2.1 Faktoriális függvény ................................ ................................ ................................ ..............  37 5.2.3 Egy szám páros vagy páratlan hatványa  ................................ ................................ .................  38 5.2.3 Fibonacci függvény  ................................ ................................ ................................ ...............  39 5.2.4 Hanoi tornyai függvény  ................................ ................................ ................................ .........  41 5.2.5 Ackermann függvény  ................................ ................................ ................................ ............  42 5.2.6 Hofstadter Female -Male függvény  ................................ ................................ ........................  44 6.Kihívások a fejlesztés során  ................................ ................................ ................................ ................  45 6.1 Dinamikus string tömb kompilálása  ................................ ................................ .............................  45 6.2 A vizualizációk láthatósága  ................................ ................................ ................................ ..........  48 9  7.Összefoglaló  ................................ ................................ ................................ ................................ .......  49 8.Továbbfejlesztési lehetőségek  ................................ ................................ ................................ .............  50 Irodalomjegyzék  ................................ ................................ ................................ ................................ .... 51                           10   Ábrák jegyzéke :    2.1.ábra :Fibonacci számsorozat (Forrás:[9])   2.2 ábra:  Összeadás és szorzás rekurzív képletek (Forrás:[1])  2.3 ábra : Ackermann képlete (Forrás:[ 2]) 2.4 ábra:  Arany spirál (Forrás:[ 3]) 2.5 ábra : Rekurzív brokkoli (Forrás:[ 10])  2.6. ábra : Aranymetszet a természetben (Forrás:[ 11]) 2.7 ábra : Hanoi tornyai rekurzív implementációja  2.8. ábra : Hanoi tornyai iteratív megvalósítás  2.9. ábra : Hanoi tornyai iteratív megvalósítás  3.1. ábra :VisuAlgo Fibonacci(5) értékre (Forrás:[ 5]) 3.2.ábra : QuickSort a Sort Visualizer programban (Forrás:[ 12]) 3.3.ábra : Merge Sort a Sort Visualizer programban (Forrás:[ 12]) 3.4. ábra:  Rekurzió lépcsőzetes ilusztrációja (Forrás:[ 8]) 4.1. ábra:  Use case diagramm  4.2. ábra : Activity diagramm  4.3. ábra:  Rendszer architektúra  4.4. ábra:  Szekvencia diagramm függvény választ ásnál  4.5. ábra : Szekvencia diagramm függvény írásnál  5.1. ábra:  Az alkalmazás főoldala és a választó ablak  5.2. ábra:  Főoldal részlet a létrehozott szövegdobozzal  5.3. ábra : Nézet a saját kód megírásához  5.4. ábra : Szövegdobozok generálása  11  5.5. ábra:  A kód megírásának folyamata  5.6. ábra : Faktoriális függvény  5.7.ábra : Hatványozás, indirekt rekurzió  5.8. ábra : Fibonacci függvény  5.9. ábra : Fibonacci függvény, szintek megjelölve  5.10. ábra : Hanoi tornyai  5.11.  ábra:  Ackermann függvény (2,4) értékekre  5.12. ábra : Ackermann függvény (2,20) értékre  5.13. ábra:  Ackermann függvény (3,4) értékre  5.14. ábra:  Hofstadter Female -Male függvény 7 -es értékre  5.15. ábra: Hofstadter Female -Male függvény 25 -ös értékre  6.1. ábra : Reflexióhoz szükséges osztályok  6.2. ábra : Main meghívása a dinamikusan futtatott objektumból  6.3. ábra:  Objektum létrehozása stringek segítségével  6.4. ábra : Vonal meghúzása a kezdet és a végpont közé  6.5. ábra : Közelítés a vizualizáción            12  1.Beve zető   A rekurzió egyike azon  programozásban használt  fogalmaknak, amely ek sok fejtörést okoznak a liceumokban, illetve az egyetemeken tanuló diákoknak.  A tapasztalat azt mutatja, hogy a rekurzió programkód alapú elemzését a legtöbb, programozási készségeit tekintve kezdő diák, nehézk esnek találja.   Ezen okból kifolyólag, napjainkra már nagyon sok segédeszköz elérhető számítógépes szoftverek, illetve az online térben weboldalak formájában , amelyek arra hivatottak, hogy segítsék a diákokat a rekurzió elsajátításában. Általában ezek a segédeszközök a rekurzió vizualizálásával foglalkoznak, a legtöbb esetben egy fa struktúrát hozva létre , ahol a fának a levelei a rekurzív hívásokat szemléltetik.  A fa struktúra által való vizualizációnak viszont van egy eléggé szembetűnő gyengesége. A viz ualizáció jól működik kisebb értékekre, viszont ahogy növekedik a bemeneti adatok értéke, egyre nehezebbé válik a vizualizáció értelmezése.   Ennek okán született meg az a gondolat, hogy hozzunk létre egy olyan oktatási, illetve kutatási  eszközt, amely más szemszögből közelíti meg a rekurzió vizualizálását. Az általam készített szoftver a hagyományos fa struktúra helyett, egy koordináta rendszerben ábrázolja a rekurzív függvényeket , ezáltal könnyebbé téve annak megértését, hogy a rekurzív hívások milyen mély ségeket járnak be mielőtt visszatérnek az eredeti hívó füg gvényhez.  Ezen vizualizációs módszer a bemeneti adatok növelésén kívül, lehetővé teszi különböző mintázatok ismétlődésének a megfigyelését bizonyos függvényeknél, megfelelő felületet nyújtva  ezáltal  azok számára is akik nemcsak megérteni, hanem kutatni is szeretnék a rekurzió jelenségét .  2.Elméleti megalapozás   A rekurzivítás mint fogalom, az életünk számos területén felbukkan. A rekurzió megfigyelhető például a természetben és a matematikában is. K étségtelen viszont, hogy a rekurzió fő felhasználási területe nem más mint az informatika.  Tekintsük át most röviden ezeket a területeket.  13  2.1. A rekurzió története   Amikor a rekurzióra gondolunk, valószínű, hogy első meggondolásra a modern kor számítógépei és az ezekre megírt rekurzív programkódok jutnak eszünkbe. Nem sokan gondolnák, de rekurzív definiciók már az ókori és középkori matematikában is megjelentek. Ezen definíciók egyik legismertebb példája a Fibonacci számsorozat mely et a 13. -ik században Leonardo di Pisa jegyzett fel . A Fibonaccihoz hasonló számsorozatok már az időszámításunk előtti 700 -as évektől megtalálhatók különböző egyiptomi, görög és szanszkrit iratokban  [1]. A Fibonacci számsorozat megadható az alábbi rekurzív  kapcsolattal :  2.1 ábra . Fibonacci számsorozat [ 9]  A 19. -ik század közepére megnőtt az érdeklődés a rekurzió iránt, és a függvénydefiníciók egyik módozataként kezdték használni. Ebben az időszakban például Grassman és Pierce rekurzív definíciókat adott az összeadás, illetve a szorzás műveleteknek  [1].  2.2 ábra . Összeadás és szorzás rekurzív képletek[1]  A 20. -ik sz ázad elején egy a Thoralf Albert Skolem által kiadott cikk nagy befolyással volt a rekurzió számítástechnikai elméletének fejlődésére. Ezen cikk tartalmaz egy leírást olyan függvénekről, amelyeket napjainkban primitív rekurzív függvényeknek nevezünk [1]. Skolem, illetve a későbbiekben Hilbert, Bernays és Ackermann munkássága nagyban hozzájárult a rekurzió számítástechnikai felhasználásának megs zületéséhez.  14  2.2. Rekurzió a matematikában    Amint azt már az előző alpontban is megemlítettük, a matematika volt az a tudományág, amely elsőként használta valamilyen formában a rekurzivítás fogalmát [1]. A matematikában a rekurzió egy ik klasszikus p éldája a faktoriális függvény amely kijelenti, hogy n ! = n * (n -1)!ahol n egy po zitív ternmészetes szám kell hogy legyen. Ez a rekurzív folyamat egészen addig folytatódik amíg az (n -1) egyenlő nem lesz 0 -val, ugyanis a 0 ! = 1. Ha egy programo zásban használatos kifejezést szeretnénk használni, a 0 ! az algoritmus meg állási feltételének felel meg.   A matematikában egymásba ágyazott rekurzióra is találunk példákat. Megemlíthetnénk például az Ackermann függvényt, mely a nevét a felfedezőjéről, Wilhelm Ackermannról ka pta. Az Ackermann függvény a,  teljesen kiszámítható függvények közé tartozik, viszont nem primitív rekurzív. Az idők során nagyon sok változata elterjedt, melyek közül az egyik legismertebb az Ackermann -Péter függvény, amely a következőképpen definiálható [2]:  2.3 ábra . Ackermann képlete [2]   Egy másik klasszikus példa amírő l bővebben szeretnénk beszélni ebben az alpontban, az nem más, mint a már említett Fibonacci szá msorozat. Ez a számsorozat a végtelenségig növelhető, de  vegyük most csak  az első  tíz elemét : 0, 1, 1, 2, 3, 5, 8, 13, 21, 34, 5 5.  Az n. -ik Fibonacci szám a következő rekurzív képlettel írható fel: F(n) = F(n -1) + F(n -2) ahol az n egy pozitív természetes szám, amely nagyobb mint 1. Első látásra ez a számsorozat lehet, hogy nem túlságos an érdkefeszítő, de figyeljük meg egy kicsit, hogy mi történik akkor, ha minden egyes számot elosztuk az előtte található Fibonacci számmal. Ha ezt megtesszük a következő számsorozatot kapjuk : 1/1, 2/1, 3/2, 5/3, 8/5, 13/8, 21/13, 34/21 , 55/34. Ezen os ztások eredményei : 1, 2, 1.5, 1.667, 1.625, 1.615, 1.619, 1.617. Megfi gyelhető, hogy ahogy a számok növekednek, az osztások eredményei egyre inkább közelítenek az 1,618033988749 895-ös 15  számhoz, ami nem más mint az aranymetszet. A 2.4-es ábrán az aranymetszet al apján megrazolt aranyspirál látható. Az aranymetszet, többek között a természetben is megfigyelhető. [3]    2.4 ábra.  Arany spirál [3]  2.3 Rekurzió a természetben    A rekurzivítás meglepően sok formában fellelhető a természetben. Rekurzív jellegeket figyelhetünk meg például hegyek, felhők és folyók elágazó szerkezetében, de még az állati bőr mintázataiban is.  A növényvilágban is számtalan példát találunk, amikor egy növény önmagára hasonlító mintázatokat mutat, a nagyobb forma mitha saját magának kise bb változatait hordozná magában. Természetesen a természet korlátozva van a rekurziót tekintve, ezek a kisebb formák nem zsugorodnak össze a végtelenségig [4]. Ezen növények ékes példája, az úgynevez ett Romanesco brokkoli ami a 2.5 -ös ábrán látható.   A term észetben  az önhasonló alakzatokon kívül megfigyelhető még az előző alcímben fejtegetett aranymetszet jelenléte is.  Ez a szabályosság megfigyelhető külünböző virágok szirmainak , illetve a napraforgóvirág megvainak elhelyezkedésében.  16                                  2.5 ábra  Rekurzív brokkoli [10]                             2.6. ábra  Aranymetszet a természetben [11] 2.4 Rekurzió a programozásban    Ezen alcím alatt a rekurzió fő felhasználási területéről fogunk beszélni, ami nem más mint a számítógépes programozás. A programozásban azt a folyamatot nevezzük rekurziónak, amikor egy függvény önmagát hívja meg, egy feladat megoldásának érdekében.  A rekurzió alap kérdéséül az szolgál, hogy hogyan lehet egy feladatot visszavezetni egyetlen egyszerűbb feladatra.  Ha egy aDr. Kátai Zoltán által használt hasonlattal  szeretnénk élni a rekurzív hívásokat tekintően, mondhatnánk azt is, hogy a függvény amel yből kiindul a rekurzív hívás, létre hoz egy klónt saját magáról  és a feladatának nagy részét át adja ennek a klónnak. Ez a klón ugyan azt az alapelvet követi, így létrehoz magáról egy következő klónt. Ez a folyamat nem folytatódik a végtelenségig, mivel  a függvényhívás feltételes kell legyen, ami azt jelenti, hogy van egy megállási feltétele, ami ha beteljesül, többé már nem jön létre egy következő klón , hanem vissza térítődnek az értékekek  az előző klónokhoz . Típusait tekintve a rekurziót két  különböző ré szre bonthatjuk : direkt vag y közvetlen rekurzió, illetve indirekt vagy közvetett rekurzió. Direkt rekurziónak nevezzük azt amikor egy függvény saját magára hivatkozik amikor függvényhívást végez. Indirekt rekurziónak azt nevezzük amikor egy rekurzív függvé ny nem saját magát hívja meg, hanem egy másik függvényt, amely szintén nem önmagát hívja meg, hanem azt a fügvényt aki őt meghívta.   17  2.5 Ciklus VS Rekurzió    A rekurzió ellenpárja az iteratív ciklusos megoldás.  Annak ellenére, hogy ellenpároknak hívjuk őket , a rekurz ív függvényeket ciklussá lehet alakítani és ugyan így az iteratív ciklusokat rekurzióvá. Elmondható, hogy az iteráció  gyorsabb a rekurziónál, mivel a rekurzió esetében függvényhívás történik, ami meg növeli a futási időt. A rekurziónak eg y másik hátránya az, hogyha a rekurzió túl nagy mélységeket jár be, akkor feltelhet a verem.   De miért éri meg akkor rekurziót használni ? A rekurzi ó ereje nem a gyorsaságában, hanem az eleganciájában rejlik. Sok esetbe n a rekurzióval megoldott feladat tömörebb és jobban olvasható mint az iterációs ellenpárja. Ennek egyik ékes példája a Hanoi tornyai nevű feladvány. A Hanoi tornyai rekurzív implementálása nagyon rövid és elegáns . Lásd 2.7  ábra.    2.7 ábra . Hanoi tornyai rekurzív implementációja  Ezzel ellentétben, Hanoi tornyai iteratív implementálása még sok informatika tanárt is gondolkodóba ejtene. Fi gyeljük meg egy kicsit a 2.8 -as és 2.9 -es ábrán ezt a megvalósítást is, a fentiekben látott bemeneti értékekre.  Ezeken  az ábrákon megfigyelhető, hogy Hanoi tornyai iteratív megvalósítása több mint tizszer annyi kódolást igényel mint a rekurzív megvalósítás . 18   2.8. ábra  Hanoi t ornyai iteratív megvalósítás    2.9. ábra Hanoi t ornyai iteratív megvalósítás   Ezen két megvalósításból  láthatjuk, hogy a a re kurziót igenis megéri használni, mert a példaként említett Hanoi tornyai probléma rekurzív megvalósítása sokkal  érthetőbb,  rövidebb  és elegánsabb mint az iterációval megírt ellenpárja . 19  2.6 A rekurzió oktatása    A reku rzív programozás egyike azon témáknak, amelynek tanítása során az oktatók előszeretettel nyúlnak bizonyos oktatási segédeszközökhöz. A legtöbb ilyen segédeszköz  a látást célozza meg mint felhasználandó érzéket, mivel felismerték, hogy a látás fontos szerep et játszik az új fogalmak elsajátításában. Ezen felismerés különböző kutatási vonalakat nyitott meg a rekurzió oktatását tekintve, mint például a rekurzió vizuális analógiái, vagy a programok eredményének animálása [13].   Az analógiákat tekintve az oktatók és kutatók túlnyomó többsége ugyan azokkal a példákkal áll elő, ilyen például a rekurzív mintázatokat mutató brokkoli, a fák ágai, illetve az egymással szembe helyezett tükrök tükröződései.  A kutatások során nem csak tárgyakat, hanem külöböző rekurzív foly amatokat is megvizsgáltak mindennapi példák segítségével. Megvizsgálták például azt, hogy hogyan értelmezik a gyerekek az egymás mellé helyezett dominók eldőlését [13].  A 12 év körüli és idősebb gyerekek esetében a dominók eldőlésének leírásában megfigyelh ető a rekurzív gondolkodás, mivel a gyerekek megfigyelték, hogy minden dominóelem eldőlését az előtte levő dominó okozta. Ezzel ellentétben, a 12 évnél fiatalabb gyerekek esetében a leírás inkább iteratív jellegű, eldől egy dominó, majd a következő, egésze n ameddig egy se marad állva[13].   A rekurzi ót kutató személyek  számos javaslatot tettek a rekurziós gráfok használatára, annak érdekében, hogy gyorsítani lehessen ezáltal a kezdőknél a rekurzió elsajátításának a folyamatát. Ezen gráfok lehetővé teszik a d iákok számára a függvényhívások kiértékelésének a követését  és mélyebb elemzését . Ha ezen gráf egy bináris fa, akkor minden egyes csomópont ugyan azt a függvényhívást jelenti [13].     20  3.Hasonló alkalmazások  és munkák    3.1. VisuAlgo     A “VisuAlgo” egy interneten el érhető weboldal, amely animációk segítségével próbál vizualizálni különböző adatstruktúrákat és algoritmusokat .[5] Az oldal segítségével többek között képesek vagyunk vizualizálni rendezéseket, láncolt listákat, hasító táblákat, és nem utolsó sorban, a rekurziót .   3.1 ábra  VisuAlgo Fibonacci(5) értékre [5]  A „VisuAlgo” a rekurziót egy fa struktúra segítségév el vizualizálja, ahogy ezt a 3.1 -es ábra is mutatja.  Az oldal bal alsó sarkában található egy mező, amely segítségével ki tudjuk választani, hogy mit i s szeretnénk vizualizálni. A 3.1 -es ábrán például a Fibonacci számok vizualizációja van kiválasztva n =5 értékre. A Fibonacci számokon kívül további 19 függvé ny vizualizációjára ad lehetőseget a program, amelyeknek forráskódját ki is vetíti egy szövegdobozba. Lehetőség van saját kód kipróbálására is, ugyanis a lenyíló listában az utoló elem a „Custom code” nevet viseli, ha ezt kiválasztjuk, akkor megírhatjuk a szövegdobozban a saját kódunkat JavaScript programozási nyelv segítségével.   21   Ahogy a 3.1 -es ábra jobb oldalán is megfigyelhető , a fa struktúra levelei különböző színeket  vesznek fel. A legalsó szinteken található levelek a zöld színt veszik fel, ezek a le velek azokat a rekurzív hívásokat jelölik, amikor a megállási feltétel igaznak bizonyul és elkezdődik az értékek visszatérítése.  A levelek fehér színűek amikor egy hívás az adott n értékre először történt meg.  A program világoskék színnel jelöli azokat a h ívásokat amikor  az n bemeneti értékre a hívás egyszer már feldolgozásra került [5]. Vegyük például az ábra alapján a Fibonacci(2) – es értéket. Mivel a bináris fa balról jobbra kerül bejárásra, a fa leginkább baloldalán található kettes értékű levél fehér színnel van jelölve, míg az utána következő összes többi kettes értékű levél kék színnel lett jelölve.   Következtetésként kijelenthető, hogy a “VisuAlgo” hasznos  segédeszköznek bizonyu l a rekurzió vizualizálását illetően, és mint diákok, mint tanárok hasznát vehetik akik többet szeretnének tudni a rekurzióról.   3.2.Sort Visualizer    A “Sort Visualizer” szintén egy interneten elérhető weboldal, amely rendezési algoritmusok vizualiz álására specializálódott. A 16 darab vizualizálható a lgoritmus közül van néhány amely előszeretettel alkalmazza a rekurziót. Ilyen algoritmus például a quicksort, illetve a merge sort. Ezen alpont keretén belül szeretnénk bemutatni ezeknek a vizualizációját a program segítségével.   A quicksort vagy g yorsrendezés a divide et imp era elv alapján működik. A rendezendő listát egy pivot segítségével két különálló részre bontja, majd erre a két új listára külön külön ismét meghívja a gyorsrendezést. [6] Ez a rekurzív folyamat addig folytatódik, amíg az átadott lista hossza kisebb vagy e gyenlő nem lesz 1 -el. Nezzük meg hogyan is vizualizálja ezt a rendezést a program. Lásd 3.2  ábra.     22   3.2 ábra . QuickSort  a Sort Visualizer  programban  [12]  Első lépéskent a rendező algoritmus végig iterál a listán, és elkezdi kicserélni a kiválasztott pivot elem két oldalán levő értékeket. Azokat az elemeket amelyek kisebbek mint a pivot a bal oldalára rendezi, míg azokat amelyek nagyobbak a jobb oldalára. Ez után következik az algoritmus rekurzív része , amit az előbbiekben már ismertettünk. Megfigyelhe tő hogy a lista legeleje kerül leghamarabb rendezésre, ez annak köszönhető, hogy az oszd meg és uralkodj módszert használó algoritmus, először a pivot bal oldalán levő listára hívja meg rekurzívan a quicksortot.   A következőkben figyeljük meg egy kicsit, h ogyan figyelhető meg a rekurzió a merge sort esetében.  Lásd 3.3  ábra.   3.3 ábra . Merge Sort a  Sort Visualizer  programban  [12] 23    A merge sort a quicksorthoz hasonlóan az oszd meg és uralkodj módszert alkalmazza. A rendező algoritmus rekurzívan felosztja a bemeneti listát, egészen ameddig az átadott lista csupán egyetlen elemet tartalmaz. Amint ez megtörténik, a részsorozatok összevonódnak és rendezésre kerülnek. Az algoritmus fokozatosan összevonja a részlistákat, egészen addig amíg egyetlen rendezett lista  marad a végén.[7]  Az összevonás folyamata a 3.3 -as ábrán is nagyon jól megfigyelhető.   Összességében kijelethető, hogy a “Sort Visualizer” is sokat tud segíteni egy felhasználónak a rekurzió megértésében.      3.3 Rekurzió kutatása a Sapientia egyetemen     A Sapientia Erdélyi Magyar Tudományegyetem Marosvásárhelyi karán a 2008 -as évben Dr. Kátai Zoltán vezetésével elvégzésre került egy kutatás, amelynek keretén belül egy úgynevezett többérzékelős módszert probáltak ki a rekurzió oktatására.  Ezen alpontban bemutatásra kerül ez a kutatás, amely a [8] –as cikkben található, és az ehhez fejlesztett szoftver is bemutatásra kerül.   A kutatás egyik részeként megkértek az egyetem diákjai közül néhányat, hogy játszák el egy rekurzív függvény futási f olyamatát. Az első diák szemléltette a main függvényt, míg a többiek  a rekurzív függvény példányait szemléltették. Amikor egy a cikk által rekurzív szereplőnek megnevezett diák meghívásra került, a szereplő kilépett a meghívója mögül és elkezdte elemezni az általa kapott feladatot. Két lehetősége volt, követi a rekurzív forgatókönyvet, vagy követi a triviálisat , ami a megállási feltétel teljesülését jelentette. Ha az első lehetőséget választotta, akkor meghívta a társát  és saját magát felfüggesztette amíg nem kapott választ a hívásra. A legutolsó diáknak a triviális forgatókönyvet kellett választania, mivel akkor teljesült a megállási feltétel. Neki az volt a dolga, hogy a részfeladatának az eredményét átadja a hívójának, aki ennek hatására felébredt a felf üggesztett állapotából és ugyan ezt a 24  műveletet elvégezte.  Ez a folyamat addig folytatódott amí a main függvényt szemléltető diák megkapta az eredményt [8].   Ezen kísérlet segített a diákoknak jobban megérteni, hogy hogyan is működik a rekurzió.  A néző diá kok megérthették belőle a rekurzív folyamatok működését, míg azok a diákok aki eljátszodták folyamatokat, kinetikus módon is memorizálták a rekurziót, a műveletekhez kapcsolódó mozgások által  [8].  A kutatás egy másik fontos része , egy a rekurzió oktatására  kifejlesztett szoftver kipróbálása volt.  Ezen szoftver audio -vizuális eszközökkel próbálja megértetni a felhasználóval a rekurzivítást. A rekurziót a program lépcsőzetesen vizualizálja, ezáltal minden egyes rekurzív hívás egy úgynevezett emelete t hoz létr e . Lásd 3.4 -es ábra. Minden egyes emeleten a vizualizációhoz egy zenei bejátszás is társul, melynek hangmagassága az emelet magasságának függvényében növekszik.   3.4 ábra.  Rekurzió lépcsőzetes ilusztrációja  [8]  A kísérletben 43 nagyjából azonos képességekkel rendelkező  első éves  diák vett részt . A diákokat két csoportra osztották, 23 -at közűlük a tradicionális módszerekkel tanítottak, míg a megmaradt 20 diáknál az előbbiekben említett módszereket használták a rekurzió oktatására. Az utólag os teszt eredmények azt mutatták, hogy akiket a többérzékelős módszerekkel tanítottak, jobban teljesítettek mint azok a társaik akik tradicionális oktatásban részesültek. [8] Ezen kísérlet ékes példája annak, hogy a különböző segédeszközök könnyebbé tudják tenni a rekurzió megértését és tanulását.  25  4.Szoftver tervezése és kivitelezése    A dolgozat ezen részében bemutatásra kerül a szoftver, amelyet a rekurzió lépcsőzetes módszerrel való vizualizálásához fejlesztettem. Az alkalmazás  egy Windows Form aplikáció amely  C# programozási nyelven íródott és a .Net keretrendszer 4.7.2 - es verzióját használja.  A szoftver lehetőséget ad rekurzív függvények illetve rekurzív eljárások vizualizációjára.  A különbség a két fogalom között az, hogy míg a rekurzív függvény vissza  térít egy eredményt a hívójához, addig a rekurzív eljárás csupán elvégez egy feladatot anélkül, hogy bármit is vissza térítene a hívójához. Természetesen a rekurzív eljárásokban is jelen van a megállási feltétel [14].  4.1 Felhasználói követelmények    Az szoftver  elindítása  után, a felhasználó előtt egyenesen az alkalmazás fő ablaka jelenik meg. Ezen a fő ablakon történik meg a rekurzív függvények vizualizálása egy koordináta rendszerben. Az elindítás pillanatában a fő ablakon három gomb jelenik meg, a “Choose File”, “Run”, illetve a “Write own c ode” elneve zésekkel.   A “Choose File”  gomb lenyomásávál egy különálló ablakban megnyílik  a projektnek a könyvtára, ahol a felhasználó ki tudja választani az előre megírt rekurzív jellegű függvények közül azt amelyiket vizualizálni szeretné. Minden egyes függvény különálló .txt kiterjesztésű fájlokban van megírva, a felhasználónak csak annyi a  feladata, hogy kiválassza a fájlt és megnyomja az „Open” gombot.  Miután ki lett választva a függvény, a szoftver átvizsgálja a kapott függvényt és megállapítja, hogy hány paraméter megadására van szüksége az adott függvénynek. Annak fügvényében, hogy ez a  szám mennyi, a szoftver kigenerálja azokat a szövegdobozokat ahova a felhasználó be tudja írni az értékeket. Például, ha kiválasztottuk a faktoriális függvényt, aminek meghívásához egyetlen paraméterre van szükség, a program egyetlen szövegdobozt fog létr ehozni ahova be tudjuk írni ezt az értéket.   A “Run” gomb lenyomásával tudjuk elindítani az előző lépésben kiválasztott függvény vizualizációját. Ha sikeres volt a program lefuttatása, akkor az ablak gombok alatti üres részében megjelenik a függvény vizual izációja. Abban ez esetben ha nem választottunk még ki egyetlen 26  függvényt sem amit vizualizálni szeretnénk és megnyomjuk a “Run” gombot, a szoftver egy üzenetet közvetít a felhasználó felé, hogy előbb válasszon ki egy függvényt és csak azután nyomja meg a “Run” gombot. Hasonl ó figyelmeztetést kapunk abban az esetben  is ha a kigenerált szövegdobozokba egy érvénytelen karaktert ütünk be. Minden beütött érték szám kell hogy legyen, ennek értelmében ha egy betüt adunk meg paraméterként, a szoftver figyelmeztet,  hogy a megadott paraméter nem érvényes.   4.1 ábra.  Use case diagramm   27   A “Write own c ode” gomb megny omásával egy új ablak fog megnyílni a felhasználó előtt. Ebben az új ablakban lehetőség nyílik arra, hogy a felhasználó egy saját maga által szerkesztett kódot is levizualizáljon. Az ablak megnyitásakor még nincs kigenerálva az a szövegdoboz , ahova a felhasználó beírhatja a saját C # nyelven megírt kódját, viszont az ablak legtetején talál két gombot, név szerint a “Direct Recursion” és az “Indirect Recursio n” gombokat. Ezek a gombok azért szükségesek, hogy a felhasználó ki tudja választani a kívánt rekuzió típusát. Ha a felhasználó a “Direct Recursion” gombot n yomja meg akkor egyetlen szövegdoboz kerül kigenerálásra, mivel a közvetlen rekurzióhoz csak egyetl en megírt függvényre van szükség. Ha az “Indirekt Recursion” gombot nyomja meg a felhasz náló, két szövegdoboz generálódik ki, mivel a közvetett rekurzióhoz legalább két függvényre van szükség. Az előzőekben feldolgozott fájl kiválasztásos módszernél azért nem volt szükség hasonló műveletre, mivel a szoftver a beolvasott szöveges fájl alapján el tudja dönteni a rekurzió típusát.   4.2 ábra . Activity diagramm  28   Miután ki lett generálva a megfelelő számú szövegdoboz a függvények beírásához, a felhasználó neki kezdhet kódolni. A szövegdoboz első sorába a felhasz náló az úgynevezett “method signaturet” kell hogy beírja, amely tartalmazza a függvény nevét, típusát, és  a függvény paramétereit. Miután az első sor be lett írva, enter gomb lenyomására a program meghatározza, hogy hány paramétere van a megírt metódusnak, amely után kigenerálja a megfelelő mennyiségű szövegdobozt a paraméterek értékeinek megadására. Abban ez  esetben ha hibát vétettünk ezen műveletek közben, például nem adtunk meg megfelelő mennyiségű paramétert az első sorban, de már kigeneráltuk a paraméterek szövegdobozait, nyomjuk meg a “Clear all” elnevezésű gombot, mely vissza állít mindent az eredeti ál lapotára.Ezután előlről kezdhetjük az előbbiekben vázolt műveleteket. A füg</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -724,6 +795,11 @@
           <t>A dolgozat témája  egy webalkalmazás  fejlesztése , amely a hallgatókat, a cégeket és az egyetemeket a szakmai gyakorlat tevékenysége során köti össze . A cél az, hogy egy könnyen használható, felhasználóbarát platformot fejlesszek, amely képes a szakmai gyakorlatokkal kapcsolatos teljes folyamat lebonyolí tására.   A projekt egyik célja, hogy a hallgatók és a cégek számára egy szakmai  közösségi platformként működjön az alkalmazás, ezáltal elősegítve a szakmai kapcsolatok kialakulását, valamint a cégek és az egyetemek közötti partneri kapcsolatok ápolását.   A projekt másik fontos célja, hogy a platformon a hallgatók a saját profiljuknak és szakjuknak megfelelően kapjanak ajánlásokat. Ez lehetővé teszi számukra, hogy releváns lehetőségeket találjanak a szakmai gyakorlatok terén. Az ajánlórendszerem  algoritmusa i, például a Cosinus hasonlóságot felhasználva figyelembe veszik a hallgatók készségeit, érdeklődését és a cégek által meghatározott követelményeket. Így a platform segít a hallgatóknak a legmegfelelőbb gyakorlati helyek megtalálásában, optimalizálva ezzel  a kapcsolódó folyamatokat és eredményessé téve a gyakorlatokat.   A projekt elkészítéséhez modern webes technológiákat használok, Angular -t, Java Spring Bootot, PostgreSQL -t és AWS -t. Ezek segítenek a platformomat robusztussá, skálázhatóvá biztonságossá és  gyorssá tenni.</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Internship, Ajánlórendszer, Cosinus hasonlóság, Angular, Spring Boot       WEB APPLICATION FOR MANAGING INTERNSHIP AND TRAINEESHIP ACTIVITIES</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -742,6 +818,11 @@
           <t>A biztonsági rendszerek az emberek, vállalkozások és intézmények számára egyarántfontosak a biztonságos környezet fenntartásához és az anyagi javak megóvásához. A maimodern technológia erre változatos megoldásokat nyújt. Minden ilyen rendszernek fcélja kiszrni az illetéktelen behatolókat a belép joggal rendelkez emberek közül. Abeléptet rendszerek erre egy hatékony valós idej megoldást kínálnak. Az épületekbevaló bejutást csak azoknak a személyeknek teszik lehetvé, akik megfelel engedéllyelrendelkeznek, tehát hitelesíteni tudják magukat.A diplomamunkám témájának egy biometrikus beléptet rendszer megvalósításátválasztottam, ami arcfelismerés segítségével azonosítja az embereket. Célom volt egykönnyen kezelhet, gyors, hatékony és els sorban biztonságos rendszer megvalósításaegy költséghatékony módon, ezzel megkönnyítve az emberek mindennapjait, illetve le-egyszersítve az épületekbe belépni vágyó személyek azonosításását.A nagymérték biztonság érdekében a biometrikus azonosítási módszerek közül azarcfelismerést választottam, ez egy széleskörben ismert és használt technológia, gyakranhasználják biztonságos számítógépes rendszerekhez, laptopokhoz, okostelefonokhoz vagybankautomatákhoz. Az elnyei mellett megemlíthet, hogy nem igényel közvetlen ﬁzikaiérintést az azonosítás során, illetve gyors és hatékony módszer.Más hasonló azonosításhoz viszonyítva biztonságosabb, illetve nehezebben átjátszha-tóbb egy arcfelismerésen alapuló rendszer. A jelszavak és PIN kódok könnyen kitudódhat-nak, feltörhetek, a különböz kártyák és kulcsok pedig elveszíthetek vagy ellophatóak,így illetéktelen kezekbe kerülve visszaélés történhet a biztonsági intézkedésekkel szemben.Ezeket a szempontokat szemeltt tartva terveztem meg a rendszer mködését. Abelépéshez feltétel hogy az adminisztrátor hozzáadja a személyek adatait és képeit. Enneka feltételnek a beteljesülésével belépésre jogsult az épületbe. A felhasználó egyszerencsak a kamera elé áll, megfelel ható távolságban és ha megtalálható a rendszerben, akkorkinyílik az ajtó és beléphet. A könny használat érdekében létrehoztam egy felhasználóifelületet is, amelynek segítségével egyszeren hozzá lehet adni a személyeket, illetve akövethetség érdekében megtekinthet az épületbe belép személyek listája is, pontosbelépési idvel együtt.Az általam megvalósított rendszer megkönnyíti a belépés során az azonosítás folya-matát, és egy biztonságos megoldást nyújt az illetéktelen személyek kiszrésére a min-dennapokban</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>arcfelismerés, azonosítás, biometria, beléptet rendszer, biztonság</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -760,6 +841,11 @@
           <t>A dolgozat célja egy web alkalmazás, amely digitalizálja a diploma témák választását.Szükség volt egy megoldásra, ami segítene és megkönnyítene hallgatók munkáját a dip-loma témával kapcsolatos teendknél.Célkitzések közé tartozott egy olyan web applikáció lefejlesztése, amely képes nagy-számú adatot és felhasználót kezelni és könnyedén használható bárki számára. Az adottapplikáció feleljen meg minden egyetemi elvárásnak és kérés esetén tovább fejleszthetlegyen. Legyen biztonságos és biztosítva legyen, hogy az applikáció karbantartható.Sikerült megvalósítani a célkitzéseket minden terén. Egy olyan web applikáció szü-letett, amelyet azoak a személyek használhatnak akik részt vesznek a diploma dolgozatokmeghirdetésében és hallgatókhoz való hozzárendelésében. A tanszéki titkárok és munka-folyamatot hozhatnak létre és meghívhatják a tanárokat és a hallgatókat a rendszerbe. Atanárok feltölthetik a diploma témáikat és a hallgatók jelentkezhetnek azokra. Vendégekpedig megtekinthetik az elkészített diploma témákat.A fejlesztéshez használtam az Angular és Spring Boot keretrendszereket, melyekneksegítségével egy skálázható és biztonságos web applikációt lett fejlesztve. Az adatoktárolásához a PostgreSQL adatbázis használva és a karbantarthatóság érdekében tesztelkeretrendszereket és applikációkat, a Cypress-t és Postman-t.AbstractThe aim of the thesis is to design and develop a web application that digitises thechoice of subjects for the diploma. A solution was needed that would help and facilitatethe work of the university committee and students in the diploma topic selection process.Our objectives included the development of a web application that could handle alarge number of data and users and could be easily used by anyone. The applicationshould meet all university requirements and could be further developed on request. Besecure and ensure that the application is maintainable.The objectives have been achieved in all areas. A web application has been developedthat secretaries can log into and create periods and invite teachers and students to thesystem. Teachers can upload their degree topics and students can apply for them. Andguests can view the diploma topics they have created.A wide range of technologies have been used in the development. Most prominent arethe frontend and backend frameworks. Using Angular and Spring to boot I was able todevelop a highly scalable and secure web application. Using PostgreSQL database to storedata and testing frameworks and applications Cypress and Postman for maintainability.TartalomjegyzékÁbrák jegyzéke 3Táblázatok jegyzéke 41. Bevezet 52. Elméleti megalapozás és szakirodalmi tanulmány 72.1. Szakirodalmi tanulmány ........................... 72.2. Elméleti alapok ................................ 82.2.1. Hatékony eszközök a webalkalmazások fejlesztéséhez ........ 82.3. Ismert hasonló alkalmazások ......................... 82.4. Felhasznált technológiák ........................... 92.4.1. Angular frontend keretrendszer ................... 92.4.2. Spring boot backend keretrendszer ................. 102.4.3. Szervletek ............................... 132.4.4. Postgres és annak kezelése ...................... 142.4.5. Liquibase ............................... 152.4.6. Tesztelést elsegít frameworkok ................... 152.4.7. Verzió követ és feladat vezérl alkalmazások ............ 163. A rendszer speciﬁkációi és architektúrája 173.1. Követelmény speciﬁkációk .......................... 173.1.1. Funkcionális követelmények ..................... 173.1.2. Nem funkcionális követelmények ................... 213.2. Adatbázis ................................... 223.3. Alkalmazás architektúra ........................... 244. Részletes tervezés 304.1. Tervezési fázisok ............................... 304.1.1. Frontend ................................ 304.1.2. Backend ................................ 424.2. Tesztelés .................................... 484.2.1. Frontend tesztelés ........................... 484.2.2. Backend tesztelés ........................... 504.2.3. Éles tesztelés ............................. 5115. Üzembe helyezési lépések 525.1. Felmerült problémák és megoldásaik .................... 525.1.1. Idszakok beintegrálása az applikációba ............... 525.1.2. Hallgatók leosztása automatikusan ................. 536. Következtetések 546.1. Megvalósítások ................................ 546.2. Továbbfejlesztési lehetségek ......................... 54Irodalomjegyzék 56Függelék 57F.1. Kód részletek ................................. 572Ábrák jegyzéke2.1. Különbség egy MPA (Multiple Page Application) és egy SPA (Single PageApplication) között [ 8]............................ 92.2. Angular applikáció elemi felépítése [ 1].................... 102.3. Mikroszolgáltatások felépítése [ 5]...................... 112.4. Rétegelt architektúra megvalósítása Spring bootban. ............ 122.5. ORM mködése[ 4].............................. 143.1. Adatbázis diagram .............................. 243.2. Alkalmazás architektúra [ 3]......................... 254.1. Frontend oldali typescript osztály ...................... 374.2. Szerver oldali java osztály .......................... 374.3. Cypress tesztelés ............................... 504.4. Postman tesztelés ............................... 504.5. Diploma téma jelentkezés hallgató szemszögébl .............. 514.6. Diploma téma leosztás eredményei ...................... 513Táblázatok jegyzéke3.1. Bejelentkezési funkció ............................. 193.2. Hallgatók feltöltése funkció .......................... 203.3. Diplomamunka létrehozása funkció ..................... 203.4. Véglegesíteni a leosztott eredményeket a saját szakukról funkció. ..... 203.5. Diplomamunkára jelentkezni funkció. .................... 213.6. Keresni az elvégzett diplomamunkák között név és</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>alapjánfunkció. .................................... 2141. fejezetBevezetA mostani elrehaladott korban nagy mértékben kiegészíti életünket a digitális vilá</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -778,6 +864,11 @@
           <t>A dolgozat célja a mellkasi röntgenfelvételek osztályozása tüdőgyulladás jelenléténekdetektálására. A kutatásban egy konvolúciós neurális hálózatot alkalmaztunk a pon-tosabb osztályozás elérése érdekében. Célunk az volt, hogy fejlesszünk egy hatékonyosztályozót, amely egy saját modell által létrehozott neurális háló, vagy egy GoogleNetarchitektúrájú neuronháló, amelyet “transfer learning” technikával saját célokra edzet-tünk fel.A kutatási módszerünk a meglévő megoldások tanulmányozásán, saját kísérletekenés adatgyűjtésen alapult. A “transfer learning” technikát alkalmaztuk a GoogleNet ar-chitektúrára, ami egy előzetesen tréningezett nagy modell, ezáltal javítva az osztályozáspontosságát. Az adatgyűjtés során tüdőgyulladással és tünetmentes esetekkel rendelkezőmellkasi röntgenfelvételeket használtunk.Az eredmények alapján sikerült fejlesztenünk egy grafikus felhasználói felületet, amelylehetővé teszi a mellkasröntgen automatikus osztályozását és a tüdőgyulladás diagnózisát.A GoogleNet architektúrájú neuronháló kiemelkedő pontosságot ért el a tesztelt adathal-mazon, és összehasonlítva a saját osztályozó hálóval, szignifikánsan jobb eredményeketprodukált, hasonlóan a szakirodalomból tanulmányozott háló eredményeihez.Ezen eredmények alapján arra a következtetésre jutottunk, hogy a jól megírt, aGoogleNet architektúrával együttműködő neurális háló hatékonyan képes detektál-ni a tüdőgyulladást a mellkasi röntgenfelvételek alapján. Ez a kutatás hozzájárulhataz orvosi diagnosztika fejlesztéséhez, segítve a korai felismerést és a hatékonyabb kezelést.</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>mellkasi röntgenfelvétel, osztályozás, konvolúciós neurális hálózat,transfer learning, GoogleNet architektúra</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -800,6 +891,11 @@
           <t>Az ember életében az egyik legértékesebb és legfontosabb dolog az idő. A mai rohanó világban annyira felgyorsultak az események, hogy valódi nehézséget jelent kézben tartani őket és jól menedzselni az időnket. Az időmegtakarítás céljából számos okos készül ék és rendszer jelent meg, megkönnyítve az emberek életét. Akár úgy is fogalmazhatunk, hogy az okos rendszerek korát éljük.  A dolgozatom témája is egy ilyen rendszert foglal magába. Nemcsak időt spórol a felhasználóknak, hanem egy felelősségtől is megszaba dítja őket. Ez a modern és innovatív megoldás lehetővé teszi, hogy gondoskodjunk növényeinkről a legmegfelelőbb módon, miközben minimalizáljuk a gondozási feladatokat és maximalizáljuk a virágok egészségét és szépségét. Segít, hogy a növények optimális áll apotát fenntartsuk, különösen akkor, amikor távol vagyunk otthonunktól vagy nem tudunk elég időt fordítani a gondozásra. Az érzékelők figyelik a környezeti paramétereket, azaz a hőmérsékletet és nedvességtartalmat. Az okos virágtartó rendszer automatikusan  szabályozza az öntözést és világítást, biztosítva a növények számára a megfelelő mennyiségű vizet és hőmérsékletet a megfelelő időben. Nem kell többé aggódnunk a túl vagy alulöntözés miatt, hiszen a rendszer precízen és pontosan gondoskodik a virágaink ví zellátásáról.  A felhasználói felület segítségével könnyedén beállíthatjuk az öntözési ütemtervet, profilokat hozhatunk létre, nyomon követhetjük a növények állapotát és a környezeti paramétereket. Akár otthon vagyunk, akár távol, a rendszer távoli elérést biztosít, hogy mindig kapcsolatban maradhassunk a növényeinkkel és szükség esetén beavatkozhassunk.  A rendszer vezérléséhez az ESP32 mikrovezérlőt használtam, ami egy rendkívül sokoldalú és erőteljes platform és feladata a rendszer teljes körű vezérlése és  felügyelete.</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>felhasználói felület, okos rendszer, mikrovezérlő</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -818,6 +914,11 @@
           <t>Az ipari robotok egyre inkább elterjednek a különböző gyártási és logisztikai folyamatokban, ahol a pontosság, a sebesség és a biztonság fontos szempontok. A robotok képesek automatizálni olyan feladatokat, amelyek unalmasak, veszélyesek vagy túl bonyolultak az emberek számára. Azonban a robotok és az emberek közötti együttműködés még mindig kihívást jelent, különösen akkor, ha a robotnak rugalmasan kell alkalmazkodniuk a változó környezethez és feladatokhoz.   Téglatest alakú tárgyak felismerése és mozgatása olyan feladat, amelyet számos ipari és oktatási célra használnak. A tárgyak típusának és elhelyezkedésének meghatározása azonban nem mindig egyszerű, különösen akkor, ha azok színükben vagy méretükben hasonlítanak egymásra. Ebben a dolgozatban egy olyan módszert mutatok be, amely a Baxter robot az ArUco kódok segítségével könnyeden megkülönbözteti a kockákat. Leírom, hogyan programoztam a Baxter robotot, hogy képes legyen meghatározni egy munkafelületen lévő tárgyak típusát és helyzetét, valamint rendezni azokat. A tanulmányom során részletesen bemutatom a rendszer tervezését, megvalósítását és tesztelését.  A dolgozatomban egy olyan rendszert fejlesztettem ki, amely képes a Baxter robotot vezérelni úgy, hogy képes legyen téglatest alakú tárgyakat felismerni és mozgatni. A rendszer három fő komponensből áll: egy képfeldolgozó modulból, amely az opencv valamit a cv2.aruco könyvtárak segítségével érzékelik és azonosítják a tárgyakat, egy kommunikációs modulból, amely ZMQ (ZeroMQ) protokollt használva küldi és fogadja az adatokat, és egy robotvezérlő modulból, amely ROS (Robot Operating System) könyvtárakat használva irányítja a robot karjait és megfogóit. A rendszer működése során a robot fényképet csinál a munkaterületről, meghatározza a tárgyak helyzetét és típusát, majd ezek alapján elvégzi a szétválogatást.</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Baxter, ROS, ArUco, Opencv, Python, képfeldolgozás, ipari es oktatási robotika</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -836,6 +937,11 @@
           <t>Napjainkban  minden  ember  rendelkezik  okostelefonnal,  amelyek  segítségével  rengeteg problémát megoldhat különböző alkalmazásokkal. Ilyen hasznos alkalmazások például a számláink kifizetésére szolgáló alkalmazások, de akár feladataink vezetésére is rengeteg alkalmazást találunk.  A  telefonos  alkalmazások  nem  csak  a  mindennapjainkat  könnyítik  meg,  hanem  akár  a tanügyi intézményekben is segítségünkre lehetnek. A legtöbb telefonos alkalmazás, amit előszeretettel használnak az iskolákban és az egyetemeken: a különböző számológépek, fordítók és a jegyzetelésre szolgáló alkalmazások.   Viszont a PowerPoint bemutatására szolgáló alkalmazások az emberek körében nincsenek elterjedve, ezért a számuk igen kevés és nem a legjobban karbantartottak vagy nem rendelkeznek sok lehetőséggel, amely értelmet adna ezen alkalmazások használatának azon kívül, hogy nem kell a felhasználó egy külön eszközt magánál tartson.   A dolgozatom célja egy olyan rendszer tervezése, amely segítségével PowerPoint bemutatók diáin lehessen lézer mutatót használni az okostelefonunk segítségével attól függetlenül, hogy  Android-os  vagy  IOS-es  telefonunk  van.  Ezen  felül  a  diák  közötti  váltást,  illetve  ezekre történő rajzolást is lehetővé tegye. A rendszer két komponensből épül fel: az egyik része a szerver, amely fogadja, illetve  feldolgozza a telefonunk  által küldött adatokat; a másik része  a telefon, amely a felhasználó kézmozdulatait érzékeli a telefonban található gyorsulásmérő segítségével, illetve a megjelenített gombok lenyomását is, amelyeket elküld a szervernek WiFi-n keresztül. A szerverhez történő kapcsolódáshoz szükséges adatokat a szerver által generált QR kód beolvasása teszi lehetővé.</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Mobil alkalmazás, PowerPoint, lézermutató.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -858,6 +964,11 @@
           <t>A modern és gyor san fejlődő világban már minden szükségletünk, hobby és munka mögött egy elektromos technológia áll, amiket kényelmesen, gondok nélkül használunk. A mostani időkben az infláció emelkedésével minden szükségletnek az ára megemelkedett, legfőképpen az elektro mos áram, ezáltal, hogy ha nem figyelünk oda a mindennapi energia fogyasztásunkra és nem változtatunk az energia felhasználási szokásainkon, akkor könnyen anyagi gondokba ütközhetünk.  A dolgozatom célja egy olyan IoT (Internet of Things) rendszer kialakítá sa, amely lehetővé teszi a háztartáson belüli elektronikai berendezések fogyasztásának könnyű mérését és nyomon követését. Emellett a rendszer képes monitorozni a háztartásban telepített napelemek termelését is. Az adatokat egy adatbázisban tárolom, ami le hetővé teszi a későbbi statisztikák és elemzések készítését. Ezáltal pontosabb betekintést lehet nyerni az energiaköltségekbe, valamint segít optimalizálni a fogyasztást és kihasználni a megújuló energiaforrásokat.  A különböző egységek MQTT protokollon ker esztül kommunikálnak egymásközt, a publisherek(háztartási berendezés, napelemek) küldenek mintavételezett adatokat a brokernek(Raspberry pi), ahol az adatok fel vannak dolgozva, el lesznek tárolva egy MongoDB adatbázisban és a kész adatok egy REST API szol áltatáson keresztül el lesznek küldve egy mobilos applikációra.</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>IoT, Intelligens teljesítmény mérő , MQTT, Energ ia Menedzsment</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -880,6 +991,11 @@
           <t>Az elmúlt időszakban jelentős növekedést tapasztalhattunk az ipari robotok terén és felhasználási területük is folyamatosan bővül. Ezek a robotok egyre több funkcióval rendelkeznek és egyre szélesebb körben képesek emberi munkákat elvégezni. A kutatásunk során az ipari robotok vezérlésével foglalkoztunk, célunk egy rendszer kifejlesztése volt, amely rögzíti a felhasználó mozgását és ezek alapján számítja ki az ipari robot vezérléséhez szükséges jeleket.  Diplomadolgozatomban egy távoli vezérlésű kétkarú ipari robot vezérlésére alkalmas rendszer megoldását terveztük, amely az emberi kar mozgását használja alapul. A robot mindkét karját valós időben kellett vezéreljük, ezért a második generációs Kinect érzékelőt alkalmaztuk, amely alkalmas a mozgás követésére és távolság mérésére. A Kinect kamera által nyújtott adatokat olyan formába alakítottuk át, ami alkalmas egy robotkar vezérlésére. Az ipari robot karjainak vezérléséhez a felhasználó végtagjainak és ízületeinek szögeit használtuk. A kivitelezéshez egy fejlesztési célra tervezett Baxter kooperatív robotot használtunk, amely egy fix platformra rögzített robot, amely két, egyenként hét szabadságfokkal rendelkező, robotkarral rendelkezik. A rendszer lehetővé teszi a robot kézmozdulatokkal való vezérlését.  A rendszer a robotkar mozgatása mellett lehetővé teszi a felhasználónak, hogy a robotkar megfogó eszközeit kézmozdulatokkal vezérelje. A kéz állapota alapján a robot megfogó eszközei kinyílnak vagy bezáródnak.  A dolgozatban a robot vezérlésére a ROS (Robot Operating System) könyvtárait használtam. Emellett a Kinect kamera kezelésére a Kinect SDK-t, a komponensek közötti kommunikációra ZMQ protokollt használtam. Az így kifejlesztett rendszer képes felismerni a felhasználót, lekövetni a mozgását, és egy kétkarú ipari robotra ráilleszteni azt.</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>ipari robot, gesztusok, távvezérlés, Kinect</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -900,6 +1016,11 @@
       <c r="D25" t="inlineStr">
         <is>
           <t>Atechnol ógiaifejlődésnekköszönhetőenazokostelefonok ésazinternet elengedhetetleneklettek azéletünkben, hiszen mindig kéznélvannak, ésmáramáregyfajta személyiasszisztens szerepet betöltve járulnak hozzáazéletünkmegkönnyítéséhez.Azéletünkmásiknagy részétmégmindig személyesügyintézésekéspapíralapúdokumentumokhatározzákmeg.Jólérezhet őegyfajta gátakétpólusköztmelyb őlazegyikre afolyamatosmozgás,gyorsas ágmígamásikraalassúság,időigényességjellemz ő.Adolgozat céljaegyhatékony ésgyors rendszer kidolgoz ásaamely révéneztagátatfeloldjuk, egyújfajta lehetőségetszolgáltatva abüntetésekügyintézésére.Ahagyom ányosmódszerek nem képesek lépésttartani afelgyorsult világunkkal, ésproblémákatokozhatnak, mint példáulabirságoknehézkes rendszerez éseésazebbőlfakadókifizet ésnek azelmúlasztása.Amaitechnol ógiai elvárásoknak megfelel őrendszerkidolgoz ásáttűztükkicélul.Arendszer kifejleszt ésesoránfigyelembe vettükmindk étfélt,akiabüntetéstkiosztja illetve akieztmegkapja, ésigyekezt ünkegyolyan megval ósításraamely mindk étszerepk örszámáraidőtakar ékosésgyors. Abüntetéskiszot ásáhozegyandroidos applik ációhaszn álatatűntalegmegfelel őbbnek, mivel atelefonunk állandóankéznélvanilletve interneten kereszt ülazonnali hozzáféréstistudbiztos ítaniafelhaszn álónak azadatbázishoz. Ajárművezetőknek szántrendszer kivitelez éséhezalegkézenfekv őbbnek egywebes felületmegval ósításatűntmivel ezáltalegyviszonylagnagyobb felületentudunk jobbrálátástnyújtaniszámukra abírságokkönnyebb átlátásáhozilletve kifizet éséhez.</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>büntetésekügyintézése,androidos applik áció,webes felület</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Extract Hungarian and English abstract information from PDFs
</commit_message>
<xml_diff>
--- a/szamteches_info_extracted.xlsx
+++ b/szamteches_info_extracted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,10 +451,15 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Kivonat</t>
+          <t>Kivonat (magyar)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Kivonat (angol)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Kulcsszavak</t>
         </is>
@@ -479,6 +484,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>This paper describes in detail a system and its architecture for managing direction change and braking signals on scooters and bicycle s, using a sensor with an accelerometer and gyroscope on the back of the hand. The project aims to provide a solution for direction signals on the crank without removing the hand from the handlebars, thus avoiding the resulting accidents. The user is able to indicate a change of direction by gestures such as turning the hand sideways, so that it is not necessary to take the hand completely off the steering wheel, thus maintaining the balance of the vehicle. Brake signals are automatic as a result of acceler ation sensing. The system uses two microcontrollers (ESP32 and ESP8266), one of which processes the sensor data, while the other runs a web server and lights the corresponding LEDs. The web server is responsible for the communication between the microcontr ollers and also runs a web page that acts as a user interface. On the web page, active signals such as turn signals and brake signals are displayed and can be switched on and off. Communication between the different components is wireless using WiFi techno logy.</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>mikrovezérlő, WiFi, giroszkóp, gyorsulásmérő</t>
         </is>
       </c>
@@ -505,6 +515,11 @@
         </is>
       </c>
       <c r="E3" t="inlineStr">
+        <is>
+          <t>This thesis presents the implementation of a smart home control system. The system mainly performs home automation tasks such as temperature control, watering of plants and automatic movement of shutter , thus facilitating the user's daily life. Nowadays, IoT devices are playing an increasingly important role for people, and we can't imagine our lives without them. Since most  people have an internet connection at home, building such an IoT system is easier, cheaper and more efficient because there is no need for wires to communicate between devices.   The system I developed and built consists of a central computer with a touch screen display connected to it, where you can follow and intervene in the automation processes, you can see statistics about the temperature in the room, for example. Several sensors are connected to this central part via Bluetooth or MQTT communication pr otocols, which provide data and perform the automation tasks. In my thesis I document the design and construction of this system in detail, illustrating each part with diagrams.</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
         <is>
           <t>IoT, Home -automation, Raspberry Pi,  MQTT</t>
         </is>
@@ -521,6 +536,11 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>Measuring temperature has always played an important role in human life due to the curiosity of it’s nature. With the advance of the world and the temperatures measuring technologies, this task has become a trivial problem, regardless of what we measure the temperature of.  The scope of this project is to create a heat follower robot and a mobile application for controlling it, which identifies the temperature extremes in a closed area and approaches it, as well. As for the app, my aim is to establish a Bluetooth connection between this and the robot and show a picture of it’s view to the user. Also, I want it to make manual control possible.</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>hőmérséklet mérés, bluetooth, alkalmazás, szabad vezérlés</t>
         </is>
       </c>
@@ -548,6 +568,11 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>The topic of this thesis is the classification of brain tumours using convolutionalneural networks. In the first half of the paper, I will describe neural networks basedon  the  literature,  starting  from  simple  M-P  neurons  to  convolutional  neuralnetworks, covering their structure and their training. In the second half of thepaper, I present three models I developed that classified brain tumours into fourgroups with an accuracy of over 85%. The first model I implemented was a simpleconvolutional neural network. With the second model I achieved only moderateperformance  improvements  by  changing  the  architecture  and  preventingoverfitting. For both models I tuned the hyperparameters. The best performingmodel was the third one, implemented with transfer learning and using VGG16 asthe base model. This model achieved the best accuracy (96%). In developing thethree models, I used methods to continuously improve the performance of neuralnetworks  by  understanding  the  different  mechanisms  of  action.  The  model  Ideveloped  could  form  the  basis  for  an  application  that  provides  practicingradiologists with rapid preclassification in seconds, making their job easier.Tartalomjegyzék1.  Bevezető.................................................................................................................................... 142.  Mesterséges neurális hálózatok ................................................................................................ 152.1.  A biológiai neurontól a perceptronig ................................................................................ 152.2.  Perceptron......................................................................................................................... 172.3.  MLP.................................................................................................................................. 192.4.  Aktivációs függvények ..................................................................................................... 19 Szigmoid aktivációs függvény ............................................................................................ 20 Tangens hiperbolikus függvény .......................................................................................... 20 ReLU rektifikált lineáris ...................................................................................................... 20 Leaky ReLU........................................................................................................................ 21 Softmax aktivációs függvény .............................................................................................. 21 Aktivációs függvények megválasztása ................................................................................ 213.  Neurális hálózatok tanítása ....................................................................................................... 223.1.  Költségfüggvények ........................................................................................................... 22 Átlagos négyzetes eltérés .................................................................................................... 22 Bináris kereszt-entrópia ....................................................................................................... 233.2.  Gradiens alapú tanítás ....................................................................................................... 233.3.  Hiba-visszaterjesztés ......................................................................................................... 243.4.  Stochastic Gradient Descent ............................................................................................. 283.5.  ADAM optimalizáló ......................................................................................................... 294.  Konvolúciós neurális hálózatok ................................................................................................ 314.1.  Konvolúciós réteg ............................................................................................................. 314.2.  Összevonó réteg (pooling) ................................................................................................ 325.  A modell kivitelezése ................................................................................................................ 345.1.  Használt hardver és szoftver ............................................................................................. 345.2.  Néhány definíció ............................................................................................................... 34 Tanító, validációs és tesztelő adathalmaz ............................................................................ 34 Batch.................................................................................................................................... 34 Epoch................................................................................................................................... 34 Túltanítás............................................................................................................................. 35 Dropout................................................................................................................................ 355.3.  A képek előkészítése ......................................................................................................... 355.4.  Első modell megvalósítása ................................................................................................ 37 Architektúra......................................................................................................................... 38 Hiperparaméterek hangolása ............................................................................................... 39 Tanítás................................................................................................................................. 41 Tesztelés és kiértékelés ........................................................................................................ 435.5.  Második modell megvalósítása ......................................................................................... 44 Architektúra......................................................................................................................... 44 Hiperparaméterek hangolása ............................................................................................... 45 Tanítás................................................................................................................................. 46 Tesztelés és kiértékelés ........................................................................................................ 485.6.  Harmadik modell megvalósítása ....................................................................................... 49 Architektúra......................................................................................................................... 50 Tanítás................................................................................................................................. 51 Tesztelés és kiértékelés ........................................................................................................ 53105.7.  A három modell összehasonlítása ..................................................................................... 546.  Vizuális felület a modell működésének szemléltetésére ........................................................... 556.1.  A vizuális felület működése .............................................................................................. 556.2.  A vizuális felület használata ............................................................................................. 567.  Következtetések ........................................................................................................................ 607.1.  Továbbfejlesztési lehetőségek ........................................................................................... 608.  Irodalomjegyzék ....................................................................................................................... 619.  Függelék.................................................................................................................................... 6411Ábrák  jegyzéke1. ábra: A biológiai neuron szerkezete ........................................................................................... 152. ábra: M-P neuron. Forrás [3] ..................................................................................................... 163. ábra: A perceptron. Forrás [5] .................................................................................................... 174. ábra: Lineárisan szétválasztható (A) és lineárisan nem szétválasztható (B) mintahalmazok.Forrás [7] ....................................................................................................................................... .185. ábra: MLP felépítése. Forrás [11] .............................................................................................. 196. ábra: Gradiens alapú tanítás. Forrás [21] ................................................................................... 247. ábra: A láncszabály szemléltetlse. Forrás [23] .......................................................................... 268. ábra: Konvergencia összehasonlítás. Forrás [25] ...................................................................... 299. ábra: Konvolúciós réteg három színcsatornára. Forrás[32] ....................................................... 3210. ábra: Max és Average Pooling. Forrás [34]............................................................................. 3311. ábra: Glioma tumor .................................................................................................................. 3612. ábra: Meningioma tumor ......................................................................................................... 3613. ábra: Agyalapi mirigy tumor .................................................................................................... 3614. ábra: Egészséges agyszövet..................................................................................................... 3615. ábra: Képek beolvasása ............................................................................................................ 3716. ábra: Adathalmaz felosztása .................................................................................................... 3717. ábra: Első modell architektúra ................................................................................................. 3818. ábra: model_builder függvény ................................................................................................. 3919. ábra: Hyperband ....................................................................................................................... 4020. ábra: Korai leállás és hiperparaméter keresés .......................................................................... 4021. ábra: Első modell keresés mérések .......................................................................................... 4022. ábra: Modell létrehozása a legjobb hiperparaméterekkel ........................................................ 4123. ábra: Első modell tanítás és callback....................................................................................... 4124. ábra: Veszteség alakulása az első modell tanítása során ......................................................... 4225. ábra: Pontosság alakulása az első modell tanítása során ......................................................... 4226. ábra: Első modell konfúziós mátrix ......................................................................................... 4327. ábra: Második modell architektúra .......................................................................................... 4528. ábra: Második modell keresés mérések................................................................................... 4629. ábra: Második modell tanítás és callback................................................................................ 4630. ábra: Veszteség alakulása a második modell tanítása során .................................................... 471231. ábra: Pontosság alakulása a második modell tanítása során .................................................... 4732. ábra: Második modell konfúziós mátrix .................................................................................. 4833. ábra: Alapmodell létrehozása a VGG16 alapján ...................................................................... 4934. ábra: Alapmodell kiegészítése ................................................................................................. 4935. ábra: VGG16 architektúra, kép. Forrás[40] ............................................................................. 5036. ábra: VGG16 architektúra. Forrás[41] ..................................................................................... 5037. ábra: Harmadik modell tanítás és callback .............................................................................. 5138. ábra: Veszteség alakulása a harmadik modell tanítása során .................................................. 5239. ábra: Pontosság alakulása a harmadik modell tanítása során .................................................. 5240. ábra: Harmadik modell konfúziós mátrix ................................................................................ 5341. ábra: Szekvencia diagram ........................................................................................................ 5542. ábra: Kép előfeldolgozása ........................................................................................................ 5543. ábra: Kép osztályozása ............................................................................................................. 5644. ábra: Use case diagram ............................................................................................................ 5745. ábra: Kép feltöltés UI elem ...................................................................................................... 5746. ábra: Feltöltött kép megjelenítése ............................................................................................ 5847. ábra: Osztályozás eredményének megtekintése ....................................................................... 59Táblázatok jegyzéke1. táblázat Az első modell architektúrája ....................................................................................... 382. táblázat Az első modell hangolásra kiválasztott hiperparaméterei ............................................ 393. táblázat Az első modell optimálisnak talált hiperparaméterei ................................................... 414. táblázat A második modell architektúrája ................................................................................. 445. táblázat A második modell hangolásra kiválasztott hiperparaméterei ....................................... 456. táblázat A második modell optimálisnak talált hiperparaméterei .............................................. 467. táblázat Az általam hozzárakott rétegek felépítése .................................................................... 518. táblázat A modellek összehasonlítása ........................................................................................ 54131.BevezetőA mesterséges intelligencia egy számítógép azon képessége, hogy olyan feladatokat végezzen,amelyeket intelligens lényekkel társítunk. Az ilyen típusú feladatok megoldásához a modellnekrendelkeznie kell olyan emberre jellemző képességekkel mint az érvelés, felfedezés, általánosításés a múltbeli tapasztalatokból való tanulás. A gépi tanulás a mesterséges intelligencia egy olyanrészhalmaza, amely lehetővé teszi a rendszerek számára, hogy automatikusan tanuljanak, ésjavuljanak. A mesterséges neur ális hálózatok olyan számítási modellek, amelyeknek működését a biológiaineurális hálózatok ihlették. Úgy tervezték őket, hogy szimulálják a biológiai neuronok tanulásiés  döntéshozatali  képességét.  A  mesterséges  neurális  hálózatok  már  régóta  léteznek,  de  amúltban  a  fejlődésük  más  gépi  tanulási  módszerek  elterjedése  miatt  a  háttérbe  szorult.Napjainkban azonban a mesterséges neur ális hálózatok hatalmas népszerűségre tettek szert. Ezegyrészt annak köszönhető, hogy a digitális korszak rengeteg adatot termelt, így bőven vanamivel tanítani a neurális hálózatokat, másrészt Moore-törvénye beigazolódni látszott, az elmúlt50  évben  két  évente  megduplázódott  tranzisztorok  száma  az  integrált  áramkörökben,  és  aszámítási teljesítmény hatalmas növekedésen ment keresztül. Ezt a teljesítményt, ráadásul, afelhőplatformok elérhetővé tették bárki számára. Egy  típusa  a  mesterséges  neurális  hálózatoknak  a  konvolúciós  neuronhálók,  amelyek  a  jóképfeldolgozó  képességük  miatt,  gyakran  használnak  orvosi  leletek  analizálására  is.  Akonvolúciós neurális hálózatok kiválóan alkalmasak a bonyolult minták megragadására és areleváns  jellemzők  kinyerésére  az  orvosi  képekből,  ezáltal   lehetővé  téve  a  betegségek,rendellenességek  azonosítását.  Egy  tipikus  alkalmazási  területe  a   konvolúciós  neurálishálózatoknak képosztályozás, amely során a bemeneti képeket a jellemzőik, sajátosságaik szerintkülönböző osztályokba soroljuk.142.Mesterséges neurális hálózatok2.1. A biológiai neurontól a perceptronigA mesterséges  neurális  hálózatok ötlete a biológiai  neurális  hálózatokból alakult  ki, ezeketpróbálja modellezni és továbbfejleszteni. Ezért fontos, hogy a felvázoljuk, hogyan működik abiológiai neurális hálózat mielőtt rátérnénk a mesterséges neurális hálózatra.A biológiai idegrendszer idegsejtekből épül fel, amelyeknek három részük van. A dendritek aneuron  sejttestéből  nyúlnak  ki,  feladatuk  az  információk  fogadása.  A  sejttest  a  bemenetfeldolgozásáért felelős. Az axon, amely az idegsejtben a sejttest és a szinaptikus végződésekközött helyezkedik el, döntő szerepet játszik az idegsejtek összekapcsolásában és a köztük levőinformáció továbbításában. Azt folyamatot, amely során az egyik sejt axonja kapcsolódik amásik sejt dentritjéhez és a neurotranszmitterek segítségével megtörténik az információ átadás akét sejt között, szinapszisnak nevezzük.Az egyes neuronok működése önmagában elég egyszerű, erejük abban rejlik, hogy mindegyikükkapcsolódhat több ezer más neuronhoz, így, egy rendszert alkotva, már sokkal bonyolultabbműveletek elvégzésére is képesek.A mesterséges neuron fogalmát Warren McCullock neurofiziológus és Walter Pitts matematikusvezették be az 1943-ban a ’’A Logical Calculus of Ideas Immanent in Nervous Activity’’ címűtanulmányukban[2].  Az  általuk  felvázolt  neuronra  M-P  neuronként  hivatkozunk.Ennek  aneuronnak bináris bemenetei voltak és egy bináris kimenete.151. ábra: A biológiai neuron szerkezete . Forrás [1]xn - a neuron n-edik bináris bemenetey - a bináris kimenetg - az összegző függvényf - a küszöbfüggvényA neuron működésének két része van. Az első rész, g összegzi a bemeneteket, míg a másodikrész, f annak függvényében, hogy az így kapott érték nagyobb-e mint küszöbérték, hoz egydöntést.[4]g(x1,x2,x3,…,x2)=g(X)=∑i=1xiy=f(g(X))={1ifg(X)≥θ0ifg(X)&lt;θEzt a modellt fejlesztette tovább 1957-ben Frank Rosenblatt amerikai pszichológus, aki a Hebbtörvényből ihletődve rájött arra, hogy ha lazítunk az M-P neuron szabályain és nem egyenlőenjárul hozzá minden bemenet a kimenet értékéhez, akkor a mesterséges neuron képes tanulni.162. ábra: M-P neuron. Forrás [3]2.2. PerceptronA legegyszerűbb tanítható mesterséges neurális hálózat a perceptron. A neuron bemenetei azokaz értékek amelyek alapján kell meghoznunk a döntést. A neuron minden egyes bemenetéheztartozik egy tanítható wi súly.xn - a neuron n-edik bemenetey - a neuron kimenetewn - az n-edig tartozó súlytényezőb - a bias értékf - az aktivációs függvényAz y kimenetet úgy kapjuk meg, hogy kiszámítjuk a  bemenetek súlyozott összegét, hozzáadjuk abias értéket, és ha az így kapott eredmény meghaladja az adott θ küszöbértéket, akkor a kimenetértéke 1, ellenkező esetben a kimenet értéke 0. y={1if∑xiwi+b≥θ0ellenkezőesetbenAz egyszerű perceptron a bin áris kimenetéből és lineáris szeparálási képességéből adódóan csakegyszerűbb gyakorlati feladatok megoldására alkalmas, mint a bináris osztályozás. A perceptronképes arra, hogy megfelelő beállítás és tanítás után két lineárisan szeparálható mintahalmaztszétválasszon. Egy két dimenziós minthalmazt akkor nevezzük lineárisan szeparálhatónak, ha azegyik osztály elemeit el tudjuk választani a másik osztály elemeitől egyetlen egyenes vonallal. [6]173. ábra: A perceptron. Forrás [5]A perceptron tanításán a súlytényezők módosítását értjük addig amíg a z osztályozás mindenbemeneti vektorra helyes lesz. Ez a következőképpen történik:1.Inicializáljuk a súlytényezőket, ez történhet véletlenszerűen is;2.A tanítóhalmazból veszünk egy mintát, és kiszámoljuk rá a neuron kimenetét:y=f(Σwnxn+b)3.Módosítjuk a súlytényezőket a kiszámolt kimenet és az elvárt kimenet közti különbség,valamint a tanítási együttható szerint:wn[k+1]=wn[k]+µ(d−y)μ - a tanítási együtthatód - az elvárt kimenet[8]Ahogy fentebb is eml ítettem, az egyszerű perceptron csak lineárisan szeparálható mintahalmaztképest szétválasztani. Erre hívták fel a figyelmet Marvin Minsky és Seymour Papert az 1969-benkiadott tanulmányukban[9]. Egy híres példa erre az XOR függvény, amit az egyszerű perceptronnem tud megtanulni mert nem lineárisan szétválasztható. Ez a probléma viszont leküzdhetőazzal,  ha  több  rétegnyi  perceptront  kapcsolunk  össze,  ezáltal  létrehozva  egy  többrétegűelőrecsatolt neuronhálót, azaz MLP-t.184.  ábra:  Lineárisan  szétválasztható  (A)  és  lineárisan  nemszétválasztható (B) mintahalmazok. Forrás [7]2.3. MLPTopológiai szempontból az MLP neuronhálót alkotó neuronokat rétegekbe rendezzük. Az egyesrétegek neuronjai össze vannak kapcsolva a szomszédos rétegek összes neuronjával, és mindenkapcsolathoz  tartozik  egy  súly  érték  is.  Az  MLP  neuronháló  esetében  három  rétegetkülönböztetünk meg: bemeneti réteg, rejtett réteg és kimeneti réteg.A  bemeneti  réteg  a  neuronháló  első  rétege,  nincs  jelentős  szerepe  a neuronháló működéseszempontjából, csupán fogadja a bemeneti adatokat és továbbítja a rejtett rétegekben találhatóneuronok  bemenetére.  A  bemenetei  réteg  neuronjai  általában  nem  tartalmaznak  hangolhatóparamétereket. A rejtett réteg neuronjai a bemeneti és a kimeneti rétegeke között helyezkednekel, nincsenek közvetlen kapcsolatban a külvilággal. A rejtett réteg neuronjai a bemenetüket azelőző réteg neuronjaitól kapják, kiszámítják a súlyozott összegüket majd ezt továbbítják egyaktivációs  függvénynek.  A  rejtett  rétegek  számát,  és  az  egyes  rerjtett  rétegekben  találhatóneuronok számát az adott feladat összetettsége határozza meg.[10]2.4. Aktivációs függvényekMielőtt rátérnénk a neuronhálók tanítására, fontos, hogy megértsük az aktivációs függvényekfontosságát.  Az  M-P  neuronnál  használt  lépcsőfüggvény  lecserélése  más,  nemlineárisfüggvényekre  egy  fontos  mérföldkő  volt  a  neurális  hálózatok  történelmében.  Azért  vanszükségünk nemlineáris függvényekre, mert ha több lineáris függvényt láncolunk egymás után,195. ábra: MLP felépítése. Forrás [11]akkor  szintén  lineáris  függvényt  kapunk  eredményként.  Így  nincs  semmi  nemlineáritás  aneuronháló rétegei között, és több összekapcsolt lineáris réteg is, igazából egy lineáris rétegnekfelel meg, és ezzel nem lehet összetettebb problémákat megoldani.[12]Szigmoid aktivációs f üggvényA  szigmoid  aktivációs  függvény,  más  néven  logisztikus  aktivációs  függvény,  teljestartományban differenciálható, és a kimenetet a 0 és 1 közötti tartományba képezi le a következőegyenlet szerint:f(x)=11+e−xMivel a függvény kimenete 0 és 1 között van, ezért különösen olyan modelleknél használják,ahol valószínűséget kell megjósolni.[13]Tangens hiperbolikus függvényMint  ahogy  a  szigmoid  függvény,  a  tangens  hiperbolikus  függvény  is  folytonos  ésdifferenciálható. Az a különbség, hogy a kimenetet a -1 és 1 közötti tartományba képezi le.Emiatt, nagyobb az esély, hogy a tanítás elején a rétegek kimenete többé-kevésbé 0 körül legyen,ami gyakran segít felgyorsítani a konvergenciát. A tangens hiperbolikus függvény értékát akövetkező egyenlet alapján számoljuk ki:[14]f(x)=ex−e−xex+e−xReLU rektifikált lineárisJelenleg  a  legelterjedtebb  aktivációs  függvény.  Ez  a  gyorsaságából  fakad,  a  közelmúltbanbizonyosodott  be,  hogy hatszor gyorsabb  konvergenciát  biztosít  mint  a  tanges  hiperbolikusaktivációs függvény. A ReLU, ha a bemenet pozitív, ugyanazt az értéket téríti vissza, ellenkezőesetben nullát. A ReLU deriváltja minden esetben egy, és a kimenet sincs szaturálva. A ReLU-nak  az  az  egyetlen  hátránya,  hogy  mivel  az  összes  negatív  értéket  nullának  állítja,  ezértcsökkentheti a modell tanulási képességét, mert a negatív elemeket nem megfelően képezi le. Ezthaldokló ReLU problémának is nevezzük.[15]f(x)=max(0,x)20Leaky ReLUA  haldokló  ReLU  probléma  kiküszöbölésére  fejlesztették  ki.  Hasonló  a  ReLU-hoz,  az  akülönbség, hogy egy szivárgást biztosít a negatív bemeneteknek, ezáltal nem nullának lesznekleképezve, így biztosítja a tanulást ezen a szakaszon is.[16]f(x)={αxhax&lt;0xhax≥0Softmax aktivációs függvényA  softmax aktivációs függvény, a szigmoid függvényhez hasonlóan a kimenetet a 0 és 1 közöttitartományba képezi le. A softmax aktivációs függvényt gyakran használják a kimeneti rétegben  atöbbosztályos osztályozási feladatoknál. Egy valós számokból álló vektort alakít át valószínűségieloszlássá, amelynek minden egyes eleme egy adott osztályba tartozás valószínűségét jelöli.[17]s(xi)=exi∑j=1nexjAktivációs függvények megválasztásaA neurális hálózatok tervezésénél az aktivációs függvényt megválasztása nagyon fontos döntés.Az aktivációs függvény típusa függhet a probléma jellegétől és attól, hogy a neuron kimenetemilyen  értéket  vehet  fel.  Bináris  osztályozási  feladatoknál  általában  szigmoid  aktivációsfüggvényt használunk, mivel a kimenetet egy 0 és 1 közötti tartományba képezik le, amit egyvalószínüséget reprezentál. Többosztályos osztályozási problémák esetén a softmax aktivációsfüggvényt használjuk, mert a neurális hálózat kimenetét egy valószínűségi eloszlássá alakítja át.MLP és konvolúciós neuronhálók esetében a rejtett rétegekben érdemes a ReLU vagy LeakyReLU aktivációs függvényt alkalmazni, mert gyorsan konvergál és kevésbé kitett az eltűnőgradiens problémának.[18]213. Neurális hálózatok tanításaA neurális hálózatok tanítása olyan folyamat, amely lehetővé teszi a hálózat számára, hogyadatokból tanulva minél pontosabb előrejelzést vagy osztályozást készítsen. Ha különbségetakarunk  tenni  egy  kerékpár  és  egy  autó  között,  melyik  tulajdonságát  vennénk  figyelembeleginkább, a kerekek számát, a maximális sebességet vagy a színét? Természetesen, a kerekekszáma és a maximális sebesség alapján hoznánk meg a döntésünket, és nem a szín szerint. A gépis ugyanígy jár a el, minden jellemzőhöz egy súlyértéket rendel, ami segít, hogy megértse melyikjellemzőket fontos figyelembe venni az osztályozás során. A gép a legjobb döntés meghozásaérdekében módosítja a súlytényezőit. Ezt úgy teszi, hogy összehasonlítja a döntés értékét a tanítóhalmazbeli elvárt értékkel, költségfüggvényeket használva.[19]3.1. KöltségfüggvényekA  gradiens  alapú  tanítás  során  szükségünk  vagy  olyan  függvényre,  ami  deriválható,  ésszámszerűsíti a neuronháló hibáját, a neuronháló kimenete és az elvárt kimenet közötti eltérést.Ez a függvény méri fel, hogy mennyire teljesít jól a neurális hálózatunk az adott feladatratekintve. A következőkben egy pár, gyakran használt költségfüggvényt fogok ismertetni:Átlagos négyzetes eltérésAz átlagos négyzetes eltérés, vagy MSE (mean squared error) a neuronháló kimenete és az elvártkimenet  közötti  átlagos  négyzetes  különbséget  számítja  ki.  Nagyon  gyakran  használjákregressziós feladatoknál. Érzékeny a kiugró értékekre, mivel a különbségeket négyzetre emeli.[20]CMSE=12∑(di−yi)2ahol,di - az elvárt i-edik kimenet yi- az i-edik kimenet22Bináris kereszt-entrópiaA  bináris  kereszt-entrópia  költségfüggvényt  bináris  osztályozási  feladatoknál  használják.Megméri a megjósolt osztályba tartozási valószínűségek és az elvárt kimenet közti eltérést.CCE=−12∑[yi⋅ln(di)+(1−yi)⋅ln(1−di)]ahol, di- az elvárt i-edik kimenetyi - az i-edik kimenetA több osztályos osztályozási feladatok során a Categorical Cross-Entropy valamint SparseCategorical Cross-Entropy költségfüggvényeket használjuk. A különbség a két függvény között,hogy a Categorical Cross-Entropy függvénynél az elvárt kimeneteket vektoriális formában kellmegadni, míg a Sparse Categorical Cross-Entropy függvénynél egész számként.3.2. Gradiens alapú tanításA  gradiens  alapú  tanítás  egy  széles  körben  használt  optimalizálási  algoritmus  a  neurálishálózatok tanításához és más különböző gépi tanulási problémák megoldásához. A gradiens nemmás, mint a függvények deriválásának általánosítása többváltozós függvényekre. A gradiensalapú  tanítás  célja  a  költségfüggvény  minimalizálása  és  a  modell  teljesítményét  javítóparaméterek megtalálása.Ahhoz, hogy minimalizáljuk a költségfüggvényt optimalizálnunk kell a súlyokat, ehhez pedigmeg kell vizsgálnunk hogyan változik a költségfüggvény értéke a súlyértékek függvényében.Következő lépésben kiszámoljuk a költségfüggvény deriváltját a súlytényező függvényében. Ezta deriváltat nevezzük gradiensnek.Ha a hiba növekszik a súlytényezők növekedésével, akkor a gradiens pozitív lesz, és ha a hibacsökken a súlytényező növekedésével, akkor a gradiens negatív lesz. Tehát mindig a negatívgradiens mutatja azt az irányt amilyen irányba kell változtatni a súlyok értékét a költségfüggvényminimalizálása érdekében23A gradiens módszer alapján a súlyértékek változtatása a következőképpen történik:wúj=wrégi−μ⋅∂E∂wahol,w - a tanítani kívánt súlyértékE - a költségfüggvényμ - a tanítási együttható3.3. Hiba-visszaterjesztésA hiba-visszaterjesztés, vagy backpropagation algoritmus alapgondolata a hibák továbbítása akimeneti rétegből a bemeneti rétegbe egy láncszabály segítségével. A hiba-visszaterjesztés egyalgoritmus a költségfüggvény gradiensének a kiszámítására.[2 2]Először kezdjük egy egyszerűbb többrétegű neuronhálóval, ahol minden rétegben csak egy darabneuron van.246. ábra: Gradiens alapú tanítás. Forrás [21]Használt jelölések:L - a rétegek számaa - a neuron kimeneti értékekea(L−1) - az utolsó előtti rétegbeli neuron kimenetew - súlytényezőw(L−1) - az utolsó előtti réteghez tartozó súlytényezőb - a bias értékCk- egy tanítási adatra számolt hibay - az elvárt kimenetf - az aktivációs függvényLegyen a költségfüggvényünk az átlagos négyzetes eltérés, ami alapján egyetlen tanítási adatáltal okozott hiba a következőképpen írható fel:C0=(a(L)−y)2Az utolsó neuron kimenetét egy súly, egy bias érték és az azelőtti neuron kimenete határozzameg egy aktivációs függvény segítségével.a(L)=f(w(L)a(L−1)+b(L))Legyen z az inger, amit a következőképpen számolunk ki:z(L)=w(L)a(L−1)+b(L)Tehát:a(L)=f(z(L)) Azt szeretnénk megérteni, mennyire érzékeny a C0 költség a w(L) súly változására. Ehhez ki kellszámolnunk a ∂C0∂w(L) deriváltat.25Ha  ránézünk  a  neuronhálónk  felépítésére,  láthatjuk,  hogy  a  w(L)-ben  végbemenő  változásbefolyásolja z(L) értékét, a z(L)-ben végmenő változás befolyásolja az a(L) értékét, és végül az a(L)változása befolyásolja a C0 értékét.Ezeket a változásokat parciális deriváltakkal írhatjuk fel, ahol az egyenlet jobb oldalán levő elsőparciális derivált megadja a z(L)-ben w(L) által okozott változás értéket, a második az a(L)-ben z(L)által okozott változás értékét és a harmadik a  C0-ban  a(L) által okozott változás értékét. Ez aláncszabály, ahol a három parciális derivált szorzata megadja végül a mennyire érzékeny a C0költség a w(L) súly változására.∂C0∂w(L)=∂z(L)∂w(L)∂a(L)∂z(L)∂C0∂a(L)A parciális deriváltak kiszámítása:z(L)=w(L)a(L−1)+b(L)→ ∂z(L)∂w(L)=a(L−1)a(L)=f(z(L)) →∂a(L)∂z(L)=f'(z(L))C0=(a(L)−y)2    →∂C0∂a(L)=2(a(L)−y)267. ábra: A láncszabály szemléltetlse. Forrás [23]A kiszámolt parciális deriváltak alapján kapjuk, hogy:∂C0∂w(L)=a(L−1)f'(z(L))2(a(L)−y)Hasonlóan  járunk  el  ha  a  b(L) bias  értékre  szeretnénk  kiszámítani  a  költségfüggvényérzékenységét.∂C0∂b(L)=∂z(L)∂b(L)∂a(L)∂z(L)∂C0∂a(L)Láthatjuk, hogy csak az első parciális derivált értéke tér el, amit a következőképpen számolunkki:z(L)=w(L</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>konvolúciós neuronhálók, agydaganat, osztályozás, keras</t>
         </is>
       </c>
@@ -575,6 +600,11 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>The  topic  of  my  paper  is  documenting  and  tracking  the  game  of  backgammon  game  in  which  I  dealt  with  game  programming,  image  processing,  and  real-time  game  tracking  of  game  progres.  Backgammon  and  image  processing  cover  two  areas  of  particular  interest  to  me..  The  Romanian  Backgammon  Federation  organizes  various  national  and  international  competitions,  where tracking and automatic arbitration are of particular interest.  The  Python  programming  language  allows  for  the  creation  of  virtual  versions  of  backgammon,  which  gives  the  game  a  new  dimension  by  interactively  playing  it  on  the  computer .  The  goal  of  game  programming  was  to  enable  two  players  to  compete  against  each  other  on  the  computer  and record the game for later replay .  OpenCV  (Open  Source  Computer  Vision  Library)  is  a  popular  library  used  in  image  processing.  With  its  help,  the  computer  can  recognize  shapes  and  process  images,  allowing  for  capturing  the  sequential  playing  positions.  My  goal  in  the  field  of  image  processing,  was  to  extract  still  frames  from a video and identify the position of pieces, thus tracking the game's progress.  Therefore,  my  objective  was  to  create  an  application  by  combining  Python  and  OpenCV  that  automatically  evaluates  the  board  game.The  software  to  be  made  must  recognize  the  positions  of  pieces and tracks the players' moves, allowing for virtual gameplay between two individuals.</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>táblajáték, képfeldolgozás, opencv , python</t>
         </is>
       </c>
@@ -598,6 +628,11 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t>Nowadays, using s ensors has become so popular that we do not even notice how easy it is for us to measure the world around us. Today we have the possibility and the technology to measure the physical, chemical and the biological characteristics of the world around us.  The goal of my thesis was to build a scalable system for sensors, created with the help of an Arduino, which helps in the integration of new sensors in the system for users, who may face a challenge when integrating a new sensor in an environment with Arduino and microcontrollers.  At the beginning I had to create a text -based protocol, written with ASCII code, which provides for the user an interface for dynamic configuration of the sensors and for the collective data forwarding.  Several different sensors have  been integrated into the sensor system, with which it is possible to measure different physical quantities and monitor changes in values , but also an interface for the collected data.  For the better understanding of the real -time data collected by the sen sors with the help of the Arduino I have also created a desktop application, , through which the real -time data measured by the sensors connected to the Arduino can be displayed, and it is also possible to save and review the data.  The communication betwee n the application and the sensors is realized by serial communication.  I designed the application to be used for laboratory purposes.  Keyword s: Arduino, protocol, sensors, desktop application         8  Tartalomjegyzék  1. Bevez ető ................................ ................................ ................................ ...............................  11 1.1. Bevezető  ................................ ................................ ................................ .......................  11 1.2. Célkitűzések  ................................ ................................ ................................ ..................  11 2. Elméleti megalap ozás ................................ ................................ ................................ ...........  13 2.1. Arduino  ................................ ................................ ................................ .........................  13 2.2. Arduino Uno  ................................ ................................ ................................ .................  13 2.3. Arduino IDE  ................................ ................................ ................................ .................  15 2.4. Soros kommunikáció  ................................ ................................ ................................ ..... 16 2.5. ASCII protokoll  ................................ ................................ ................................ ............  17 2.6. Érzékelők  ................................ ................................ ................................ ......................  18 2.6.1. Akadályelkerülő érzékelő  ................................ ................................ .......................  19 2.6.2.  Analóg hőmérséklet érzékelő  ................................ ................................ .................  20 2.6.3. Analóg mágneses Hall érzékelő  ................................ ................................ .............  20 2.6.4. Digitális hőmérséklet érzékelő  ................................ ................................ ...............  21 2.6.5. Fényblokkolás  érzékelő  ................................ ................................ ..........................  22 2.6.6. Hőmérséklet és páratartalom érzékelő  ................................ ................................ .... 22 2.6.7. Vonalkövető érzékelő  ................................ ................................ ............................  23 2.7. Asztali alkalmazás ................................ ................................ ................................ .........  24 3. A rendszer specifikációi és architektúrája  ................................ ................................ .............  25 3.1. Követelmény specifik áció ................................ ................................ .............................  27 3.1.1.  Felhasználói követelmények  ................................ ................................ ..................  28 3.1.2. Rendszerkövetelmények  ................................ ................................ ........................  29 4. Részletes tervezés és gyakorlati megvalósítás  ................................ ................................ ....... 32 4.1. Arduino kód  ................................ ................................ ................................ ..................  32 4.1.1.  Protokoll működésének bemutatása ................................ ................................ ........  33 4.2. Asztali alkalmazás ................................ ................................ ................................ .........  37 4.2.1.  Kezdőoldal ................................ ................................ ................................ .............  39 4.2.2. Érzékelő adatlapja oldal  ................................ ................................ .........................  40 4.2.3. Konfigurációs oldal  ................................ ................................ ................................  41 4.2.4. Adatok megjelenítése oldal  ................................ ................................ ....................  43 4.2.5. Folytonos olvasás oldal  ................................ ................................ ..........................  45 4.2.6. Korábbi mérések oldal  ................................ ................................ ...........................  47 5. Következtetések  ................................ ................................ ................................ ....................  50 5.1. Megvalósítások  ................................ ................................ ................................ .............  50 5.2. Továbbfejlesztési lehetőségek  ................................ ................................ .......................  50 6. Irodalomjegyzék  ................................ ................................ ................................ ...................  52     9  Ábrák jegyzék e 1.  ábra - Arduino Uno áramköri lap  ................................ ................................ .........................  13 2. ábra - Arduino Uno perifériáinak lábkiosztás a ................................ ................................ ...... 14 3. ábra - Arduino IDE  ................................ ................................ ................................ ...............  16 4. ábra - Soros kommunikáció  ................................ ................................ ................................ .. 16 5. ábra - ASCII kódtábla  ................................ ................................ ................................ ...........  17 6. ábra - Érzékelő működési elve  ................................ ................................ ..............................  18 7. ábra – Breadboard  ................................ ................................ ................................ .................  19 8. ábra - HW-488 érzékelő  ................................ ................................ ................................ ........  19 9. ábra - HW-498 érzékelő  ................................ ................................ ................................ ........  20 10. ábra - HW-495 érzékelő  ................................ ................................ ................................ ...... 21 11. ábra - HW-506 érzékelő  ................................ ................................ ................................ ...... 21 12. ábra - HW-487 érzékelő  ................................ ................................ ................................ ...... 22 13. ábra - DHT11 érzék elő................................ ................................ ................................ ........  23 14. ábra - HW-511 érzékelő  ................................ ................................ ................................ ...... 23 15. ábra - .NET MAUI  ................................ ................................ ................................ ..............  24 16. ábra – A rendszer vázlata  ................................ ................................ ................................ .... 25 17. ábra - Tömbvázlat  ................................ ................................ ................................ ...............  26 18. ábra - Arduinohoz kötött érzékelők  ................................ ................................ .....................  27 19. ábra - Alkalmazás Használat -Eset diagramja  ................................ ................................ ....... 28 20. ábra - Digitális bemenet konfigurálása  ................................ ................................ ................  34 21. ábra - Hibás konfigurációs parancs küldése  ................................ ................................ .........  34 22. ábra - Olvasási parancs küldése  ................................ ................................ ...........................  34 23 . ábra – Érzékelők nevei és a hozzá tartozó függvények map tárolója  ................................ ... 35 24. ábra - hibás olvasási parancs küldése  ................................ ................................ ..................  35 25. ábra - Hibás olvasási parancs küldése ................................ ................................ ..................  35 26. ábra - Folyamatos olvasási parancs küldése ................................ ................................ .........  36 27. ábra - Folyamatos olvasás leállítása  ................................ ................................ ....................  36 28. ábra - Ismeretlen parancs küldése  ................................ ................................ ........................  36 29. ábra – Soros kommunikáció elindítása  ................................ ................................ ................  37 30. ábra - Függvény a kommunikációs kapcsolat létrehozására  ................................ .................  38 31. ábra - Hivatkozás könyvtár csomagokra  ................................ ................................ ..............  38 32. ábra - MVVM tervezési minta ................................ ................................ .............................  39 33. ábra – Alkalmazás kezdőoldala  ................................ ................................ ...........................  40 34. ábra - Kiválasztott bekötési rajz megjelenítése  ................................ ................................ .... 40 35. ábra - Érzékelő adatlap oldala  ................................ ................................ .............................  41 36. ábra - Kivezetés konfigurálása  ................................ ................................ ............................  42 37. ábra - Konfigurálás után kapott visszajelzések  ................................ ................................ .... 42 38. ábra - Nincs csatlakoztatva az Arduino áramköri lap  ................................ ...........................  42 39. ábra - Érzékelő adatainak beolvasása  ................................ ................................ ..................  43 40. ábra - Hibaüzenet, ha nem volt érzékelő kiválasztva  ................................ ...........................  43 41. ábra – Szenzor adatok  megjelenítése oldal  ................................ ................................ ..........  44 42. ábra - Üres oldal  ................................ ................................ ................................ .................  45 43. ábra - Folytonos olvasás megjelenítése  ................................ ................................ ...............  46 44. ábra - Folytonos olvasás folytatása  ................................ ................................ ......................  46 45. ábra – Jelmagyarázat  ................................ ................................ ................................ ...........  47 46. ábra - Mérési adatok l istázása  ................................ ................................ .............................  47    10  47. ábra - Mentett mérési adatok  ................................ ................................ ...............................  48 48. ára - Sikeres mentés  ................................ ................................ ................................ ............  48 49. ábra - Navigációs függvény  ................................ ................................ ................................  49 50. ábra - Gomb adattagjainak megadása  ................................ ................................ ..................  49  Táblázatok  jegyzéke  1. táblázat - Arduino Uno paraméterei  ................................ ................................ ......................  15 2. táblázat - HW-488 paraméterei  ................................ ................................ .............................  19 3. táblázat - HW-498 paraméterei  ................................ ................................ .............................  20 4. táblázat - HW-495 paraméterei  ................................ ................................ .............................  21 5.táblázat - HW-506 paraméterei  ................................ ................................ ..............................  22 6. táblázat - HW-487 paraméterei  ................................ ................................ .............................  22 7. táblázat - DHT11 paraméterei  ................................ ................................ ...............................  23 8. táblázat - HW-511 paraméterei  ................................ ................................ .............................  24     11  1. Bevezető  1.1.  Bevezető  Az információk világában élünk , amikor azt szeretnénk, hogy minél több  inform ációhoz hozzáférhessünk a környezetünkből . A különbö ző érzékelők  mára már nagyon elterjedtek, a mindennapjaink részévé váltak. Egyre több elekt ronikus készülék kerül a piacra, amik működéséhez elengedhetet len az érzékelők használata és ezáltal azok folyamatos fejlődése. Szenzorok használata által lehetőség van a környezetünk fizikai, kémiai, biológiai tulajdonságainak mérésére és ezek villamos mennyiséggé alakítá sára.   Az érzékelők megfelelő összekötése, több érzékelő integrálása egyetlen rendszerbe kihívá st jelenthet, mivel a szenzorok  különböző típúsúak, az adatokat nem egységes formában továbbítják. Az interaktív érzékelőrendszer használatával ez tehető könnye bbé, egy olyan felhasználó számára, aki szeretne  kicsit jobban elmerülni az érzékelők  és az Arduino, mikrovezérlők  világában.  Egy protokoll segítségével egységes formában érhetőek el az ér zékelők adatai, lehetőséget teremtve az adatok elemzésére, azok öss zehasonlítására. A rendszer segítségével nincs szükség arra, hogy minden, a rendszerben megtalálható szenzor kódját külön -külön megírja, hanem ehhez kap  egy egységes felületet  a felhasználó . A rendszer lehetőséget teremt különböző típusú érzékelők egyszerű  és hatékony int egrálására. A szenzorok használa tával a rendszer felhasználói követhetik a hőmérséklet, páratartalom változását a környezetükben, de más mérések elvégzése is lehetséges.  Ha adott a felhasználó számára egyetlen felület, amelyen keresztül kez elhető egy rendszer az a felhasználóban is pozitív benyomást kelt, hiszen megkönnyíti számára egy feladat elvégzését, könnyedén hozzájuthat  minden információhoz az érzékelőkkel kapcsolat ban. Az egységes felület előnyei a hatékonyság, felhasználói élmény ja vítása, idő sporlása. A dolgozatban bemutatott interaktív érzékelőrendszer egy könnyen kezelhető felületet nyújt a felhasználó számára az érézkelők világában, így elősegítve, hogy minél jobban megismerhesse azt. 1.2. Célkitűzések  A dolgozat elkészítése során a következő célok voltak kitűzve:     12   Szöveges parancsértelmező kódjának a megírása , általános protokoll kivitelezése : egy olyan kód megírása, ami segítségével szöveges parancsokat lehet küldeni  és fogadni a mikrovezérlőn, a szenzorok dinami kus konfigurálása, ad atainak tov ábbítása is ezen keresztül valósul meg. A protokollnak biztosítania kell, hogy az adatok egységes formában legyenek továbbítva, valamint minden elküldött parancsra érkezzen egy válasz.   Különböző érzékelők  a rendszerbe való integrálása és program ozása: a különböző szenzorok kódjának összegyűjtése és azok olyan formában történő átírása, amelyek a protokoll alapján képesek megvalósítani az adatgyűjtést . Az érzékelők dinamikus konfigurálása, ami azt jelenti, hogy a rendszer használata közben választh ató ki, hogy melyik kivezetésre kötjük a szenzort, nem kell ezt már a kódban előre meghatározni.  Lehetőség legyen arra, hogy egy rendszerhez egyszerre több érzékelőt is lehessen csatlakoztatni, így egy időben több különböző szenzor által küldött adat is rö gzíthető.   Felhasználói felület készítése: egy olyan alkalmazás elkészítése, ami lehetővé teszi a felhasználó számára, hogy a szenzorokat dinamikusan konfigurálja és az azoktól kapott adatokat megjelenítse . A felület tervezése során fontos figyelembe venni,  hogy a felület  olyan legyen, aminek ha sználatához nincs szüksé g hosszú tanulási időre , átlátható, felhasználóbarát. Legyen lehetősége a  felhasználónak többet megtudni  a kiválasztott érzékelőről, anélkül, hogy külön keresést kellene ehhez végeznie, így az alkalmazáson belül legyenek megjeleníthetőek a kapcsolási rajzok, megnyithatóak a szenzorok adatlapjai.  A mérési adatok rögzítése és listázása, így összehasonlíthatók a különböző időpontokban végzett mérések.     13  2. Elméleti megalapozás  2.1. Arduino  Az Arduino  egy elektronikus eszközöket és szof tvereket ter vező, gyártó, támogató hardver - és szoftvercég, ami lehetővé teszi , hogy az emberek hozzáférhessenek azokhoz  a fejlett technológiákhoz, amelyek által  kapcsolatba lépnek a fizikai világgal. Termékeik egysz erűek, nagy teljesítményűek és képesek arra, hogy a felhasználók igényeinek széles skáláját kielégítsék, kezdve a diákoktól a professzionális felhasználó kig. [1]  Az Arduino projekt 2005 -ben, Olaszországban indult, azzal a céllal, hogy olcsó és egyszerű megoldást ny újtson o lyan eszközök létrehozására, ame lyek érzékelők használatának segítségével kapcsolatba lépnek környezetükkel. [2]  Az Arduino két részből tevődik össze: az Arduino IDE -ből, vagyis egy nyílt forráskódú fejlesztői környezetből  és az Arduino lapból. Az Ardu ino lapoknak számos fajtája létezik, amik méretben, mikrovezérlő típusában, ki - és bemenetek s zámában különböz nek egymástól. [3] 2.2. Arduino Uno  A rendszer kialakí tásánál egy Arduino Uno ( 1.  ábra) típusú  lapot használ tam. Az érzékelőrendszer kialakításánál azért esett a választás, Arduino Uno mikrovezérlőre, mivel ez egy széles körben elterjedt típus, sok d okumentáció van, amelyek segítsé gül szolgá lhatnak a megvalósítás során, valamint rengeteg könyvtár megtalálható, a melyek a fejlesztésben felhasználhatóak. Ez a mikrovezérlő rendelkezik elég sok kivezetéssel, így a rends zer jól bővíthető, egy   időben több szenzor is rácsatlakoztatható.   1.  ábra - Arduino Uno áramköri lap1                                                 1 Forrás: https://circuitdigest.com/article/everything -you-need -to-know -about -arduino -uno-board -hardware     14  Megtalálható benne egy  ATMega328 /P típusú,  5V feszült ségen működő, 8 bites mikrovezérlő. Rendelkezik 2 KB SRAM memóriával, 1  KB EEPROM  memóriával a paraméterek tárolására és 32 KB flash memória áll rendelkezésre a programok tárolására. A lapon még  megtalálhatóak az analóg és d igitális ki /bemenetek, amiken keresztül kapcsolhatóak az érzékelők az Arduinohoz. A lap két oldalán található tüskesor aljzat melletti számokkal  (2. ábra) hivatkozhatunk a kódban a megfelelő kivezetésre. [4]  2. ábra - Arduino Uno perifériáinak lábkiosztása2  Az Arduino egyik érdekessége, hogy a megírt kód feltöltés után az azonnal fut rajta, ez a bootloader segítségével valósul meg. Az USB csatlakozónak kettős szerepe van, ezen keresztül tölthet ő fel rá a program valamint biztosítható a működé séhez szükséges 5V feszültség , ez megoldható a külső tápcsatlakozó használatával is. [5]  Az alábbi táblázatban ( 1. tábláza t) megtalálhatóak az Arduino Uno legfőbb jellem zői:                                                                                                                                                           2 Forrás: https://docs.arduino.cc/retired/boards/arduino -uno-rev3-with-long-pins    15  Mikrovezérlő  ATMega328 /P Órajel  16MHz  Működési feszültség  5V Analóg ki/bemenetek száma  6 Digitális ki /bemenetek száma  14 SRAM  2KB  EEPROM  1KB  Flash memória  32KB  Maximális tápfeszültség (nem ajánlott)  20V 1. tábláza t - Arduino Uno paraméterei  2.3. Arduino IDE  Az Arduino IDE az a fejlesztői környezet, amelyben programozható az Arduino Uno. A kód C/C++ nyelven írható meg. Sok könyvtár is elérhető, amik nagy segítséget nyújtanak a programkód megírásában. A környezet áll egy szövegszerkesztőből és egy fordítóból, az Arduinotól kapott válaszokat a Serial monitor és Serial plotter segítségével lehet követni, megjeleníteni.  Egy új pro gram  fájl létrehozásakor ( 3. ábra) egy sablon jelenik meg, aminek két fő része van:  a setup() és a loop() függvény.  A setup függvényben történik az inicializáció, ez egyszer fut le, itt adható meg  például az adatok átviteli seb essége (baud rate). A loop függvény az egy végtelen ciklus, ami addig fut, amíg a mikr ovezérlő feszültség alatt van.  A megírt kód h elyessége ellenőrizhető még az Arduinora való fel töltés előtt a Verify gomb megn yomásával, majd utána ha ki lett választva a megfelelő áramköri lap, esetemben  ez az Arduino Uno , és a megfelelő port az Upload go mb megnyomásával már feltölthető a kód, ami azonnal fut.     16   3. ábra - Arduino IDE  2.4. Soros kommunikáció  Soros kommunikáció során a küldött üzenet minden bitje egymás után kerül elküldésre egy soros vonalon keresztül  (4. ábra ) és abban a sorrendben is érkeznek meg a vevőhöz, ahogyan el lettek küldve . Az Arduino Uno USB csatlakozója lehetővé teszi a soros kommunikáció megvalósulását. A kommunikációs csatornán egy időpillanatban mindig csak egy bit halad át, a kommu nikáció sebességét határozza meg az Arduino kód inicializálásakor megadott adatátviteli sebesség. [7]  Arduino kód írása során a Serial osztály segítségével valósítható meg az áramköri lap és a számítógép köz ötti soros kommunikáció, minden típusú Arduino la p rendelkezik legalább egy soros porttal.    4. ábra - Soros kommunikáció3                                                 3 Forrás: Serial and Parallel Data Transmission - Serial communication - Wikipedia      17  2.5. ASCII protokoll  Az ASCII4 kód 128 különböző karakterből épül fel, ami az ango l abc betűit, számokat, írásje leket tartalmaz  (5. ábra ). Az ASCII protokoll egy kérdés -válasz alapú kommunikációs protokol l, ami abból áll, hogy a számító gép ASCII karaktereket h asználva küld el egy parancsot az eszköznek, amelyre majd választ kap az eszköztől. Eszközök konfigurálására, adatok küldésére, azok olvasására használják az ASCII parancskészletet.  A protokollban minden parancs ASCII karakterekből épül fel, minden parancs  egy előtag elválasztó kara kterrel kezdődik és egy záró karakterrel végződik . Minden használt karakter beírható egy számítógép billentyűzetéről.  Az ASCII protokollt először az 1980 -as években vezették be az RS -485 elektronikai szabványon alapuló eszközök k özötti kommunikáció során. [8]  5. ábra - ASCII kódtábla5 Általában három lezáró karaktert használnak:   visszatérítési karakter: a t erminálban az Enter leütése után ez a karakter kerül elküldésre , karakterértéke a 13  (0D) , &lt;CR&gt; formában  gyakran használják , ami a Carriage Return rövidítése, programkódban ’ \r’ formában adható meg                                                  4 American Standard Code for Information Interchange  5 Forrás:  https://www.science buddies.org/cdn/references/ascii -table.png      18   új sor kara kter: ez az &lt;LF&gt; vagyis Line  Feed  karakter, ez a ’\n’ alakban írható le, az ASCII táblázatban kódja 10 (0A)   null karakter: ez a táblázat első eleme,  &lt;NUL &gt; formában használják  [9] 2.6. Érzékelők  A szenzorok olyan eszközök, amelyek eseményeket, változásokat érzékelnek a környezetükben és ezt az információt t ovábbítják  (6. ábra). Az érzékelők a fizikai jelenségeket mérhető villamos digitális jellé alakítják. [6] Az érzékelők statikus jellemzői közé tartozik a mérési tartomány, érzékenység, kimeneti jeltartomány, túlterhelés i tartomány , ismétlőképesség, hibasáv, a dinamikus tulajdonságokhoz sorolható a holtidő, beállási idő, növekedési idő, túllövés. [10]   6. ábra - Érzékelő működési elve6 Az Arduino Uno áramköri laphoz egyaránt csatlakoztatható analó g és digitális érzékelő is, így ennek a köszönhetően az érzékelőrendszerben is megtalálható mindkettő. Ahhoz, hogy egyszerre több szenzort is lehetőség legyen az Arduinohoz kötni szüksé g van egy breadboard -ra (7. ábra). Ennek segítségével egyszerűen módosítható az áramkör, forrasztásmentesen összeköthetőek az elemek  jumperek használatával . Fontos megjegyezni, hogy 5V tápfeszültség esetén,  a csatlakoztatott érzékelők össz áramfelvétele nem haladhatja meg a 200mA értéket .                                                 6 Forrás : https://www.sciencedirect.com/science/article/pii/S2666351121000425#sec2     19   7. ábra – Breadboard  2.6.1.  Akadályelkerülő érzékelő  Az alábbi ábrán látható ( 8. ábra) érzékelő érzékeli egy akadály jelenlétét a szenzor előtt, mindezt infravörös jel has ználatával. A beépített  potencio méte r segítségével állítható az érzékelési tartomány  nagysága . Működési elve:  található benne egy infravörös LED adó és vevőegység, ha az adó által kibocsájtott fény egy akadályba ütközik, akkor az visszaverődik a vevőre, így érzékelve az előtte l évő tárgyakat.   8. ábra - HW-488 érzékelő7  Működési feszültség  3.3V -5V Áramfelvétel  ≥20mA  Működési hőmérsékleti tartomány  -10℃÷50℃ Érzékelési távolság  2cm-40cm  2. táblázat - HW-488 paraméterei                                                  7 Forrás: https://shop.tavir.hu/wp -content/uploads/sen -ir-contact -3.jpg      20  2.6.2.  Analóg hőmérséklet érzékelő  A szenzor  (9. ábra) áll egy NTC8 termisztorból valamint  egy 10k Ω ellenállásból. A termisztor el lenállása a környező hőmérsékletnek megfelelően változik és az ellenállás értéke felhasználható a pillanatnyi hőmérséklet kiszámításához.         9. ábra - HW-498 érzékelő9          3. táblázat - HW-498 paraméterei  2.6.3.  Analóg mágneses Hall érzékelő  A HW -498 ( 10. ábra) szenzor egy kisméretű Hall érzékelő, amit egy állandó mág nes vagy elektromágnes mágneses mezője működtet. A kimenő feszültség a tápfeszültségtől függ és arányosan változik a mágneses mező erősségével. A kimenő feszült ség alapérte lmezetten a tápfeszültség fele (a bemutatott rendszer esetében ez 2.5V körüli érték) , ami a polaritás függvényében változik.                                                  8NTC: Negative Temperature Coefficient  9 Forrás: https://m.media -amazon.com/i mages/I/51mbaAbnQKS.jpg  Működési feszültség  5V Mérési tartomány  -40℃÷125℃ Pontosság  (0℃÷70℃ között)  ±0.2℃ Válaszidő  ~10s     21    10. ábra - HW-495 érzékelő10  Működési feszültség  4.5V -6V Működési hőmérsékleti tartomány  -40℃÷80℃ Áramfelvétel  3.5mA  4. táblázat - HW-495 paraméterei  2.6.4.  Digitál is hőmérséklet érzékelő  A 1-Wire interfész csak egyetlen áramköri kivezetést igénye l a kommunikációhoz, ez a hőmérs éklet érzékelő ( 11. ábra) is ez szerint működik. A mért jelet 12 bitre képes felbontani, ezért maga s a pontossága, használják ipari rendszerekben, termosztatikus vezérlésben.    11. ábra - HW-506 érzékelő11                                                     10 Forrás: https://www.electronics -lab.com/wp -content/uploads/2018/04/hall -effect.jpg  11 Forrás: https://cleste.ro/2739 -superlarge_default/modul -senzor -de-temperatura -ds18b20.jpg      22  Működési feszültség  3V-5.5V  Mérési tartomány  -55℃÷125℃ Pontosság ( -10℃÷80℃ között)  ±0.5℃ Programozható felbontó képesség  9-12 bit  Konverziós idő 12 biten  750ms  Áramfelvétel  1.5mA  5.táblázat - HW-506 paraméterei  2.6.5.  Fényblokkolás érzékelő  A  12. ábra egy fényblokkoló szenzort ábrázol, az érzékelő egyik oldal án egy optikai emitter és kollektor található, a másik oldalán két ellenállás (1 Ω és 33 Ω). Az emitter egy fénysugarat bocsá t ki, ha ez nem jut el a kollektorhoz akk or egy tárgy elzárja a köztük lé vő utat.   12. ábra - HW-487 érzékel ő12  Működési feszültség  3.3V -5V Működési hőmérsékleti tartomány  -25℃÷85℃ Áramfelvétel  30mA  Emitter -kollektor közti távolság  0.2mm  6. táblázat - HW-487 paraméterei  2.6.6.  Hőmérséklet és páratartalom érzékelő  Ez egy digitális érzékelő  (13. ábra), amely egyidőben képes a hőmérséklet és a levegő nedvességtartalmának mérésére , ez annak köszönhető, hogy a szenzor két elemből épül fel: egy                                                 12 Forrás: https://cdn.sh opify.com/s/files/1/2285/0583/products/56_480x480.jpg?v=1608198336      23  kapacitív páratartalom érzékelőből és egy termisztorból . Megtalálható benne egy A/D ko nverter, ami segítségével a mért ér tékek átalakíthatóak .  13. ábra - DHT11 érzékelő13  Működési feszültség  3V-5.5V  Mérési tartomány (páratartalom)  20-90% Mérési tartomány (hőmérséklet)  0-50℃ Pontosság (pá ratartalom)  ±5% Pontosság (hőmérséklet)  ±2℃ Áramfelvétel  1.5mA   7. táblázat - DHT11 paraméterei   2.6.7.  Vonalkövető érzékelő  A vonalkövető szenzor  (14. ábra) működése egy infravörös fény segí tségével valósul meg, pontosabban, hogy a vizsgált felület elnyeli vagy visszaveri a  LED által kibocsájtott infravörös  fényt.   14. ábra - HW-511 érzékelő14                                                 13 Forrás: https://c1.neweggimages.com/productimage/nb640/AXF6D2202080NUOZ024.jpg  14 Forrás: https://shop.tavir.hu/wp -content/uploads/robot -vonalszenzor -1ch-digit-90fok -2.jpg      24   Működési feszültség  3.3V -5.5V  Áramfelvétel  20mA  Működési hőmérsékleti tartomány  -25℃÷75℃ Érzékelési távolság  10mm -12mm  8. táblázat - HW-511 paraméterei  2.7. Asztali alkalmazás  A rends zer felhasználói felülete egy .NET MAUI15 desktop alkalmazás. A .NET MAUI (15. ábra) egy cross -platform keretrendszer, ami használatával natív mobil és asztali alkalmazások fejlesztésére van lehetőség. Ezáltal az al kalmazás futhat Android, iOS, macOS, Windows rendszereken is egyetlen közös kódbázisból. A kód megírása C# és XAML nyelvek használatával történik. [11] A XAML16 egy deklaratív leíró nyelv, ami azért lett létrehozva, hogy a .NET keretrendszer használata közb en megkönnyítse a grafikus felhasználói felületek fejlesztését.   15. ábra - .NET MAUI17                                                 15 MAUI: Multi -platform App UI  16XAML: Extensible Application Markup Language  17 Forrás : https://learn.microsoft.com/en -us/dotnet/maui/media/what -is-maui/maui -overview.png     25  3. A rendszer specifikác iói és architektúrája  A rendszer két fő komponensből épül fel:  1. fizikai rendszer: az Arduino áramköri lap és az érzékelők összekapcsolása  2. asztali alkalmazás: az elkészített felhasználói felület  A rendszer leegysz erűsített vázlata az alábbi ábrán ( 16. ábra) látható:    16. ábra – A rendszer vázlata  A rendszer hard ver része, vagyis a fizikai ren dszer áll egy Arduino Uno áramköri lapból és a hozzá csatlakoztatható  érzékelőkből, a rendszer jelenlegi állapotában azok a szenzorok csatla koztathatóak, amik az Érzékelők fejezetben kerültek bemutatásra. A rendszer másik összetevője, az asztali alkalmazás, ahol a felhasználó dinamikusan tudja konfigurálni a szenzorokat és a kapott adatokat leolvasni.  Az áramköri lap egy USB csatlakozóval van bekötve így azon keresztül kapja meg a működéséhez szükséges 5V tápfeszültséget , valamint a szenzorokat is ez látja el a szükséges feszültséggel.  A 17. ábra mutatja be a rendszer tömbvázlatát, megjelenítve,  a fizik ai összetevőit a rendszernek.     26   17. ábra - Tömbvázlat  A 18. ábrán látható a rendszer, amikor az Arduino Uno áramköri laphoz csatlakoztatva van néhány szenzor, amelyek párhuzamosan  vannak  kötve. További érzékelőket lehet még hozzáadni vagy  ki lehet cserélni az szerint, hogy éppen  melyik szenzor adataira van szükség.  A képen szereplő érzékelők mindegy</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>Arduino, protokoll, érz ékelők,  asztali alkalmazás       Interactive sensor system</t>
         </is>
       </c>
@@ -621,6 +656,11 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>/document/6863114. [Hozzáférés  dátuma: 2023].  [7]  H. Aznaoui, S. Raghay, L. Aziz és A. Ait -Mlouk, „A comparative study of routing protocols in WSN,” International Conference on Information &amp; Communication Technology and Accessibility (ICTA), 2015. [Online]. Available: https://ieeexpl ore.ieee.org/abstract/document/7426884. [Hozzáférés dátuma: 2023].  [8]  H. C. Dongsoo S. Kim, „Adaptive Duty -Cycling to Enhance Topology Control Schemes in Wireless Sensor Networks,” International Journal of Distributed Sensor Networks, 2014. [Online]. Av ailable: https://www.researchgate.net/figure/Geographical -adaptive -fidelity -GAF_fig11_275468645. [Hozzáférés dátuma: 2023].  [9]  „What is OMNeT++?,” 2019. [Online]. Available: https://omnetpp.org/intro/.     49  [10]  W. Yen, C. -W. Chen és C. -h. Yang, „Single go ssiping with directional flooding routing protocol in wireless sensor networks,” 2008. [Online]. Available: https://ieeexplore.ieee.org/abstract/document/4582790. [Hozzáférés dátuma: 2023].  [11]  A. Tsapanoglou, „ResearchGate - Gossiping,” [Online]. Available: https://www.researchgate.net/figure/Gossip -protocol -response -for-a-static -6-nodes -network_fig1_224562599. [Hozzáférés dátuma: 2023].  [12]  J. S. S. M. Grover, „Optimized GAF in Wireless Sensor Network,” Proceedings of 3rd Internationa l Conference on Reliability, Infocom Technologies and Optimization, 2014. [Online]. [Hozzáférés dátuma: 2023].  [13]  „OMNeT++ Simulation Library,” doxygen, 2022. [Online]. Available: https://doc.omnetpp.org/omnetpp/api/index.html. [Hozzáférés dátuma: 2023 ].      50  UNIVERSITATEA SAPIENTIA DIN CLUJ -NAPOCA  FACULTATEA DE ȘTIINȚE TEHNICE ȘI UMANISTE, TÎRGU -MUREȘ  SPECIALIZAREA CALCULATOARE                    Vizat decan                                                                     Vizat director departament   Conf . dr. ing. Domokos József      Ș.l. dr. ing   Szabó László  Zsolt</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>hálózat, protokoll, útválasztás</t>
         </is>
       </c>
@@ -647,6 +687,11 @@
         </is>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>A significant proportion of biological phenomena can be traced back to genetics, which is based on gene sequences. Decoding these gene sequences represents a substantial challenge in the field of biological sciences. According to a bold estimate, this task could potentially engage the scientific community for the next five hundred years.  The aim of my thesis is to implement a simple gene sequence classification algorithm and integrate this algorithm into a software, equipped with a graphical user interface. This may represent a small step toward the solution of decoding gene sequences.  This implemented algorithm performs classification based on similarity data from gene sequence pairs within a larger sequence dataset. This methodology allows us to  simultaneously process large amount of protein sequences and grouping these sequences based on their similarity. This is made possible by working with sparse matrices which eliminates unnecessary operations, such as addition and multiplication with zero. At the same time, this method has significant memory efficiency, because we only store the none zero values.  This method treats the input sequence dataset as a graph. Each protein is assigned a node within the graph, and the initial edges between the nodes are received as input data from the SCOP95 database. These values were created using the BLAST algorithm and they’re form a sparse matrix. This algorithm is a modified form of Markov clustering, in which the two main operations, inflation and expansion, work against each other. Connected subgraphs remaining in the equilibrium state, defining the final result of the clustering. The main parameter of the algorithm is the inflation rate, which determines how much the algorithm separates groups from each other.  The graphical user interface provides the opportunity to perform the classification on the 11,944-element SCOP95 dataset or on its subparts, using various settings and can display these resulting protein groups. Furthermore, from any group, we can select two sequences and observe the results of their alignment, which is implemented using the Needleman-Wunsch algorithm.  The algorithm could process up to one million protein sequences in a few hours, but unfortunately an appropriate real dataset was not available for this purpose.</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>Markov klaszterezés, gráf, ritka mátrix, hatékony algoritmus, bioinformatika, fehérje szekvencia         _____________________________________________________________________________    11  Extras O proporție semnificativă a fenomenelor biologice poate fi urmărită înapoi la genetica, care se bazează pe secvențele de gen</t>
         </is>
@@ -663,6 +708,11 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>The topic of my thesis is the design and implementatio n of a system that makes the management of events of university open days easier and more transparent for both the organizers and participants.  University open days are an annual event aimed at promoting the university among high school students and provid ing insight into its operation for those interested. This is an extremely important process because an outsider can really only get a deeper look into university life here before deciding to apply. There are several tasks involved in organizing an event, s uch as managing information related to the event and participants, which are slow and cumbersome to solve with traditional methods, hence the need for a system that makes the whole process more effortless and faster.  The aim of my thesis is to create a sys tem that offers solutions to the aforementioned problems, using the advantages of two modern frameworks. My system makes it more accessible to transfer information related to events, save participant related data, and create statistics from the existing dataset for the organizers.  The system consists of three parts. I implemented the mobile application using the Flutter framework, which must be installed on users' phones and is platform -independent. Here, depending on their role, users can register, create new events, modify existing events, sign up for events, and generate statistics. In the background, a Spring Boot application runs, which provides access to the data stored in the database and processes and saves the data generated by the mobile applicatio n. The third part is the cloud -based storage provided by Firebase, where I store the images, and the MySQL relational database, where I store all other data.</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>platformfüggetlen, mobilalkalmazás, Flutter, Spring Boot, esemén</t>
         </is>
       </c>
@@ -686,6 +736,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
+          <t>The aim of this work is to implement a low cost, easily accessible digital sound effect unit. The project involves the study of digital signal processing theory, algorithm design and development, and hardware implementation. In the first phase, the studied effects were tested under Python with pre-sampled raw guitar sound files. In the second phase, the algorithms were tested on a self-developed multimedia system with an STM32G491 microcontroller using artificially generated and synthesized signals. The quality of the effects was tested using both objective and subjective methods.</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>digitális jelfeldolgozás, hang effektusok, ARM programozás, Python szimuláció</t>
         </is>
       </c>
@@ -713,6 +768,11 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t>Today, diagnostic methods in medicine are constantly evolving, and we can now apply techniques that were unimaginable before. Among the new possibilities and technological challenges, I aim to find solutions that can help us recognize and treat common cardiovascular diseases more effectively, thereby preventing premature or avoidable deaths.  The main goal of my research is to develop new and advanced diagnostic systems specifically focused on the characteristics of cardiova scular diseases. These systems would enable more accurate and efficient diagnoses during the identification and treatment of these diseases. The foundation of my approach is the utilization of electrocardiography (ECG) signals in medicine. These signals pr ovide precise and detailed information about the heart's electrical activity, making it possible to detect various heart diseases or other abnormalities.  The first step involves preprocessing the signals, applying filtering and other normalization techniqu es. Then, I create an RGB color -channel image, a spectrogram. The spectrogram is a visual representation that shows the frequency spectrum of the signal over time. Different shades of color in the channels indicate the intensity of the frequencies, making it easier to analyze the structure and changes of the signal. This process helps extract essential information from the signals and reduces distortions caused by noise.  These images serve as the input dataset for my deep learning -based training software, w hose main task is to recognize four specific diseases. Therefore, my system will be able to identify patterns or subtle details that are not visible to the human eye, providing more accurate diagnoses for people. This can significantly contribute to improv ing healthcare outcomes and enhancing the quality of life.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>mélytanulás,  szív- és érrendszeri betegségek ,  spektrogram, jel  szűrés, betegség diagnózi</t>
         </is>
       </c>
@@ -740,6 +800,11 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>People have always been interested in robots. We often meet robots, not only in science, but also in various areas of life. Although we used to think of human -robot interaction as science fiction (e.g. R2D2 from the movie  Star Wars), nowadays it has become more and more a reality.  Since people's natural communication is through speech, it is not difficult to imagine control through speech. Voice control is an exciting topic that allows robots to be controlled by voice comm ands. There are different methods for this, however, research is still ongoing in the field. This branch of science can lead to many exciting realizations and applications in all areas of life (science, entertainment, industry, etc.).    The purpose of my w ork is to present the advantages and potential of voice control in controlling mobile robots. To this end, I will present an implementation that allows controlling a robot in a simulation environment as well as a physical robot with voice commands. Further  on, you can read about the detailed implementation, the technologies used, as well as the results of the measurements, conclusions and further development possibilities.</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>mobilis  robot, hangvezérlés</t>
         </is>
       </c>
@@ -762,6 +827,11 @@
         </is>
       </c>
       <c r="E14" t="inlineStr">
+        <is>
+          <t>As cryptocurrencies have become more and more widespread these days, cryptocurrency sites and applications have become more popular. It is vital to have tools and platforms that allow trading cryptocurrencies. In the crypto world, these are the decentralised exchanges. These are platforms or applications that allow cryptocurrencies to be exchanged directly between each other without the need for an intermediary. In addition, decentralised exchanges provide a way to supply liquidity to the system. At the same time, they also allow liquidity to be withdrawn. Based on this information, the aim of my thesis is to develop a mobile application that allows users to exchange cryptocurrencies on both Android and iOS. Note that we do not allow users to buy cryptocurrencies, only to exchange them.  In creating my thesis, I needed to learn about the technologies, different principles and solutions that make a decentralised exchange possible. These included different blockchain technologies, smart contracts and the main functionalities of decentralised exchanges.</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>blokklánc, kriptovaluta, decentralizált tőzsde, okos szerződés</t>
         </is>
@@ -776,7 +846,12 @@
           <t>Napjainkra az informatika az egyik leggyorsabban növekvő iparággá nőtte ki magát. Gyakran hónaponta, vagy akár hetente hallunk új technológiák megjelenéséről. Ahhoz, hogy a felsőoktatási intézményekből érkező frissen végzett hallgatók megállják a helyüket egy ilyen dinamikusan növekvő környezetben, elengedhetetlen hogy tanulmányaik alatt jól elsajátítsák a programozás alapjait. Az egyik alapfogalom amelynek mélyebb megértése sok fejtörést tud okozni az e gyetemeken tanuló diákoknak, az nem más mint a rekurzió.   Ezen dolgozatnak és a hozzá társuló vizualizációs szoftvernek az a célja, hogy oktatási  segédeszközként szolgálljon mindazok számára, akik szeretnék mélyebben megérteni a rekurzió jelenségét. A fel használó számára lehetőség nyílik arra, hogy különböző rekurzív függvényeket vizualizáljon a szoftver segítségével. A szokásos vizualizációs eszközöktöl eltérően ez az alkalmazás a lépcsők módszerét használja a rekurzió mélységének vizualizációjához.   A be mutatott szoftver nem csak a tanulni vágyó diákok számára lehet hasznos, hanem mindazok számára is akik kutatni szeretnék a rekurzió jelenségét a vizualizációkon megfigyelhető érdekes mintázatok segítségével.             7  Abstract     Nowadays, IT has become  one of the fastest growing industries. We often hear about new technologies every month or even every week. For recent graduates from academic institutions to succeed in such a dynamic and  fast growing environment, it is essential that they have mastered the basics of programming during their studies. One of the basic concepts that can give university students a lot of headaches is recursion.  The aim of this paper and the accompanying visualisation software is to serve as an educational tool for those who wish to gain a deeper understanding of the phenomenon of recursion. The user is given the opportunity to visualise different recursive functions using the software. Unlike the usual visualization tools, this application uses the method of stairs to visuali ze the depth of recursion.   The presented software can be useful not only for students who want to learn, but also for all those who want to explore the phenomenon of recursion by observing interesting patterns in visualizations.             8  Tartalomjegyzék : 1.Beve zető ................................ ................................ ................................ ................................ ............  12 2.Elméleti megalapozás  ................................ ................................ ................................ .........................  12 2.1. A rekurziótörténete  ................................ ................................ ................................ .....................  13 2.2. Rekurzió a matematikában  ................................ ................................ ................................ ..........  14 2.3 Rekurzió a természetben  ................................ ................................ ................................ ..............  15 2.4 Rekurzió a programozásban  ................................ ................................ ................................ .........  16 2.5 Ciklus VS Rekurzió  ................................ ................................ ................................ .....................  17 2.6 A rekurzió oktatása  ................................ ................................ ................................ ......................  19 3.Hasonló alkalmazások és munkák  ................................ ................................ ................................ .......  20 3.1. VisuAlgo  ................................ ................................ ................................ ................................ .... 20 3.2.Sort Visualizer  ................................ ................................ ................................ .............................  21 3.3 Reku rzió kutatása a Sapientia egyetemen  ................................ ................................ .....................  23 4.Szoftver tervezése és kivitelezése  ................................ ................................ ................................ .......  25 4.1 Felhasználói követelmények  ................................ ................................ ................................ ........  25 4.2 Rendszer követelmények  ................................ ................................ ................................ .............  28 4.2.1. Funkcionális követelmények  ................................ ................................ ................................  28 4.2.2. Nem funkcionális követelmények  ................................ ................................ .........................  29 4.3 A rendszer architektúrája  ................................ ................................ ................................ .............  30 4.4 Függvény kiválasztása  ................................ ................................ ................................ .................  31 4.5 Függvény megírása  ................................ ................................ ................................ ......................  32 5. Szo ftver bemutatása  ................................ ................................ ................................ ...........................  34 5.1 Oldalak bemutatása  ................................ ................................ ................................ ......................  34 5.2 Megírt függvények vizualizálása  ................................ ................................ ................................ .. 37 5.2.1 Faktoriális függvény ................................ ................................ ................................ ..............  37 5.2.3 Egy szám páros vagy páratlan hatványa  ................................ ................................ .................  38 5.2.3 Fibonacci függvény  ................................ ................................ ................................ ...............  39 5.2.4 Hanoi tornyai függvény  ................................ ................................ ................................ .........  41 5.2.5 Ackermann függvény  ................................ ................................ ................................ ............  42 5.2.6 Hofstadter Female -Male függvény  ................................ ................................ ........................  44 6.Kihívások a fejlesztés során  ................................ ................................ ................................ ................  45 6.1 Dinamikus string tömb kompilálása  ................................ ................................ .............................  45 6.2 A vizualizációk láthatósága  ................................ ................................ ................................ ..........  48 9  7.Összefoglaló  ................................ ................................ ................................ ................................ .......  49 8.Továbbfejlesztési lehetőségek  ................................ ................................ ................................ .............  50 Irodalomjegyzék  ................................ ................................ ................................ ................................ .... 51                           10   Ábrák jegyzéke :    2.1.ábra :Fibonacci számsorozat (Forrás:[9])   2.2 ábra:  Összeadás és szorzás rekurzív képletek (Forrás:[1])  2.3 ábra : Ackermann képlete (Forrás:[ 2]) 2.4 ábra:  Arany spirál (Forrás:[ 3]) 2.5 ábra : Rekurzív brokkoli (Forrás:[ 10])  2.6. ábra : Aranymetszet a természetben (Forrás:[ 11]) 2.7 ábra : Hanoi tornyai rekurzív implementációja  2.8. ábra : Hanoi tornyai iteratív megvalósítás  2.9. ábra : Hanoi tornyai iteratív megvalósítás  3.1. ábra :VisuAlgo Fibonacci(5) értékre (Forrás:[ 5]) 3.2.ábra : QuickSort a Sort Visualizer programban (Forrás:[ 12]) 3.3.ábra : Merge Sort a Sort Visualizer programban (Forrás:[ 12]) 3.4. ábra:  Rekurzió lépcsőzetes ilusztrációja (Forrás:[ 8]) 4.1. ábra:  Use case diagramm  4.2. ábra : Activity diagramm  4.3. ábra:  Rendszer architektúra  4.4. ábra:  Szekvencia diagramm függvény választ ásnál  4.5. ábra : Szekvencia diagramm függvény írásnál  5.1. ábra:  Az alkalmazás főoldala és a választó ablak  5.2. ábra:  Főoldal részlet a létrehozott szövegdobozzal  5.3. ábra : Nézet a saját kód megírásához  5.4. ábra : Szövegdobozok generálása  11  5.5. ábra:  A kód megírásának folyamata  5.6. ábra : Faktoriális függvény  5.7.ábra : Hatványozás, indirekt rekurzió  5.8. ábra : Fibonacci függvény  5.9. ábra : Fibonacci függvény, szintek megjelölve  5.10. ábra : Hanoi tornyai  5.11.  ábra:  Ackermann függvény (2,4) értékekre  5.12. ábra : Ackermann függvény (2,20) értékre  5.13. ábra:  Ackermann függvény (3,4) értékre  5.14. ábra:  Hofstadter Female -Male függvény 7 -es értékre  5.15. ábra: Hofstadter Female -Male függvény 25 -ös értékre  6.1. ábra : Reflexióhoz szükséges osztályok  6.2. ábra : Main meghívása a dinamikusan futtatott objektumból  6.3. ábra:  Objektum létrehozása stringek segítségével  6.4. ábra : Vonal meghúzása a kezdet és a végpont közé  6.5. ábra : Közelítés a vizualizáción            12  1.Beve zető   A rekurzió egyike azon  programozásban használt  fogalmaknak, amely ek sok fejtörést okoznak a liceumokban, illetve az egyetemeken tanuló diákoknak.  A tapasztalat azt mutatja, hogy a rekurzió programkód alapú elemzését a legtöbb, programozási készségeit tekintve kezdő diák, nehézk esnek találja.   Ezen okból kifolyólag, napjainkra már nagyon sok segédeszköz elérhető számítógépes szoftverek, illetve az online térben weboldalak formájában , amelyek arra hivatottak, hogy segítsék a diákokat a rekurzió elsajátításában. Általában ezek a segédeszközök a rekurzió vizualizálásával foglalkoznak, a legtöbb esetben egy fa struktúrát hozva létre , ahol a fának a levelei a rekurzív hívásokat szemléltetik.  A fa struktúra által való vizualizációnak viszont van egy eléggé szembetűnő gyengesége. A viz ualizáció jól működik kisebb értékekre, viszont ahogy növekedik a bemeneti adatok értéke, egyre nehezebbé válik a vizualizáció értelmezése.   Ennek okán született meg az a gondolat, hogy hozzunk létre egy olyan oktatási, illetve kutatási  eszközt, amely más szemszögből közelíti meg a rekurzió vizualizálását. Az általam készített szoftver a hagyományos fa struktúra helyett, egy koordináta rendszerben ábrázolja a rekurzív függvényeket , ezáltal könnyebbé téve annak megértését, hogy a rekurzív hívások milyen mély ségeket járnak be mielőtt visszatérnek az eredeti hívó füg gvényhez.  Ezen vizualizációs módszer a bemeneti adatok növelésén kívül, lehetővé teszi különböző mintázatok ismétlődésének a megfigyelését bizonyos függvényeknél, megfelelő felületet nyújtva  ezáltal  azok számára is akik nemcsak megérteni, hanem kutatni is szeretnék a rekurzió jelenségét .  2.Elméleti megalapozás   A rekurzivítás mint fogalom, az életünk számos területén felbukkan. A rekurzió megfigyelhető például a természetben és a matematikában is. K étségtelen viszont, hogy a rekurzió fő felhasználási területe nem más mint az informatika.  Tekintsük át most röviden ezeket a területeket.  13  2.1. A rekurzió története   Amikor a rekurzióra gondolunk, valószínű, hogy első meggondolásra a modern kor számítógépei és az ezekre megírt rekurzív programkódok jutnak eszünkbe. Nem sokan gondolnák, de rekurzív definiciók már az ókori és középkori matematikában is megjelentek. Ezen definíciók egyik legismertebb példája a Fibonacci számsorozat mely et a 13. -ik században Leonardo di Pisa jegyzett fel . A Fibonaccihoz hasonló számsorozatok már az időszámításunk előtti 700 -as évektől megtalálhatók különböző egyiptomi, görög és szanszkrit iratokban  [1]. A Fibonacci számsorozat megadható az alábbi rekurzív  kapcsolattal :  2.1 ábra . Fibonacci számsorozat [ 9]  A 19. -ik század közepére megnőtt az érdeklődés a rekurzió iránt, és a függvénydefiníciók egyik módozataként kezdték használni. Ebben az időszakban például Grassman és Pierce rekurzív definíciókat adott az összeadás, illetve a szorzás műveleteknek  [1].  2.2 ábra . Összeadás és szorzás rekurzív képletek[1]  A 20. -ik sz ázad elején egy a Thoralf Albert Skolem által kiadott cikk nagy befolyással volt a rekurzió számítástechnikai elméletének fejlődésére. Ezen cikk tartalmaz egy leírást olyan függvénekről, amelyeket napjainkban primitív rekurzív függvényeknek nevezünk [1]. Skolem, illetve a későbbiekben Hilbert, Bernays és Ackermann munkássága nagyban hozzájárult a rekurzió számítástechnikai felhasználásának megs zületéséhez.  14  2.2. Rekurzió a matematikában    Amint azt már az előző alpontban is megemlítettük, a matematika volt az a tudományág, amely elsőként használta valamilyen formában a rekurzivítás fogalmát [1]. A matematikában a rekurzió egy ik klasszikus p éldája a faktoriális függvény amely kijelenti, hogy n ! = n * (n -1)!ahol n egy po zitív ternmészetes szám kell hogy legyen. Ez a rekurzív folyamat egészen addig folytatódik amíg az (n -1) egyenlő nem lesz 0 -val, ugyanis a 0 ! = 1. Ha egy programo zásban használatos kifejezést szeretnénk használni, a 0 ! az algoritmus meg állási feltételének felel meg.   A matematikában egymásba ágyazott rekurzióra is találunk példákat. Megemlíthetnénk például az Ackermann függvényt, mely a nevét a felfedezőjéről, Wilhelm Ackermannról ka pta. Az Ackermann függvény a,  teljesen kiszámítható függvények közé tartozik, viszont nem primitív rekurzív. Az idők során nagyon sok változata elterjedt, melyek közül az egyik legismertebb az Ackermann -Péter függvény, amely a következőképpen definiálható [2]:  2.3 ábra . Ackermann képlete [2]   Egy másik klasszikus példa amírő l bővebben szeretnénk beszélni ebben az alpontban, az nem más, mint a már említett Fibonacci szá msorozat. Ez a számsorozat a végtelenségig növelhető, de  vegyük most csak  az első  tíz elemét : 0, 1, 1, 2, 3, 5, 8, 13, 21, 34, 5 5.  Az n. -ik Fibonacci szám a következő rekurzív képlettel írható fel: F(n) = F(n -1) + F(n -2) ahol az n egy pozitív természetes szám, amely nagyobb mint 1. Első látásra ez a számsorozat lehet, hogy nem túlságos an érdkefeszítő, de figyeljük meg egy kicsit, hogy mi történik akkor, ha minden egyes számot elosztuk az előtte található Fibonacci számmal. Ha ezt megtesszük a következő számsorozatot kapjuk : 1/1, 2/1, 3/2, 5/3, 8/5, 13/8, 21/13, 34/21 , 55/34. Ezen os ztások eredményei : 1, 2, 1.5, 1.667, 1.625, 1.615, 1.619, 1.617. Megfi gyelhető, hogy ahogy a számok növekednek, az osztások eredményei egyre inkább közelítenek az 1,618033988749 895-ös 15  számhoz, ami nem más mint az aranymetszet. A 2.4-es ábrán az aranymetszet al apján megrazolt aranyspirál látható. Az aranymetszet, többek között a természetben is megfigyelhető. [3]    2.4 ábra.  Arany spirál [3]  2.3 Rekurzió a természetben    A rekurzivítás meglepően sok formában fellelhető a természetben. Rekurzív jellegeket figyelhetünk meg például hegyek, felhők és folyók elágazó szerkezetében, de még az állati bőr mintázataiban is.  A növényvilágban is számtalan példát találunk, amikor egy növény önmagára hasonlító mintázatokat mutat, a nagyobb forma mitha saját magának kise bb változatait hordozná magában. Természetesen a természet korlátozva van a rekurziót tekintve, ezek a kisebb formák nem zsugorodnak össze a végtelenségig [4]. Ezen növények ékes példája, az úgynevez ett Romanesco brokkoli ami a 2.5 -ös ábrán látható.   A term észetben  az önhasonló alakzatokon kívül megfigyelhető még az előző alcímben fejtegetett aranymetszet jelenléte is.  Ez a szabályosság megfigyelhető külünböző virágok szirmainak , illetve a napraforgóvirág megvainak elhelyezkedésében.  16                                  2.5 ábra  Rekurzív brokkoli [10]                             2.6. ábra  Aranymetszet a természetben [11] 2.4 Rekurzió a programozásban    Ezen alcím alatt a rekurzió fő felhasználási területéről fogunk beszélni, ami nem más mint a számítógépes programozás. A programozásban azt a folyamatot nevezzük rekurziónak, amikor egy függvény önmagát hívja meg, egy feladat megoldásának érdekében.  A rekurzió alap kérdéséül az szolgál, hogy hogyan lehet egy feladatot visszavezetni egyetlen egyszerűbb feladatra.  Ha egy aDr. Kátai Zoltán által használt hasonlattal  szeretnénk élni a rekurzív hívásokat tekintően, mondhatnánk azt is, hogy a függvény amel yből kiindul a rekurzív hívás, létre hoz egy klónt saját magáról  és a feladatának nagy részét át adja ennek a klónnak. Ez a klón ugyan azt az alapelvet követi, így létrehoz magáról egy következő klónt. Ez a folyamat nem folytatódik a végtelenségig, mivel  a függvényhívás feltételes kell legyen, ami azt jelenti, hogy van egy megállási feltétele, ami ha beteljesül, többé már nem jön létre egy következő klón , hanem vissza térítődnek az értékekek  az előző klónokhoz . Típusait tekintve a rekurziót két  különböző ré szre bonthatjuk : direkt vag y közvetlen rekurzió, illetve indirekt vagy közvetett rekurzió. Direkt rekurziónak nevezzük azt amikor egy függvény saját magára hivatkozik amikor függvényhívást végez. Indirekt rekurziónak azt nevezzük amikor egy rekurzív függvé ny nem saját magát hívja meg, hanem egy másik függvényt, amely szintén nem önmagát hívja meg, hanem azt a fügvényt aki őt meghívta.   17  2.5 Ciklus VS Rekurzió    A rekurzió ellenpárja az iteratív ciklusos megoldás.  Annak ellenére, hogy ellenpároknak hívjuk őket , a rekurz ív függvényeket ciklussá lehet alakítani és ugyan így az iteratív ciklusokat rekurzióvá. Elmondható, hogy az iteráció  gyorsabb a rekurziónál, mivel a rekurzió esetében függvényhívás történik, ami meg növeli a futási időt. A rekurziónak eg y másik hátránya az, hogyha a rekurzió túl nagy mélységeket jár be, akkor feltelhet a verem.   De miért éri meg akkor rekurziót használni ? A rekurzi ó ereje nem a gyorsaságában, hanem az eleganciájában rejlik. Sok esetbe n a rekurzióval megoldott feladat tömörebb és jobban olvasható mint az iterációs ellenpárja. Ennek egyik ékes példája a Hanoi tornyai nevű feladvány. A Hanoi tornyai rekurzív implementálása nagyon rövid és elegáns . Lásd 2.7  ábra.    2.7 ábra . Hanoi tornyai rekurzív implementációja  Ezzel ellentétben, Hanoi tornyai iteratív implementálása még sok informatika tanárt is gondolkodóba ejtene. Fi gyeljük meg egy kicsit a 2.8 -as és 2.9 -es ábrán ezt a megvalósítást is, a fentiekben látott bemeneti értékekre.  Ezeken  az ábrákon megfigyelhető, hogy Hanoi tornyai iteratív megvalósítása több mint tizszer annyi kódolást igényel mint a rekurzív megvalósítás . 18   2.8. ábra  Hanoi t ornyai iteratív megvalósítás    2.9. ábra Hanoi t ornyai iteratív megvalósítás   Ezen két megvalósításból  láthatjuk, hogy a a re kurziót igenis megéri használni, mert a példaként említett Hanoi tornyai probléma rekurzív megvalósítása sokkal  érthetőbb,  rövidebb  és elegánsabb mint az iterációval megírt ellenpárja . 19  2.6 A rekurzió oktatása    A reku rzív programozás egyike azon témáknak, amelynek tanítása során az oktatók előszeretettel nyúlnak bizonyos oktatási segédeszközökhöz. A legtöbb ilyen segédeszköz  a látást célozza meg mint felhasználandó érzéket, mivel felismerték, hogy a látás fontos szerep et játszik az új fogalmak elsajátításában. Ezen felismerés különböző kutatási vonalakat nyitott meg a rekurzió oktatását tekintve, mint például a rekurzió vizuális analógiái, vagy a programok eredményének animálása [13].   Az analógiákat tekintve az oktatók és kutatók túlnyomó többsége ugyan azokkal a példákkal áll elő, ilyen például a rekurzív mintázatokat mutató brokkoli, a fák ágai, illetve az egymással szembe helyezett tükrök tükröződései.  A kutatások során nem csak tárgyakat, hanem külöböző rekurzív foly amatokat is megvizsgáltak mindennapi példák segítségével. Megvizsgálták például azt, hogy hogyan értelmezik a gyerekek az egymás mellé helyezett dominók eldőlését [13].  A 12 év körüli és idősebb gyerekek esetében a dominók eldőlésének leírásában megfigyelh ető a rekurzív gondolkodás, mivel a gyerekek megfigyelték, hogy minden dominóelem eldőlését az előtte levő dominó okozta. Ezzel ellentétben, a 12 évnél fiatalabb gyerekek esetében a leírás inkább iteratív jellegű, eldől egy dominó, majd a következő, egésze n ameddig egy se marad állva[13].   A rekurzi ót kutató személyek  számos javaslatot tettek a rekurziós gráfok használatára, annak érdekében, hogy gyorsítani lehessen ezáltal a kezdőknél a rekurzió elsajátításának a folyamatát. Ezen gráfok lehetővé teszik a d iákok számára a függvényhívások kiértékelésének a követését  és mélyebb elemzését . Ha ezen gráf egy bináris fa, akkor minden egyes csomópont ugyan azt a függvényhívást jelenti [13].     20  3.Hasonló alkalmazások  és munkák    3.1. VisuAlgo     A “VisuAlgo” egy interneten el érhető weboldal, amely animációk segítségével próbál vizualizálni különböző adatstruktúrákat és algoritmusokat .[5] Az oldal segítségével többek között képesek vagyunk vizualizálni rendezéseket, láncolt listákat, hasító táblákat, és nem utolsó sorban, a rekurziót .   3.1 ábra  VisuAlgo Fibonacci(5) értékre [5]  A „VisuAlgo” a rekurziót egy fa struktúra segítségév el vizualizálja, ahogy ezt a 3.1 -es ábra is mutatja.  Az oldal bal alsó sarkában található egy mező, amely segítségével ki tudjuk választani, hogy mit i s szeretnénk vizualizálni. A 3.1 -es ábrán például a Fibonacci számok vizualizációja van kiválasztva n =5 értékre. A Fibonacci számokon kívül további 19 függvé ny vizualizációjára ad lehetőseget a program, amelyeknek forráskódját ki is vetíti egy szövegdobozba. Lehetőség van saját kód kipróbálására is, ugyanis a lenyíló listában az utoló elem a „Custom code” nevet viseli, ha ezt kiválasztjuk, akkor megírhatjuk a szövegdobozban a saját kódunkat JavaScript programozási nyelv segítségével.   21   Ahogy a 3.1 -es ábra jobb oldalán is megfigyelhető , a fa struktúra levelei különböző színeket  vesznek fel. A legalsó szinteken található levelek a zöld színt veszik fel, ezek a le velek azokat a rekurzív hívásokat jelölik, amikor a megállási feltétel igaznak bizonyul és elkezdődik az értékek visszatérítése.  A levelek fehér színűek amikor egy hívás az adott n értékre először történt meg.  A program világoskék színnel jelöli azokat a h ívásokat amikor  az n bemeneti értékre a hívás egyszer már feldolgozásra került [5]. Vegyük például az ábra alapján a Fibonacci(2) – es értéket. Mivel a bináris fa balról jobbra kerül bejárásra, a fa leginkább baloldalán található kettes értékű levél fehér színnel van jelölve, míg az utána következő összes többi kettes értékű levél kék színnel lett jelölve.   Következtetésként kijelenthető, hogy a “VisuAlgo” hasznos  segédeszköznek bizonyu l a rekurzió vizualizálását illetően, és mint diákok, mint tanárok hasznát vehetik akik többet szeretnének tudni a rekurzióról.   3.2.Sort Visualizer    A “Sort Visualizer” szintén egy interneten elérhető weboldal, amely rendezési algoritmusok vizualiz álására specializálódott. A 16 darab vizualizálható a lgoritmus közül van néhány amely előszeretettel alkalmazza a rekurziót. Ilyen algoritmus például a quicksort, illetve a merge sort. Ezen alpont keretén belül szeretnénk bemutatni ezeknek a vizualizációját a program segítségével.   A quicksort vagy g yorsrendezés a divide et imp era elv alapján működik. A rendezendő listát egy pivot segítségével két különálló részre bontja, majd erre a két új listára külön külön ismét meghívja a gyorsrendezést. [6] Ez a rekurzív folyamat addig folytatódik, amíg az átadott lista hossza kisebb vagy e gyenlő nem lesz 1 -el. Nezzük meg hogyan is vizualizálja ezt a rendezést a program. Lásd 3.2  ábra.     22   3.2 ábra . QuickSort  a Sort Visualizer  programban  [12]  Első lépéskent a rendező algoritmus végig iterál a listán, és elkezdi kicserélni a kiválasztott pivot elem két oldalán levő értékeket. Azokat az elemeket amelyek kisebbek mint a pivot a bal oldalára rendezi, míg azokat amelyek nagyobbak a jobb oldalára. Ez után következik az algoritmus rekurzív része , amit az előbbiekben már ismertettünk. Megfigyelhe tő hogy a lista legeleje kerül leghamarabb rendezésre, ez annak köszönhető, hogy az oszd meg és uralkodj módszert használó algoritmus, először a pivot bal oldalán levő listára hívja meg rekurzívan a quicksortot.   A következőkben figyeljük meg egy kicsit, h ogyan figyelhető meg a rekurzió a merge sort esetében.  Lásd 3.3  ábra.   3.3 ábra . Merge Sort a  Sort Visualizer  programban  [12] 23    A merge sort a quicksorthoz hasonlóan az oszd meg és uralkodj módszert alkalmazza. A rendező algoritmus rekurzívan felosztja a bemeneti listát, egészen ameddig az átadott lista csupán egyetlen elemet tartalmaz. Amint ez megtörténik, a részsorozatok összevonódnak és rendezésre kerülnek. Az algoritmus fokozatosan összevonja a részlistákat, egészen addig amíg egyetlen rendezett lista  marad a végén.[7]  Az összevonás folyamata a 3.3 -as ábrán is nagyon jól megfigyelhető.   Összességében kijelethető, hogy a “Sort Visualizer” is sokat tud segíteni egy felhasználónak a rekurzió megértésében.      3.3 Rekurzió kutatása a Sapientia egyetemen     A Sapientia Erdélyi Magyar Tudományegyetem Marosvásárhelyi karán a 2008 -as évben Dr. Kátai Zoltán vezetésével elvégzésre került egy kutatás, amelynek keretén belül egy úgynevezett többérzékelős módszert probáltak ki a rekurzió oktatására.  Ezen alpontban bemutatásra kerül ez a kutatás, amely a [8] –as cikkben található, és az ehhez fejlesztett szoftver is bemutatásra kerül.   A kutatás egyik részeként megkértek az egyetem diákjai közül néhányat, hogy játszák el egy rekurzív függvény futási f olyamatát. Az első diák szemléltette a main függvényt, míg a többiek  a rekurzív függvény példányait szemléltették. Amikor egy a cikk által rekurzív szereplőnek megnevezett diák meghívásra került, a szereplő kilépett a meghívója mögül és elkezdte elemezni az általa kapott feladatot. Két lehetősége volt, követi a rekurzív forgatókönyvet, vagy követi a triviálisat , ami a megállási feltétel teljesülését jelentette. Ha az első lehetőséget választotta, akkor meghívta a társát  és saját magát felfüggesztette amíg nem kapott választ a hívásra. A legutolsó diáknak a triviális forgatókönyvet kellett választania, mivel akkor teljesült a megállási feltétel. Neki az volt a dolga, hogy a részfeladatának az eredményét átadja a hívójának, aki ennek hatására felébredt a felf üggesztett állapotából és ugyan ezt a 24  műveletet elvégezte.  Ez a folyamat addig folytatódott amí a main függvényt szemléltető diák megkapta az eredményt [8].   Ezen kísérlet segített a diákoknak jobban megérteni, hogy hogyan is működik a rekurzió.  A néző diá kok megérthették belőle a rekurzív folyamatok működését, míg azok a diákok aki eljátszodták folyamatokat, kinetikus módon is memorizálták a rekurziót, a műveletekhez kapcsolódó mozgások által  [8].  A kutatás egy másik fontos része , egy a rekurzió oktatására  kifejlesztett szoftver kipróbálása volt.  Ezen szoftver audio -vizuális eszközökkel próbálja megértetni a felhasználóval a rekurzivítást. A rekurziót a program lépcsőzetesen vizualizálja, ezáltal minden egyes rekurzív hívás egy úgynevezett emelete t hoz létr e . Lásd 3.4 -es ábra. Minden egyes emeleten a vizualizációhoz egy zenei bejátszás is társul, melynek hangmagassága az emelet magasságának függvényében növekszik.   3.4 ábra.  Rekurzió lépcsőzetes ilusztrációja  [8]  A kísérletben 43 nagyjából azonos képességekkel rendelkező  első éves  diák vett részt . A diákokat két csoportra osztották, 23 -at közűlük a tradicionális módszerekkel tanítottak, míg a megmaradt 20 diáknál az előbbiekben említett módszereket használták a rekurzió oktatására. Az utólag os teszt eredmények azt mutatták, hogy akiket a többérzékelős módszerekkel tanítottak, jobban teljesítettek mint azok a társaik akik tradicionális oktatásban részesültek. [8] Ezen kísérlet ékes példája annak, hogy a különböző segédeszközök könnyebbé tudják tenni a rekurzió megértését és tanulását.  25  4.Szoftver tervezése és kivitelezése    A dolgozat ezen részében bemutatásra kerül a szoftver, amelyet a rekurzió lépcsőzetes módszerrel való vizualizálásához fejlesztettem. Az alkalmazás  egy Windows Form aplikáció amely  C# programozási nyelven íródott és a .Net keretrendszer 4.7.2 - es verzióját használja.  A szoftver lehetőséget ad rekurzív függvények illetve rekurzív eljárások vizualizációjára.  A különbség a két fogalom között az, hogy míg a rekurzív függvény vissza  térít egy eredményt a hívójához, addig a rekurzív eljárás csupán elvégez egy feladatot anélkül, hogy bármit is vissza térítene a hívójához. Természetesen a rekurzív eljárásokban is jelen van a megállási feltétel [14].  4.1 Felhasználói követelmények    Az szoftver  elindítása  után, a felhasználó előtt egyenesen az alkalmazás fő ablaka jelenik meg. Ezen a fő ablakon történik meg a rekurzív függvények vizualizálása egy koordináta rendszerben. Az elindítás pillanatában a fő ablakon három gomb jelenik meg, a “Choose File”, “Run”, illetve a “Write own c ode” elneve zésekkel.   A “Choose File”  gomb lenyomásávál egy különálló ablakban megnyílik  a projektnek a könyvtára, ahol a felhasználó ki tudja választani az előre megírt rekurzív jellegű függvények közül azt amelyiket vizualizálni szeretné. Minden egyes függvény különálló .txt kiterjesztésű fájlokban van megírva, a felhasználónak csak annyi a  feladata, hogy kiválassza a fájlt és megnyomja az „Open” gombot.  Miután ki lett választva a függvény, a szoftver átvizsgálja a kapott függvényt és megállapítja, hogy hány paraméter megadására van szüksége az adott függvénynek. Annak fügvényében, hogy ez a  szám mennyi, a szoftver kigenerálja azokat a szövegdobozokat ahova a felhasználó be tudja írni az értékeket. Például, ha kiválasztottuk a faktoriális függvényt, aminek meghívásához egyetlen paraméterre van szükség, a program egyetlen szövegdobozt fog létr ehozni ahova be tudjuk írni ezt az értéket.   A “Run” gomb lenyomásával tudjuk elindítani az előző lépésben kiválasztott függvény vizualizációját. Ha sikeres volt a program lefuttatása, akkor az ablak gombok alatti üres részében megjelenik a függvény vizual izációja. Abban ez esetben ha nem választottunk még ki egyetlen 26  függvényt sem amit vizualizálni szeretnénk és megnyomjuk a “Run” gombot, a szoftver egy üzenetet közvetít a felhasználó felé, hogy előbb válasszon ki egy függvényt és csak azután nyomja meg a “Run” gombot. Hasonl ó figyelmeztetést kapunk abban az esetben  is ha a kigenerált szövegdobozokba egy érvénytelen karaktert ütünk be. Minden beütött érték szám kell hogy legyen, ennek értelmében ha egy betüt adunk meg paraméterként, a szoftver figyelmeztet,  hogy a megadott paraméter nem érvényes.   4.1 ábra.  Use case diagramm   27   A “Write own c ode” gomb megny omásával egy új ablak fog megnyílni a felhasználó előtt. Ebben az új ablakban lehetőség nyílik arra, hogy a felhasználó egy saját maga által szerkesztett kódot is levizualizáljon. Az ablak megnyitásakor még nincs kigenerálva az a szövegdoboz , ahova a felhasználó beírhatja a saját C # nyelven megírt kódját, viszont az ablak legtetején talál két gombot, név szerint a “Direct Recursion” és az “Indirect Recursio n” gombokat. Ezek a gombok azért szükségesek, hogy a felhasználó ki tudja választani a kívánt rekuzió típusát. Ha a felhasználó a “Direct Recursion” gombot n yomja meg akkor egyetlen szövegdoboz kerül kigenerálásra, mivel a közvetlen rekurzióhoz csak egyetl en megírt függvényre van szükség. Ha az “Indirekt Recursion” gombot nyomja meg a felhasz náló, két szövegdoboz generálódik ki, mivel a közvetett rekurzióhoz legalább két függvényre van szükség. Az előzőekben feldolgozott fájl kiválasztásos módszernél azért nem volt szükség hasonló műveletre, mivel a szoftver a beolvasott szöveges fájl alapján el tudja dönteni a rekurzió típusát.   4.2 ábra . Activity diagramm  28   Miután ki lett generálva a megfelelő számú szövegdoboz a függvények beírásához, a felhasználó neki kezdhet kódolni. A szövegdoboz első sorába a felhasz náló az úgynevezett “method signaturet” kell hogy beírja, amely tartalmazza a függvény nevét, típusát, és  a függvény paramétereit. Miután az első sor be lett írva, enter gomb lenyomására a program meghatározza, hogy hány paramétere van a megírt metódusnak, amely után kigenerálja a megfelelő mennyiségű szövegdobozt a paraméterek értékeinek megadására. Abban ez  esetben ha hibát vétettünk ezen műveletek közben, például nem adtunk meg megfelelő mennyiségű paramétert az első sorban, de már kigeneráltuk a paraméterek szövegdobozait, nyomjuk meg a “Clear all” elnevezésű gombot, mely vissza állít mindent az eredeti ál lapotára.Ezután előlről kezdhetjük az előbbiekben vázolt műveleteket. A füg</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Nowadays, IT has become  one of the fastest growing industries. We often hear about new technologies every month or even every week. For recent graduates from academic institutions to succeed in such a dynamic and  fast growing environment, it is essential that they have mastered the basics of programming during their studies. One of the basic concepts that can give university students a lot of headaches is recursion.  The aim of this paper and the accompanying visualisation software is to serve as an educational tool for those who wish to gain a deeper understanding of the phenomenon of recursion. The user is given the opportunity to visualise different recursive functions using the software. Unlike the usual visualization tools, this application uses the method of stairs to visuali ze the depth of recursion.   The presented software can be useful not only for students who want to learn, but also for all those who want to explore the phenomenon of recursion by observing interesting patterns in visualizations.             8  Tartalomjegyzék : 1.Beve zető ................................ ................................ ................................ ................................ ............  12 2.Elméleti megalapozás  ................................ ................................ ................................ .........................  12 2.1. A rekurziótörténete  ................................ ................................ ................................ .....................  13 2.2. Rekurzió a matematikában  ................................ ................................ ................................ ..........  14 2.3 Rekurzió a természetben  ................................ ................................ ................................ ..............  15 2.4 Rekurzió a programozásban  ................................ ................................ ................................ .........  16 2.5 Ciklus VS Rekurzió  ................................ ................................ ................................ .....................  17 2.6 A rekurzió oktatása  ................................ ................................ ................................ ......................  19 3.Hasonló alkalmazások és munkák  ................................ ................................ ................................ .......  20 3.1. VisuAlgo  ................................ ................................ ................................ ................................ .... 20 3.2.Sort Visualizer  ................................ ................................ ................................ .............................  21 3.3 Reku rzió kutatása a Sapientia egyetemen  ................................ ................................ .....................  23 4.Szoftver tervezése és kivitelezése  ................................ ................................ ................................ .......  25 4.1 Felhasználói követelmények  ................................ ................................ ................................ ........  25 4.2 Rendszer követelmények  ................................ ................................ ................................ .............  28 4.2.1. Funkcionális követelmények  ................................ ................................ ................................  28 4.2.2. Nem funkcionális követelmények  ................................ ................................ .........................  29 4.3 A rendszer architektúrája  ................................ ................................ ................................ .............  30 4.4 Függvény kiválasztása  ................................ ................................ ................................ .................  31 4.5 Függvény megírása  ................................ ................................ ................................ ......................  32 5. Szo ftver bemutatása  ................................ ................................ ................................ ...........................  34 5.1 Oldalak bemutatása  ................................ ................................ ................................ ......................  34 5.2 Megírt függvények vizualizálása  ................................ ................................ ................................ .. 37 5.2.1 Faktoriális függvény ................................ ................................ ................................ ..............  37 5.2.3 Egy szám páros vagy páratlan hatványa  ................................ ................................ .................  38 5.2.3 Fibonacci függvény  ................................ ................................ ................................ ...............  39 5.2.4 Hanoi tornyai függvény  ................................ ................................ ................................ .........  41 5.2.5 Ackermann függvény  ................................ ................................ ................................ ............  42 5.2.6 Hofstadter Female -Male függvény  ................................ ................................ ........................  44 6.Kihívások a fejlesztés során  ................................ ................................ ................................ ................  45 6.1 Dinamikus string tömb kompilálása  ................................ ................................ .............................  45 6.2 A vizualizációk láthatósága  ................................ ................................ ................................ ..........  48 9  7.Összefoglaló  ................................ ................................ ................................ ................................ .......  49 8.Továbbfejlesztési lehetőségek  ................................ ................................ ................................ .............  50 Irodalomjegyzék  ................................ ................................ ................................ ................................ .... 51                           10   Ábrák jegyzéke :    2.1.ábra :Fibonacci számsorozat (Forrás:[9])   2.2 ábra:  Összeadás és szorzás rekurzív képletek (Forrás:[1])  2.3 ábra : Ackermann képlete (Forrás:[ 2]) 2.4 ábra:  Arany spirál (Forrás:[ 3]) 2.5 ábra : Rekurzív brokkoli (Forrás:[ 10])  2.6. ábra : Aranymetszet a természetben (Forrás:[ 11]) 2.7 ábra : Hanoi tornyai rekurzív implementációja  2.8. ábra : Hanoi tornyai iteratív megvalósítás  2.9. ábra : Hanoi tornyai iteratív megvalósítás  3.1. ábra :VisuAlgo Fibonacci(5) értékre (Forrás:[ 5]) 3.2.ábra : QuickSort a Sort Visualizer programban (Forrás:[ 12]) 3.3.ábra : Merge Sort a Sort Visualizer programban (Forrás:[ 12]) 3.4. ábra:  Rekurzió lépcsőzetes ilusztrációja (Forrás:[ 8]) 4.1. ábra:  Use case diagramm  4.2. ábra : Activity diagramm  4.3. ábra:  Rendszer architektúra  4.4. ábra:  Szekvencia diagramm függvény választ ásnál  4.5. ábra : Szekvencia diagramm függvény írásnál  5.1. ábra:  Az alkalmazás főoldala és a választó ablak  5.2. ábra:  Főoldal részlet a létrehozott szövegdobozzal  5.3. ábra : Nézet a saját kód megírásához  5.4. ábra : Szövegdobozok generálása  11  5.5. ábra:  A kód megírásának folyamata  5.6. ábra : Faktoriális függvény  5.7.ábra : Hatványozás, indirekt rekurzió  5.8. ábra : Fibonacci függvény  5.9. ábra : Fibonacci függvény, szintek megjelölve  5.10. ábra : Hanoi tornyai  5.11.  ábra:  Ackermann függvény (2,4) értékekre  5.12. ábra : Ackermann függvény (2,20) értékre  5.13. ábra:  Ackermann függvény (3,4) értékre  5.14. ábra:  Hofstadter Female -Male függvény 7 -es értékre  5.15. ábra: Hofstadter Female -Male függvény 25 -ös értékre  6.1. ábra : Reflexióhoz szükséges osztályok  6.2. ábra : Main meghívása a dinamikusan futtatott objektumból  6.3. ábra:  Objektum létrehozása stringek segítségével  6.4. ábra : Vonal meghúzása a kezdet és a végpont közé  6.5. ábra : Közelítés a vizualizáción            12  1.Beve zető   A rekurzió egyike azon  programozásban használt  fogalmaknak, amely ek sok fejtörést okoznak a liceumokban, illetve az egyetemeken tanuló diákoknak.  A tapasztalat azt mutatja, hogy a rekurzió programkód alapú elemzését a legtöbb, programozási készségeit tekintve kezdő diák, nehézk esnek találja.   Ezen okból kifolyólag, napjainkra már nagyon sok segédeszköz elérhető számítógépes szoftverek, illetve az online térben weboldalak formájában , amelyek arra hivatottak, hogy segítsék a diákokat a rekurzió elsajátításában. Általában ezek a segédeszközök a rekurzió vizualizálásával foglalkoznak, a legtöbb esetben egy fa struktúrát hozva létre , ahol a fának a levelei a rekurzív hívásokat szemléltetik.  A fa struktúra által való vizualizációnak viszont van egy eléggé szembetűnő gyengesége. A viz ualizáció jól működik kisebb értékekre, viszont ahogy növekedik a bemeneti adatok értéke, egyre nehezebbé válik a vizualizáció értelmezése.   Ennek okán született meg az a gondolat, hogy hozzunk létre egy olyan oktatási, illetve kutatási  eszközt, amely más szemszögből közelíti meg a rekurzió vizualizálását. Az általam készített szoftver a hagyományos fa struktúra helyett, egy koordináta rendszerben ábrázolja a rekurzív függvényeket , ezáltal könnyebbé téve annak megértését, hogy a rekurzív hívások milyen mély ségeket járnak be mielőtt visszatérnek az eredeti hívó füg gvényhez.  Ezen vizualizációs módszer a bemeneti adatok növelésén kívül, lehetővé teszi különböző mintázatok ismétlődésének a megfigyelését bizonyos függvényeknél, megfelelő felületet nyújtva  ezáltal  azok számára is akik nemcsak megérteni, hanem kutatni is szeretnék a rekurzió jelenségét .  2.Elméleti megalapozás   A rekurzivítás mint fogalom, az életünk számos területén felbukkan. A rekurzió megfigyelhető például a természetben és a matematikában is. K étségtelen viszont, hogy a rekurzió fő felhasználási területe nem más mint az informatika.  Tekintsük át most röviden ezeket a területeket.  13  2.1. A rekurzió története   Amikor a rekurzióra gondolunk, valószínű, hogy első meggondolásra a modern kor számítógépei és az ezekre megírt rekurzív programkódok jutnak eszünkbe. Nem sokan gondolnák, de rekurzív definiciók már az ókori és középkori matematikában is megjelentek. Ezen definíciók egyik legismertebb példája a Fibonacci számsorozat mely et a 13. -ik században Leonardo di Pisa jegyzett fel . A Fibonaccihoz hasonló számsorozatok már az időszámításunk előtti 700 -as évektől megtalálhatók különböző egyiptomi, görög és szanszkrit iratokban  [1]. A Fibonacci számsorozat megadható az alábbi rekurzív  kapcsolattal :  2.1 ábra . Fibonacci számsorozat [ 9]  A 19. -ik század közepére megnőtt az érdeklődés a rekurzió iránt, és a függvénydefiníciók egyik módozataként kezdték használni. Ebben az időszakban például Grassman és Pierce rekurzív definíciókat adott az összeadás, illetve a szorzás műveleteknek  [1].  2.2 ábra . Összeadás és szorzás rekurzív képletek[1]  A 20. -ik sz ázad elején egy a Thoralf Albert Skolem által kiadott cikk nagy befolyással volt a rekurzió számítástechnikai elméletének fejlődésére. Ezen cikk tartalmaz egy leírást olyan függvénekről, amelyeket napjainkban primitív rekurzív függvényeknek nevezünk [1]. Skolem, illetve a későbbiekben Hilbert, Bernays és Ackermann munkássága nagyban hozzájárult a rekurzió számítástechnikai felhasználásának megs zületéséhez.  14  2.2. Rekurzió a matematikában    Amint azt már az előző alpontban is megemlítettük, a matematika volt az a tudományág, amely elsőként használta valamilyen formában a rekurzivítás fogalmát [1]. A matematikában a rekurzió egy ik klasszikus p éldája a faktoriális függvény amely kijelenti, hogy n ! = n * (n -1)!ahol n egy po zitív ternmészetes szám kell hogy legyen. Ez a rekurzív folyamat egészen addig folytatódik amíg az (n -1) egyenlő nem lesz 0 -val, ugyanis a 0 ! = 1. Ha egy programo zásban használatos kifejezést szeretnénk használni, a 0 ! az algoritmus meg állási feltételének felel meg.   A matematikában egymásba ágyazott rekurzióra is találunk példákat. Megemlíthetnénk például az Ackermann függvényt, mely a nevét a felfedezőjéről, Wilhelm Ackermannról ka pta. Az Ackermann függvény a,  teljesen kiszámítható függvények közé tartozik, viszont nem primitív rekurzív. Az idők során nagyon sok változata elterjedt, melyek közül az egyik legismertebb az Ackermann -Péter függvény, amely a következőképpen definiálható [2]:  2.3 ábra . Ackermann képlete [2]   Egy másik klasszikus példa amírő l bővebben szeretnénk beszélni ebben az alpontban, az nem más, mint a már említett Fibonacci szá msorozat. Ez a számsorozat a végtelenségig növelhető, de  vegyük most csak  az első  tíz elemét : 0, 1, 1, 2, 3, 5, 8, 13, 21, 34, 5 5.  Az n. -ik Fibonacci szám a következő rekurzív képlettel írható fel: F(n) = F(n -1) + F(n -2) ahol az n egy pozitív természetes szám, amely nagyobb mint 1. Első látásra ez a számsorozat lehet, hogy nem túlságos an érdkefeszítő, de figyeljük meg egy kicsit, hogy mi történik akkor, ha minden egyes számot elosztuk az előtte található Fibonacci számmal. Ha ezt megtesszük a következő számsorozatot kapjuk : 1/1, 2/1, 3/2, 5/3, 8/5, 13/8, 21/13, 34/21 , 55/34. Ezen os ztások eredményei : 1, 2, 1.5, 1.667, 1.625, 1.615, 1.619, 1.617. Megfi gyelhető, hogy ahogy a számok növekednek, az osztások eredményei egyre inkább közelítenek az 1,618033988749 895-ös 15  számhoz, ami nem más mint az aranymetszet. A 2.4-es ábrán az aranymetszet al apján megrazolt aranyspirál látható. Az aranymetszet, többek között a természetben is megfigyelhető. [3]    2.4 ábra.  Arany spirál [3]  2.3 Rekurzió a természetben    A rekurzivítás meglepően sok formában fellelhető a természetben. Rekurzív jellegeket figyelhetünk meg például hegyek, felhők és folyók elágazó szerkezetében, de még az állati bőr mintázataiban is.  A növényvilágban is számtalan példát találunk, amikor egy növény önmagára hasonlító mintázatokat mutat, a nagyobb forma mitha saját magának kise bb változatait hordozná magában. Természetesen a természet korlátozva van a rekurziót tekintve, ezek a kisebb formák nem zsugorodnak össze a végtelenségig [4]. Ezen növények ékes példája, az úgynevez ett Romanesco brokkoli ami a 2.5 -ös ábrán látható.   A term észetben  az önhasonló alakzatokon kívül megfigyelhető még az előző alcímben fejtegetett aranymetszet jelenléte is.  Ez a szabályosság megfigyelhető külünböző virágok szirmainak , illetve a napraforgóvirág megvainak elhelyezkedésében.  16                                  2.5 ábra  Rekurzív brokkoli [10]                             2.6. ábra  Aranymetszet a természetben [11] 2.4 Rekurzió a programozásban    Ezen alcím alatt a rekurzió fő felhasználási területéről fogunk beszélni, ami nem más mint a számítógépes programozás. A programozásban azt a folyamatot nevezzük rekurziónak, amikor egy függvény önmagát hívja meg, egy feladat megoldásának érdekében.  A rekurzió alap kérdéséül az szolgál, hogy hogyan lehet egy feladatot visszavezetni egyetlen egyszerűbb feladatra.  Ha egy aDr. Kátai Zoltán által használt hasonlattal  szeretnénk élni a rekurzív hívásokat tekintően, mondhatnánk azt is, hogy a függvény amel yből kiindul a rekurzív hívás, létre hoz egy klónt saját magáról  és a feladatának nagy részét át adja ennek a klónnak. Ez a klón ugyan azt az alapelvet követi, így létrehoz magáról egy következő klónt. Ez a folyamat nem folytatódik a végtelenségig, mivel  a függvényhívás feltételes kell legyen, ami azt jelenti, hogy van egy megállási feltétele, ami ha beteljesül, többé már nem jön létre egy következő klón , hanem vissza térítődnek az értékekek  az előző klónokhoz . Típusait tekintve a rekurziót két  különböző ré szre bonthatjuk : direkt vag y közvetlen rekurzió, illetve indirekt vagy közvetett rekurzió. Direkt rekurziónak nevezzük azt amikor egy függvény saját magára hivatkozik amikor függvényhívást végez. Indirekt rekurziónak azt nevezzük amikor egy rekurzív függvé ny nem saját magát hívja meg, hanem egy másik függvényt, amely szintén nem önmagát hívja meg, hanem azt a fügvényt aki őt meghívta.   17  2.5 Ciklus VS Rekurzió    A rekurzió ellenpárja az iteratív ciklusos megoldás.  Annak ellenére, hogy ellenpároknak hívjuk őket , a rekurz ív függvényeket ciklussá lehet alakítani és ugyan így az iteratív ciklusokat rekurzióvá. Elmondható, hogy az iteráció  gyorsabb a rekurziónál, mivel a rekurzió esetében függvényhívás történik, ami meg növeli a futási időt. A rekurziónak eg y másik hátránya az, hogyha a rekurzió túl nagy mélységeket jár be, akkor feltelhet a verem.   De miért éri meg akkor rekurziót használni ? A rekurzi ó ereje nem a gyorsaságában, hanem az eleganciájában rejlik. Sok esetbe n a rekurzióval megoldott feladat tömörebb és jobban olvasható mint az iterációs ellenpárja. Ennek egyik ékes példája a Hanoi tornyai nevű feladvány. A Hanoi tornyai rekurzív implementálása nagyon rövid és elegáns . Lásd 2.7  ábra.    2.7 ábra . Hanoi tornyai rekurzív implementációja  Ezzel ellentétben, Hanoi tornyai iteratív implementálása még sok informatika tanárt is gondolkodóba ejtene. Fi gyeljük meg egy kicsit a 2.8 -as és 2.9 -es ábrán ezt a megvalósítást is, a fentiekben látott bemeneti értékekre.  Ezeken  az ábrákon megfigyelhető, hogy Hanoi tornyai iteratív megvalósítása több mint tizszer annyi kódolást igényel mint a rekurzív megvalósítás . 18   2.8. ábra  Hanoi t ornyai iteratív megvalósítás    2.9. ábra Hanoi t ornyai iteratív megvalósítás   Ezen két megvalósításból  láthatjuk, hogy a a re kurziót igenis megéri használni, mert a példaként említett Hanoi tornyai probléma rekurzív megvalósítása sokkal  érthetőbb,  rövidebb  és elegánsabb mint az iterációval megírt ellenpárja . 19  2.6 A rekurzió oktatása    A reku rzív programozás egyike azon témáknak, amelynek tanítása során az oktatók előszeretettel nyúlnak bizonyos oktatási segédeszközökhöz. A legtöbb ilyen segédeszköz  a látást célozza meg mint felhasználandó érzéket, mivel felismerték, hogy a látás fontos szerep et játszik az új fogalmak elsajátításában. Ezen felismerés különböző kutatási vonalakat nyitott meg a rekurzió oktatását tekintve, mint például a rekurzió vizuális analógiái, vagy a programok eredményének animálása [13].   Az analógiákat tekintve az oktatók és kutatók túlnyomó többsége ugyan azokkal a példákkal áll elő, ilyen például a rekurzív mintázatokat mutató brokkoli, a fák ágai, illetve az egymással szembe helyezett tükrök tükröződései.  A kutatások során nem csak tárgyakat, hanem külöböző rekurzív foly amatokat is megvizsgáltak mindennapi példák segítségével. Megvizsgálták például azt, hogy hogyan értelmezik a gyerekek az egymás mellé helyezett dominók eldőlését [13].  A 12 év körüli és idősebb gyerekek esetében a dominók eldőlésének leírásában megfigyelh ető a rekurzív gondolkodás, mivel a gyerekek megfigyelték, hogy minden dominóelem eldőlését az előtte levő dominó okozta. Ezzel ellentétben, a 12 évnél fiatalabb gyerekek esetében a leírás inkább iteratív jellegű, eldől egy dominó, majd a következő, egésze n ameddig egy se marad állva[13].   A rekurzi ót kutató személyek  számos javaslatot tettek a rekurziós gráfok használatára, annak érdekében, hogy gyorsítani lehessen ezáltal a kezdőknél a rekurzió elsajátításának a folyamatát. Ezen gráfok lehetővé teszik a d iákok számára a függvényhívások kiértékelésének a követését  és mélyebb elemzését . Ha ezen gráf egy bináris fa, akkor minden egyes csomópont ugyan azt a függvényhívást jelenti [13].     20  3.Hasonló alkalmazások  és munkák    3.1. VisuAlgo     A “VisuAlgo” egy interneten el érhető weboldal, amely animációk segítségével próbál vizualizálni különböző adatstruktúrákat és algoritmusokat .[5] Az oldal segítségével többek között képesek vagyunk vizualizálni rendezéseket, láncolt listákat, hasító táblákat, és nem utolsó sorban, a rekurziót .   3.1 ábra  VisuAlgo Fibonacci(5) értékre [5]  A „VisuAlgo” a rekurziót egy fa struktúra segítségév el vizualizálja, ahogy ezt a 3.1 -es ábra is mutatja.  Az oldal bal alsó sarkában található egy mező, amely segítségével ki tudjuk választani, hogy mit i s szeretnénk vizualizálni. A 3.1 -es ábrán például a Fibonacci számok vizualizációja van kiválasztva n =5 értékre. A Fibonacci számokon kívül további 19 függvé ny vizualizációjára ad lehetőseget a program, amelyeknek forráskódját ki is vetíti egy szövegdobozba. Lehetőség van saját kód kipróbálására is, ugyanis a lenyíló listában az utoló elem a „Custom code” nevet viseli, ha ezt kiválasztjuk, akkor megírhatjuk a szövegdobozban a saját kódunkat JavaScript programozási nyelv segítségével.   21   Ahogy a 3.1 -es ábra jobb oldalán is megfigyelhető , a fa struktúra levelei különböző színeket  vesznek fel. A legalsó szinteken található levelek a zöld színt veszik fel, ezek a le velek azokat a rekurzív hívásokat jelölik, amikor a megállási feltétel igaznak bizonyul és elkezdődik az értékek visszatérítése.  A levelek fehér színűek amikor egy hívás az adott n értékre először történt meg.  A program világoskék színnel jelöli azokat a h ívásokat amikor  az n bemeneti értékre a hívás egyszer már feldolgozásra került [5]. Vegyük például az ábra alapján a Fibonacci(2) – es értéket. Mivel a bináris fa balról jobbra kerül bejárásra, a fa leginkább baloldalán található kettes értékű levél fehér színnel van jelölve, míg az utána következő összes többi kettes értékű levél kék színnel lett jelölve.   Következtetésként kijelenthető, hogy a “VisuAlgo” hasznos  segédeszköznek bizonyu l a rekurzió vizualizálását illetően, és mint diákok, mint tanárok hasznát vehetik akik többet szeretnének tudni a rekurzióról.   3.2.Sort Visualizer    A “Sort Visualizer” szintén egy interneten elérhető weboldal, amely rendezési algoritmusok vizualiz álására specializálódott. A 16 darab vizualizálható a lgoritmus közül van néhány amely előszeretettel alkalmazza a rekurziót. Ilyen algoritmus például a quicksort, illetve a merge sort. Ezen alpont keretén belül szeretnénk bemutatni ezeknek a vizualizációját a program segítségével.   A quicksort vagy g yorsrendezés a divide et imp era elv alapján működik. A rendezendő listát egy pivot segítségével két különálló részre bontja, majd erre a két új listára külön külön ismét meghívja a gyorsrendezést. [6] Ez a rekurzív folyamat addig folytatódik, amíg az átadott lista hossza kisebb vagy e gyenlő nem lesz 1 -el. Nezzük meg hogyan is vizualizálja ezt a rendezést a program. Lásd 3.2  ábra.     22   3.2 ábra . QuickSort  a Sort Visualizer  programban  [12]  Első lépéskent a rendező algoritmus végig iterál a listán, és elkezdi kicserélni a kiválasztott pivot elem két oldalán levő értékeket. Azokat az elemeket amelyek kisebbek mint a pivot a bal oldalára rendezi, míg azokat amelyek nagyobbak a jobb oldalára. Ez után következik az algoritmus rekurzív része , amit az előbbiekben már ismertettünk. Megfigyelhe tő hogy a lista legeleje kerül leghamarabb rendezésre, ez annak köszönhető, hogy az oszd meg és uralkodj módszert használó algoritmus, először a pivot bal oldalán levő listára hívja meg rekurzívan a quicksortot.   A következőkben figyeljük meg egy kicsit, h ogyan figyelhető meg a rekurzió a merge sort esetében.  Lásd 3.3  ábra.   3.3 ábra . Merge Sort a  Sort Visualizer  programban  [12] 23    A merge sort a quicksorthoz hasonlóan az oszd meg és uralkodj módszert alkalmazza. A rendező algoritmus rekurzívan felosztja a bemeneti listát, egészen ameddig az átadott lista csupán egyetlen elemet tartalmaz. Amint ez megtörténik, a részsorozatok összevonódnak és rendezésre kerülnek. Az algoritmus fokozatosan összevonja a részlistákat, egészen addig amíg egyetlen rendezett lista  marad a végén.[7]  Az összevonás folyamata a 3.3 -as ábrán is nagyon jól megfigyelhető.   Összességében kijelethető, hogy a “Sort Visualizer” is sokat tud segíteni egy felhasználónak a rekurzió megértésében.      3.3 Rekurzió kutatása a Sapientia egyetemen     A Sapientia Erdélyi Magyar Tudományegyetem Marosvásárhelyi karán a 2008 -as évben Dr. Kátai Zoltán vezetésével elvégzésre került egy kutatás, amelynek keretén belül egy úgynevezett többérzékelős módszert probáltak ki a rekurzió oktatására.  Ezen alpontban bemutatásra kerül ez a kutatás, amely a [8] –as cikkben található, és az ehhez fejlesztett szoftver is bemutatásra kerül.   A kutatás egyik részeként megkértek az egyetem diákjai közül néhányat, hogy játszák el egy rekurzív függvény futási f olyamatát. Az első diák szemléltette a main függvényt, míg a többiek  a rekurzív függvény példányait szemléltették. Amikor egy a cikk által rekurzív szereplőnek megnevezett diák meghívásra került, a szereplő kilépett a meghívója mögül és elkezdte elemezni az általa kapott feladatot. Két lehetősége volt, követi a rekurzív forgatókönyvet, vagy követi a triviálisat , ami a megállási feltétel teljesülését jelentette. Ha az első lehetőséget választotta, akkor meghívta a társát  és saját magát felfüggesztette amíg nem kapott választ a hívásra. A legutolsó diáknak a triviális forgatókönyvet kellett választania, mivel akkor teljesült a megállási feltétel. Neki az volt a dolga, hogy a részfeladatának az eredményét átadja a hívójának, aki ennek hatására felébredt a felf üggesztett állapotából és ugyan ezt a 24  műveletet elvégezte.  Ez a folyamat addig folytatódott amí a main függvényt szemléltető diák megkapta az eredményt [8].   Ezen kísérlet segített a diákoknak jobban megérteni, hogy hogyan is működik a rekurzió.  A néző diá kok megérthették belőle a rekurzív folyamatok működését, míg azok a diákok aki eljátszodták folyamatokat, kinetikus módon is memorizálták a rekurziót, a műveletekhez kapcsolódó mozgások által  [8].  A kutatás egy másik fontos része , egy a rekurzió oktatására  kifejlesztett szoftver kipróbálása volt.  Ezen szoftver audio -vizuális eszközökkel próbálja megértetni a felhasználóval a rekurzivítást. A rekurziót a program lépcsőzetesen vizualizálja, ezáltal minden egyes rekurzív hívás egy úgynevezett emelete t hoz létr e . Lásd 3.4 -es ábra. Minden egyes emeleten a vizualizációhoz egy zenei bejátszás is társul, melynek hangmagassága az emelet magasságának függvényében növekszik.   3.4 ábra.  Rekurzió lépcsőzetes ilusztrációja  [8]  A kísérletben 43 nagyjából azonos képességekkel rendelkező  első éves  diák vett részt . A diákokat két csoportra osztották, 23 -at közűlük a tradicionális módszerekkel tanítottak, míg a megmaradt 20 diáknál az előbbiekben említett módszereket használták a rekurzió oktatására. Az utólag os teszt eredmények azt mutatták, hogy akiket a többérzékelős módszerekkel tanítottak, jobban teljesítettek mint azok a társaik akik tradicionális oktatásban részesültek. [8] Ezen kísérlet ékes példája annak, hogy a különböző segédeszközök könnyebbé tudják tenni a rekurzió megértését és tanulását.  25  4.Szoftver tervezése és kivitelezése    A dolgozat ezen részében bemutatásra kerül a szoftver, amelyet a rekurzió lépcsőzetes módszerrel való vizualizálásához fejlesztettem. Az alkalmazás  egy Windows Form aplikáció amely  C# programozási nyelven íródott és a .Net keretrendszer 4.7.2 - es verzióját használja.  A szoftver lehetőséget ad rekurzív függvények illetve rekurzív eljárások vizualizációjára.  A különbség a két fogalom között az, hogy míg a rekurzív függvény vissza  térít egy eredményt a hívójához, addig a rekurzív eljárás csupán elvégez egy feladatot anélkül, hogy bármit is vissza térítene a hívójához. Természetesen a rekurzív eljárásokban is jelen van a megállási feltétel [14].  4.1 Felhasználói követelmények    Az szoftver  elindítása  után, a felhasználó előtt egyenesen az alkalmazás fő ablaka jelenik meg. Ezen a fő ablakon történik meg a rekurzív függvények vizualizálása egy koordináta rendszerben. Az elindítás pillanatában a fő ablakon három gomb jelenik meg, a “Choose File”, “Run”, illetve a “Write own c ode” elneve zésekkel.   A “Choose File”  gomb lenyomásávál egy különálló ablakban megnyílik  a projektnek a könyvtára, ahol a felhasználó ki tudja választani az előre megírt rekurzív jellegű függvények közül azt amelyiket vizualizálni szeretné. Minden egyes függvény különálló .txt kiterjesztésű fájlokban van megírva, a felhasználónak csak annyi a  feladata, hogy kiválassza a fájlt és megnyomja az „Open” gombot.  Miután ki lett választva a függvény, a szoftver átvizsgálja a kapott függvényt és megállapítja, hogy hány paraméter megadására van szüksége az adott függvénynek. Annak fügvényében, hogy ez a  szám mennyi, a szoftver kigenerálja azokat a szövegdobozokat ahova a felhasználó be tudja írni az értékeket. Például, ha kiválasztottuk a faktoriális függvényt, aminek meghívásához egyetlen paraméterre van szükség, a program egyetlen szövegdobozt fog létr ehozni ahova be tudjuk írni ezt az értéket.   A “Run” gomb lenyomásával tudjuk elindítani az előző lépésben kiválasztott függvény vizualizációját. Ha sikeres volt a program lefuttatása, akkor az ablak gombok alatti üres részében megjelenik a függvény vizual izációja. Abban ez esetben ha nem választottunk még ki egyetlen 26  függvényt sem amit vizualizálni szeretnénk és megnyomjuk a “Run” gombot, a szoftver egy üzenetet közvetít a felhasználó felé, hogy előbb válasszon ki egy függvényt és csak azután nyomja meg a “Run” gombot. Hasonl ó figyelmeztetést kapunk abban az esetben  is ha a kigenerált szövegdobozokba egy érvénytelen karaktert ütünk be. Minden beütött érték szám kell hogy legyen, ennek értelmében ha egy betüt adunk meg paraméterként, a szoftver figyelmeztet,  hogy a megadott paraméter nem érvényes.   4.1 ábra.  Use case diagramm   27   A “Write own c ode” gomb megny omásával egy új ablak fog megnyílni a felhasználó előtt. Ebben az új ablakban lehetőség nyílik arra, hogy a felhasználó egy saját maga által szerkesztett kódot is levizualizáljon. Az ablak megnyitásakor még nincs kigenerálva az a szövegdoboz , ahova a felhasználó beírhatja a saját C # nyelven megírt kódját, viszont az ablak legtetején talál két gombot, név szerint a “Direct Recursion” és az “Indirect Recursio n” gombokat. Ezek a gombok azért szükségesek, hogy a felhasználó ki tudja választani a kívánt rekuzió típusát. Ha a felhasználó a “Direct Recursion” gombot n yomja meg akkor egyetlen szövegdoboz kerül kigenerálásra, mivel a közvetlen rekurzióhoz csak egyetl en megírt függvényre van szükség. Ha az “Indirekt Recursion” gombot nyomja meg a felhasz náló, két szövegdoboz generálódik ki, mivel a közvetett rekurzióhoz legalább két függvényre van szükség. Az előzőekben feldolgozott fájl kiválasztásos módszernél azért nem volt szükség hasonló műveletre, mivel a szoftver a beolvasott szöveges fájl alapján el tudja dönteni a rekurzió típusát.   4.2 ábra . Activity diagramm  28   Miután ki lett generálva a megfelelő számú szövegdoboz a függvények beírásához, a felhasználó neki kezdhet kódolni. A szövegdoboz első sorába a felhasz náló az úgynevezett “method signaturet” kell hogy beírja, amely tartalmazza a függvény nevét, típusát, és  a függvény paramétereit. Miután az első sor be lett írva, enter gomb lenyomására a program meghatározza, hogy hány paramétere van a megírt metódusnak, amely után kigenerálja a megfelelő mennyiségű szövegdobozt a paraméterek értékeinek megadására. Abban ez  esetben ha hibát vétettünk ezen műveletek közben, például nem adtunk meg megfelelő mennyiségű paramétert az első sorban, de már kigeneráltuk a paraméterek szövegdobozait, nyomjuk meg a “Clear all” elnevezésű gombot, mely vissza állít mindent az eredeti ál lapotára.Ezután előlről kezdhetjük az előbbiekben vázolt műveleteket. A függvény megírása közben a felhasználó alábbi módon jelzi azt is, hogy milyen színnel szeretné hogy kirajzolódjon egy adott művelet : “//Sz ín”. Abban az esetben ha egy nem értelmezhető színt írt be a felhasználó, egy alapértelmezett szín fogja átvenni a helyét.  Ha nem írt be megfelelő mennyiségű színt a vizualizáció megjelenítéséhez, a rendszer jelzi ezt a felhasználó felé.  Abban az esetben ha sikerült helyesen elvégezni a kód és a paraméterek megadását, nyomjuk meg a “Test function” gombot . Amikor ez a gomb megnyomódik, a szoftver lefuttatja a kódot a megadott paraméterekre, és a lap alján levő szövegdobozban jelzi, hogy a k ód sikeresen lefutott és készen áll a vizualizálásra, vagy ha hiba van a kódban, jelzi hogy nem tudta lefuttatni azt. Abban az esetben ha sikeres volt a kód tesztelése, meg kell nyomni a “Run” gombot , melynek hatására a fő ablakban végbe megy a vizualizáci ó.   4.2 Rendszer követelmények   4.2.1.  Funkcionális követelmények    A rendszernek első sorban tartalmaznia kell a vizualizációk kiválasztásához használható eszközöket. A felhasználónak két lehetősége van, kiválaszthat egy előre megírt függvényt, a fő oldal bal felső sarkában található  “Choose F ile” gomb megn zom</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -797,6 +872,11 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>The topic of the project  is to develop a web application that connects students, companies, and universities during their internships. The goal is to develop a user -friendly platform capable of managing the entire process related to internships.   One of the major objectives of th e project is for the application to function as a professional -oriented social platform for students and companies, thereby facilitating the development of professional relationships and nurturing partnerships between companies and universities.   Another i mportant objective of the project is to provide students with recommendations on the platform based on their profiles and fields of study. This allows them to find relevant opportunities in the field of internships. The algorithms of my recommendation syst em, using techniques like Cosine Similarity, consider the students' skills, interests, and the requirements set by the companies. Thus, the platform helps students find the most suitable internship positions, optimizing the related processes and ensuring t he effectiveness of the internships.   To develop the project, I am using modern web technologies such as Angular, Java Spring Boot, PostgreSQL, and AWS. These technologies help make the platform robust, scalable, secure, and fast.</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>Internship, Ajánlórendszer, Cosinus hasonlóság, Angular, Spring Boot       WEB APPLICATION FOR MANAGING INTERNSHIP AND TRAINEESHIP ACTIVITIES</t>
         </is>
       </c>
@@ -820,6 +900,11 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t>Security systems are important for individuals, businesses, and institutions to main-tain a secure environment and protect their assets. Modern technology oers varioussolutions for this purpose. The main objective of such systems is to detect unauthorizedintruders among authorized individuals. Access control systems provide an ecient real-time solution to achieve this. They allow entry only to those individuals who have theappropriate permission and can authenticate themselves.For my thesis, I chose to implement a biometric access control system that utilizesfacial recognition to identify individuals. My goal was to create an easily manageable,fast, ecient, and, above all, secure system in a cost-eective manner, thereby simplifyingthe daily lives of people and streamlining the identiﬁcation process for individuals seekingentry into buildings.To ensure a high level of security, I chose facial recognition as the biometric identiﬁ-cation method. Facial recognition technology is widely known and used, often employedin secure computer systems, laptops, smartphones, or ATMs. In addition to its advan-tages, such as not requiring direct physical contact during the identiﬁcation process andbeing a fast and ecient method, an face recognition-based system is more secure andharder to bypass compared to other identiﬁcation methods. Passwords and PIN codescan be easily compromised or hacked, and various cards and keys can be lost or stolen,potentially leading to misuse by unauthorized individuals against security measures.Taking these aspects into consideration, I designed the system’s operation. To gainentry, it is a requirement for the administrator to add the individuals’ data and images.Once this condition is met, the person is granted access to the building. The user simplystands in front of the camera at an appropriate distance, and if they are found in thesystem, the door opens, allowing them to enter. To facilitate ease of use, I created auser interface that allows for easy addition of individuals, and for traceability, the systemmaintains a list of individuals who have entered the building, along with the exact entrytime.The system I implemented simpliﬁes the identiﬁcation process during entry and pro-vides a secure solution for detecting unauthorized individuals in everyday situations.</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>arcfelismerés, azonosítás, biometria, beléptet rendszer, biztonság</t>
         </is>
       </c>
@@ -843,6 +928,11 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t>The aim of the thesis is to design and develop a web application that digitises thechoice of subjects for the diploma. A solution was needed that would help and facilitatethe work of the university committee and students in the diploma topic selection process.Our objectives included the development of a web application that could handle alarge number of data and users and could be easily used by anyone. The applicationshould meet all university requirements and could be further developed on request. Besecure and ensure that the application is maintainable.The objectives have been achieved in all areas. A web application has been developedthat secretaries can log into and create periods and invite teachers and students to thesystem. Teachers can upload their degree topics and students can apply for them. Andguests can view the diploma topics they have created.A wide range of technologies have been used in the development. Most prominent arethe frontend and backend frameworks. Using Angular and Spring to boot I was able todevelop a highly scalable and secure web application. Using PostgreSQL database to storedata and testing frameworks and applications Cypress and Postman for maintainability.TartalomjegyzékÁbrák jegyzéke 3Táblázatok jegyzéke 41. Bevezet 52. Elméleti megalapozás és szakirodalmi tanulmány 72.1. Szakirodalmi tanulmány ........................... 72.2. Elméleti alapok ................................ 82.2.1. Hatékony eszközök a webalkalmazások fejlesztéséhez ........ 82.3. Ismert hasonló alkalmazások ......................... 82.4. Felhasznált technológiák ........................... 92.4.1. Angular frontend keretrendszer ................... 92.4.2. Spring boot backend keretrendszer ................. 102.4.3. Szervletek ............................... 132.4.4. Postgres és annak kezelése ...................... 142.4.5. Liquibase ............................... 152.4.6. Tesztelést elsegít frameworkok ................... 152.4.7. Verzió követ és feladat vezérl alkalmazások ............ 163. A rendszer speciﬁkációi és architektúrája 173.1. Követelmény speciﬁkációk .......................... 173.1.1. Funkcionális követelmények ..................... 173.1.2. Nem funkcionális követelmények ................... 213.2. Adatbázis ................................... 223.3. Alkalmazás architektúra ........................... 244. Részletes tervezés 304.1. Tervezési fázisok ............................... 304.1.1. Frontend ................................ 304.1.2. Backend ................................ 424.2. Tesztelés .................................... 484.2.1. Frontend tesztelés ........................... 484.2.2. Backend tesztelés ........................... 504.2.3. Éles tesztelés ............................. 5115. Üzembe helyezési lépések 525.1. Felmerült problémák és megoldásaik .................... 525.1.1. Idszakok beintegrálása az applikációba ............... 525.1.2. Hallgatók leosztása automatikusan ................. 536. Következtetések 546.1. Megvalósítások ................................ 546.2. Továbbfejlesztési lehetségek ......................... 54Irodalomjegyzék 56Függelék 57F.1. Kód részletek ................................. 572Ábrák jegyzéke2.1. Különbség egy MPA (Multiple Page Application) és egy SPA (Single PageApplication) között [ 8]............................ 92.2. Angular applikáció elemi felépítése [ 1].................... 102.3. Mikroszolgáltatások felépítése [ 5]...................... 112.4. Rétegelt architektúra megvalósítása Spring bootban. ............ 122.5. ORM mködése[ 4].............................. 143.1. Adatbázis diagram .............................. 243.2. Alkalmazás architektúra [ 3]......................... 254.1. Frontend oldali typescript osztály ...................... 374.2. Szerver oldali java osztály .......................... 374.3. Cypress tesztelés ............................... 504.4. Postman tesztelés ............................... 504.5. Diploma téma jelentkezés hallgató szemszögébl .............. 514.6. Diploma téma leosztás eredményei ...................... 513Táblázatok jegyzéke3.1. Bejelentkezési funkció ............................. 193.2. Hallgatók feltöltése funkció .......................... 203.3. Diplomamunka létrehozása funkció ..................... 203.4. Véglegesíteni a leosztott eredményeket a saját szakukról funkció. ..... 203.5. Diplomamunkára jelentkezni funkció. .................... 213.6. Keresni az elvégzett diplomamunkák között név és</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>alapjánfunkció. .................................... 2141. fejezetBevezetA mostani elrehaladott korban nagy mértékben kiegészíti életünket a digitális vilá</t>
         </is>
       </c>
@@ -866,6 +956,11 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>The aim of this thesis is to classify chest X-rays to detect the presence of pneumonia.A convolutional neural network was used to achieve a more accurate classification. Ourgoal was to develop an efficient classifier, which is a neural network created by our ownmodel, or a neural network with GoogleNet architecture, trained for our own purposesusing “transfer learning” technique.Our research methodology was based on studying existing solutions, conducting ourown experiments and collecting data. We applied the transfer learning technique to theGoogleNet architecture, which is a pre-trained large model, thus improving the classi-fication accuracy. Data collection was performed using chest X-rays of pneumonia andasymptomatic cases.Based on the results, we were able to develop a graphical user interface that allowsautomatic classification of chest radiographs and diagnosis of pneumonia. The neural net-work with GoogleNet architecture achieved outstanding accuracy on the tested dataset,and compared to our own classification network, produced significantly better results,similar to the results of the networks studied in the literature.Based on these results, we conclude that a well-written neural network interoperatingwith the GoogleNet architecture can effectively detect pneumonia based on chest X-ray.This research could contribute to the improvement of medical diagnostics, helping earlydetection and more effective treatment.</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
           <t>mellkasi röntgenfelvétel, osztályozás, konvolúciós neurális hálózat,transfer learning, GoogleNet architektúra</t>
         </is>
       </c>
@@ -893,6 +988,11 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t>In human life, one of the most important and valuable things is time. In today's fast -paced world, events have become so accelerated that it is truly challenging to kee p them under control and manage our time effectively. To save time, numerous smart devices and systems have emerged, making people's lives easier. We can even say that we are living in the era of smart systems.  My thesis’ topic encompasses such a system. I t helps us not only to save time, but also relieves us from a responsibility. This modern and innovative solution allows us to take care of our plants in the best possible way while minimizing the tasks of plant care and maximizing the health and beauty of  our flowers. It assists in maintaining the plants in optimal condition, especially when we are not at home or don't have enough time for their care. The system's sensors and controllers monitor the environmental parameters of the plants, such as temperatu re, humidity, light intensity, and their watering needs.  The smart flowerpot system automatically regulates watering, ensuring that the plants always receive the right amount of water at the right time. We no longer need to worry about overwatering or unde rwatering, as the system takes precise care of watering our flowers.  Through an interactive and user interface, we can easily set the watering schedule, monitor the plants' condition, and track the environmental parameters. Whether we are at home or away, the system allows remote access, enabling us to stay connected with our flowers and intervene when necessary.  For the control of the system, I have used an ESP32 microcontroller. The ESP32 is an extremely versatile and powerful platform that enables full c ontrol and monitoring of my smart flowerpot system.</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>felhasználói felület, okos rendszer, mikrovezérlő</t>
         </is>
       </c>
@@ -916,6 +1016,11 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t>Industrial robots are more and more wide-spread in various manufacturing and logistics processes, where accuracy, speed, and safety are important factors. Robots are capable of automating tasks that are boring, dangerous, or too complex for humans. However, the collaboration between robots and humans represents challenges, especially when robots need to adapt flexibly to changing environments and tasks.  The recognition and manipulation of small objects are tasks widely used in industrial and educational contexts. However, determining the type and positioning of these objects is not always straightforward, particularly when they have similar colors or sizes. In this paper, I present a method that enables the Baxter robot to easily differentiate cubes using ArUco markers. I describe how I programmed the Baxter robot to determine the type and position of cubes on a workspace and arrange them accordingly. Throughout my study, I provide a detailed presentation of the system's design, implementation, and testing.  In my paper, I have developed a system that can control the Baxter robot to recognize and manipulate cuboid-shaped objects. The system consists of three main components: an image processing module that detects and identifies objects using the OpenCV and cv2.aruco libraries, a communication module that uses the ZMQ protocol to send and receive data, and a robot control module that utilizes the ROS (Robot Operating System) libraries to control the robot's arms and grippers. During the operation of the system, the robot captures an image of the workspace, determines the position and type of objects, and performs sorting based on this information.</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
           <t>Baxter, ROS, ArUco, Opencv, Python, képfeldolgozás, ipari es oktatási robotika</t>
         </is>
       </c>
@@ -939,6 +1044,11 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
+          <t>Nowadays,  everyone  has  a  smartphone  that  can  solve  many  problems  with  various applications. Such useful applications are, for example, applications for paying our bills, but we can also find many applications for managing our day-to-day tasks.  Mobile applications not only make our everyday lives easier but can also be helpful in educational institutions. The most commonly used mobile applications in schools and universities are various calculators, translators, and note-taking applications. However, applications for presenting PowerPoint presentations are not widespread among people, so their number is very small and they are not the best maintained or do not have many features that would make the use of these applications meaningful other than that the user does not have to keep a separate device with them.  My thesis aims to design a system that allows laser pointers to be used on PowerPoint presentation slides with the help of our smartphone regardless of whether we have an Android or IOS phone. In addition, it should allow switching between slides and drawing on them. The system consists of two components: one part is the server, which receives and processes data sent by our phone; the other part is the phone, which detects the user’s hand movements with the help of the accelerometer in the phone and also sends the pressing of displayed buttons to the server via WiFi. The data required to connect to the server is made possible by scanning the QR code generated by the server.</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
           <t>Mobil alkalmazás, PowerPoint, lézermutató.</t>
         </is>
       </c>
@@ -966,6 +1076,11 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t>In the modern and rapidly evolving world, there is electric technology behind all our needs, hobbies,  and work, which we use comfortably and without problems. In current times, with the increase in inflation, the prices of all necessities have risen, especially electricity. Therefore, if we do not pay attention to our daily energy consumption and do not m ake changes in our energy usage habits, we can easily encounter financial difficulties.  The aim of my thesis is to develop an IoT (Internet of Things) system that enables easy measurement and monitoring of energy consumption of electronic devices within a household. Additionally, the system is capable of monitoring the production of solar panels installed in the household. The data is stored in a database, allowing for future statistical analysis and insights. This provides a more accurate understanding of energy costs and helps optimize consumption while leveraging renewable energy sources.  The different units communicate with each other through the MQTT protocol, where publishers (household appliances, solar panels) send sampled data to the broker (Raspber ry Pi), where the data is processed, stored in a MongoDB database, and the processed data is sent to a mobile application via a  REST  API service.</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>IoT, Intelligens teljesítmény mérő , MQTT, Energ ia Menedzsment</t>
         </is>
       </c>
@@ -993,6 +1108,11 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
+          <t>In recent years, the application of industrial robots has witnessed significant growth. Their expanding applications and increasing functionality enable them to perform a wider range of human tasks. In this thesis, our research focused on developing a system that records user movements and utilizes them to calculate the necessary control signals for an industrial robot. Specifically, we designed a solution for the remote control of a two-armed industrial robot based on human arm movements.  To achieve real-time control of both robot arms, we utilized a second-generation Kinect sensor, known for its motion tracking and distance measurement capabilities. The data captured by the Kinect sensor was subsequently transformed into a suitable format for controlling the robot arm. The developed control approach is based on the angle measurement of the users limbs, and based on this information the joints of the robot arm can be directly controlled.  Our implementation applies a Baxter cooperative robot. Baxter is a fixed platform robot, equipped with two robotic arms, featuring seven degrees of freedom each. The system provides control of the robotic arms through hand gestures. The developed software provides control of the robotic arms, the gripping tools of the robot arm through hand gestures, in addition to moving the robot arm itself. Based on the state of the hand, the robot's gripping tools can open or close. In my paper, I used the ROS (Robot Operating System) libraries for robot control. Additionally, I used the Kinect SDK for handling the Kinect camera and the ZMQ protocol for communication between the components. The developed system can recognize the user, tracking their movements, and fitting them onto a dual-arm industrial robot.</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>ipari robot, gesztusok, távvezérlés, Kinect</t>
         </is>
       </c>
@@ -1019,6 +1139,11 @@
         </is>
       </c>
       <c r="E25" t="inlineStr">
+        <is>
+          <t>Thanks totechnological advances, smartphones andtheinternet havebecome crucial inourlives,because itisalways atourfingertips andalsoactsasapersonal assistant tomakeourliveseasier. Theother major partofourlivesisstilldominated bypersonal dealingsandpaper-based documents. There isaperceptible barrier between thetwopoles, oneofwhich ischaracterized byconstant movement andspeed, theother byslowness andtime-consumption.Theaimofthisthesis istodevelop anefficient system tobreak down thisbarrier, providinganewwayofprocessing driving penalties. Traditional methods cannot keepupwithourfast-paced world andcancause problems suchasthedifficulty oforganizing finesandtheresulting delay inpayment. Wesetouttodevelop asystem thatmeets today's technologicalrequirements. Indeveloping thesystem, wetookintoaccount bothparties, theonewhohands outthefineandtheonewhoreceives it,andweaimed foranimplementation thatistime-efficient forbothroles. Theuseofanandroid application todeliver thepunishmentseemed tobethemostappropriate, asourphone isalways athandwhich grants internetaccess totheuser.Themostobvious waytoimplement thesystem fordrivers wastouseaweb-based interface, asthiswould provide them arelatively large interface forabetteroverview andeasier payment offines.</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
         <is>
           <t>büntetésekügyintézése,androidos applik áció,webes felület</t>
         </is>

</xml_diff>

<commit_message>
Update: Extract Hungarian and English keywords from PDFs
</commit_message>
<xml_diff>
--- a/szamteches_info_extracted.xlsx
+++ b/szamteches_info_extracted.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,7 +461,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Kulcsszavak</t>
+          <t>Kulcsszavak (magyar)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Kulcsszavak (angol)</t>
         </is>
       </c>
     </row>
@@ -492,6 +497,11 @@
           <t>mikrovezérlő, WiFi, giroszkóp, gyorsulásmérő</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>microcontroller, WiFi, gyroscope, accelerometer</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -520,6 +530,11 @@
         </is>
       </c>
       <c r="F3" t="inlineStr">
+        <is>
+          <t>IoT, Home -automation, Raspberry Pi,  MQTT</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>IoT, Home -automation, Raspberry Pi,  MQTT</t>
         </is>
@@ -544,6 +559,11 @@
           <t>hőmérséklet mérés, bluetooth, alkalmazás, szabad vezérlés</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>temperature measurement, bluetooth, application, robot control.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -576,6 +596,7 @@
           <t>konvolúciós neuronhálók, agydaganat, osztályozás, keras</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -608,6 +629,11 @@
           <t>táblajáték, képfeldolgozás, opencv , python</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>backgammon, image processing, OpenCV ,  Python</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -636,6 +662,7 @@
           <t>Arduino, protokoll, érz ékelők,  asztali alkalmazás       Interactive sensor system</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -664,6 +691,11 @@
           <t>hálózat, protokoll, útválasztás</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>network, protocol, routing</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -694,6 +726,11 @@
       <c r="F9" t="inlineStr">
         <is>
           <t>Markov klaszterezés, gráf, ritka mátrix, hatékony algoritmus, bioinformatika, fehérje szekvencia         _____________________________________________________________________________    11  Extras O proporție semnificativă a fenomenelor biologice poate fi urmărită înapoi la genetica, care se bazează pe secvențele de gen</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Markov clustering, graph, sparse matrix, efficient algorithm, bioinformatics, protein sequence  Keywords: Markov clustering, graph, sparse matrix, efficient algorithm, bioinformatics, protein sequence   _____________________________________________________________________________    14</t>
         </is>
       </c>
     </row>
@@ -716,6 +753,11 @@
           <t>platformfüggetlen, mobilalkalmazás, Flutter, Spring Boot, esemén</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>platform -independent, mobile application, Flutter, Spring Boot, event.</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -744,6 +786,11 @@
           <t>digitális jelfeldolgozás, hang effektusok, ARM programozás, Python szimuláció</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>digital signal processing, sound effects, ARM programming, Python simulation</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -776,6 +823,11 @@
           <t>mélytanulás,  szív- és érrendszeri betegségek ,  spektrogram, jel  szűrés, betegség diagnózi</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>deep learning, cardiovascular diseases, spectrogram, signal filtering, disease diagnosis.            Tartalom</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -808,6 +860,11 @@
           <t>mobilis  robot, hangvezérlés</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>mobile robots, voice control</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -834,6 +891,11 @@
       <c r="F14" t="inlineStr">
         <is>
           <t>blokklánc, kriptovaluta, decentralizált tőzsde, okos szerződés</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>decentralized exchange, smart contract, crypto, blockchain</t>
         </is>
       </c>
     </row>
@@ -852,6 +914,7 @@
         </is>
       </c>
       <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -880,6 +943,11 @@
           <t>Internship, Ajánlórendszer, Cosinus hasonlóság, Angular, Spring Boot       WEB APPLICATION FOR MANAGING INTERNSHIP AND TRAINEESHIP ACTIVITIES</t>
         </is>
       </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Internship, Recommendation System , Cosine Similarity , Angular, Spring Boot</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -908,6 +976,11 @@
           <t>arcfelismerés, azonosítás, biometria, beléptet rendszer, biztonság</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>facial recognition, identiﬁcation, biometrics, access control system, secu-rity</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -936,6 +1009,7 @@
           <t>alapjánfunkció. .................................... 2141. fejezetBevezetA mostani elrehaladott korban nagy mértékben kiegészíti életünket a digitális vilá</t>
         </is>
       </c>
+      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -964,6 +1038,11 @@
           <t>mellkasi röntgenfelvétel, osztályozás, konvolúciós neurális hálózat,transfer learning, GoogleNet architektúra</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>chest X-ray, classification, convolutional neural network, transfer learn-ing, GoogleNet architecture</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -996,6 +1075,11 @@
           <t>felhasználói felület, okos rendszer, mikrovezérlő</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>user interface , smart system , microprocessor</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1024,6 +1108,11 @@
           <t>Baxter, ROS, ArUco, Opencv, Python, képfeldolgozás, ipari es oktatási robotika</t>
         </is>
       </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Baxter, ROS, ArUco, Opencv, Python, image processing, industrial and educational robotics</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1052,6 +1141,11 @@
           <t>Mobil alkalmazás, PowerPoint, lézermutató.</t>
         </is>
       </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Mobile application, PowerPoint, laser pointer.</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1084,6 +1178,11 @@
           <t>IoT, Intelligens teljesítmény mérő , MQTT, Energ ia Menedzsment</t>
         </is>
       </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>IoT, Smart Energy meter, MQTT, Energy Management</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1116,6 +1215,11 @@
           <t>ipari robot, gesztusok, távvezérlés, Kinect</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>industrial robot, remote control, gestures, Kinect       8</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1146,6 +1250,11 @@
       <c r="F25" t="inlineStr">
         <is>
           <t>büntetésekügyintézése,androidos applik áció,webes felület</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>traffic penalty management, android app,webinterface8</t>
         </is>
       </c>
     </row>

</xml_diff>